<commit_message>
Added to Correlation of Lit Rev
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Desktop\thesisWindows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFCD21B7-EA65-48A2-873C-C859901659A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E9FAECF-DFCE-4F0A-AA55-43DC9B36B8C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="163">
   <si>
     <t>Date</t>
   </si>
@@ -517,7 +517,10 @@
     <t>18:30 - 19:30 23:00 - 24:00</t>
   </si>
   <si>
-    <t>10:00-11:30 15:00 - 16:00</t>
+    <t>10:00-11:30 15:00 - 16:00 21:00 - 23:00</t>
+  </si>
+  <si>
+    <t>12:30 - 13:30 15:30 - 16:30 17:00 - 18:00</t>
   </si>
 </sst>
 </file>
@@ -1230,7 +1233,7 @@
                   <c:v>11.5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.5</c:v>
+                  <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0</c:v>
@@ -1254,7 +1257,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0">
-                  <c:v>17.255813953488371</c:v>
+                  <c:v>17.379310344827587</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2131,7 +2134,7 @@
   <dimension ref="A1:AMK116"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2861,7 +2864,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="37" t="s">
         <v>36</v>
       </c>
@@ -2889,9 +2892,11 @@
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
       <c r="M20" s="8">
-        <v>2.5</v>
-      </c>
-      <c r="N20" s="7"/>
+        <v>4.5</v>
+      </c>
+      <c r="N20" s="7" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="21" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
@@ -2915,10 +2920,14 @@
       <c r="I21" s="25">
         <v>43923</v>
       </c>
-      <c r="J21" s="24"/>
+      <c r="J21" s="24" t="s">
+        <v>162</v>
+      </c>
       <c r="K21" s="8"/>
       <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
+      <c r="M21" s="8">
+        <v>2</v>
+      </c>
       <c r="N21" s="7"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -3019,11 +3028,11 @@
       </c>
       <c r="M25" s="8">
         <f>SUM(M18:M24)</f>
-        <v>4.5</v>
+        <v>8.5</v>
       </c>
       <c r="N25" s="29">
         <f>SUM(K25:M25)</f>
-        <v>4.5</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -4765,15 +4774,15 @@
       </c>
       <c r="F86" s="61">
         <f>SUM(F81,F73,F65,F57,F49,F41,F33,F25,F17,F9,M9,M17,M25,M33,M41,M49,M57,M65,M73,M81)</f>
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="G86" s="63">
         <f>SUM(D86:F86) + 9</f>
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="H86" s="64">
         <f>G86/400</f>
-        <v>0.53</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.25">
@@ -4792,7 +4801,7 @@
       <c r="F88" s="61"/>
       <c r="G88" s="58">
         <f>G86*50</f>
-        <v>10600</v>
+        <v>10800</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
@@ -4804,7 +4813,7 @@
       </c>
       <c r="E90" s="67">
         <f ca="1">G86/(DATEDIF("2020-01-06",TODAY(),"d")/7)</f>
-        <v>17.255813953488371</v>
+        <v>17.379310344827587</v>
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.25">
@@ -4929,7 +4938,7 @@
       </c>
       <c r="C107" s="8">
         <f>N25</f>
-        <v>4.5</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="108" spans="2:3" x14ac:dyDescent="0.25">
@@ -5007,7 +5016,7 @@
       </c>
       <c r="C116" s="68">
         <f ca="1">E90</f>
-        <v>17.255813953488371</v>
+        <v>17.379310344827587</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LitRev Polished up to Convolution
Starting on:
 - Gaussian
 - Clustering
 - Morphology
 - Contours
 - Object Tracking
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Desktop\thesisWindows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B61492-2138-4322-B87D-4DE21B63D679}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F0EEC74-5C6C-4710-ADDB-D49C3B92FF54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="168">
   <si>
     <t>Date</t>
   </si>
@@ -533,6 +533,9 @@
   </si>
   <si>
     <t>Introduction + Referencing</t>
+  </si>
+  <si>
+    <t>11:30 - 13:00</t>
   </si>
 </sst>
 </file>
@@ -1269,7 +1272,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0">
-                  <c:v>17.305555555555554</c:v>
+                  <c:v>17.115384615384617</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2146,7 +2149,7 @@
   <dimension ref="A1:AMK116"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3085,11 +3088,15 @@
       <c r="I26" s="35">
         <v>43927</v>
       </c>
-      <c r="J26" s="32"/>
+      <c r="J26" s="32" t="s">
+        <v>167</v>
+      </c>
       <c r="K26" s="33"/>
       <c r="L26" s="33"/>
       <c r="M26" s="33"/>
-      <c r="N26" s="34"/>
+      <c r="N26" s="34" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="27" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
@@ -4839,7 +4846,7 @@
       </c>
       <c r="E90" s="67">
         <f ca="1">G86/(DATEDIF("2020-01-06",TODAY(),"d")/7)</f>
-        <v>17.305555555555554</v>
+        <v>17.115384615384617</v>
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.25">
@@ -5042,7 +5049,7 @@
       </c>
       <c r="C116" s="68">
         <f ca="1">E90</f>
-        <v>17.305555555555554</v>
+        <v>17.115384615384617</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LitRev: Clustering and MoG
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Desktop\thesisWindows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D20BAF3-0151-4FCD-A9BC-BBF7B4EE5921}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A536B2-FB41-4D42-85C4-1A728BB57E61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="175">
   <si>
     <t>Date</t>
   </si>
@@ -547,7 +547,16 @@
     <t>Researching MoG, brutal.</t>
   </si>
   <si>
-    <t>9:00 - 11:00 12:30 - 13:30 14:30 - 15:00 17:00 - 18:30</t>
+    <t>Researching MoG, brutal. + Adding to LitRev</t>
+  </si>
+  <si>
+    <t>9:00 - 11:00 12:30 - 13:30 14:30 - 15:00 17:00 - 18:30 19:45 - 20:45</t>
+  </si>
+  <si>
+    <t>9:00 - 11:00 12:30 - 14:30</t>
+  </si>
+  <si>
+    <t>Clustering + MoG LitReview</t>
   </si>
 </sst>
 </file>
@@ -558,7 +567,7 @@
     <numFmt numFmtId="164" formatCode="d\-mmm"/>
     <numFmt numFmtId="165" formatCode="d/mm/yyyy"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -609,6 +618,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFD9D9D9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -787,7 +802,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -959,6 +974,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1263,7 +1281,7 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>9.5</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -1284,7 +1302,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0">
-                  <c:v>17.462365591397848</c:v>
+                  <c:v>17.76063829787234</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1448,16 +1466,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>227880</xdr:colOff>
-      <xdr:row>82</xdr:row>
-      <xdr:rowOff>162000</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>468076</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>79174</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>2313081</xdr:colOff>
-      <xdr:row>106</xdr:row>
-      <xdr:rowOff>161280</xdr:rowOff>
+      <xdr:colOff>623429</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>78454</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1484,16 +1502,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>505239</xdr:colOff>
-      <xdr:row>90</xdr:row>
-      <xdr:rowOff>66261</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1209261</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>149087</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>865788</xdr:colOff>
-      <xdr:row>97</xdr:row>
-      <xdr:rowOff>18815</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2563722</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>101641</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1516,7 +1534,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4870174" y="25783761"/>
+          <a:off x="2749826" y="26819087"/>
           <a:ext cx="4791744" cy="1286054"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2204,8 +2222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F21" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" topLeftCell="G17" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3194,7 +3212,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
         <v>36</v>
       </c>
@@ -3213,18 +3231,20 @@
         <v>43929</v>
       </c>
       <c r="J28" s="32" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="K28" s="33"/>
       <c r="L28" s="33">
         <v>3.5</v>
       </c>
-      <c r="M28" s="33"/>
+      <c r="M28" s="33">
+        <v>2.5</v>
+      </c>
       <c r="N28" s="34" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
         <v>40</v>
       </c>
@@ -3242,11 +3262,17 @@
       <c r="I29" s="35">
         <v>43930</v>
       </c>
-      <c r="J29" s="32"/>
+      <c r="J29" s="32" t="s">
+        <v>173</v>
+      </c>
       <c r="K29" s="33"/>
       <c r="L29" s="33"/>
-      <c r="M29" s="33"/>
-      <c r="N29" s="40"/>
+      <c r="M29" s="33">
+        <v>4</v>
+      </c>
+      <c r="N29" s="70" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="22" t="s">
@@ -3372,11 +3398,11 @@
       </c>
       <c r="M33" s="8">
         <f>SUM(M26:M32)</f>
-        <v>2</v>
+        <v>8.5</v>
       </c>
       <c r="N33" s="29">
         <f>SUM(K33:M33)</f>
-        <v>9.5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
@@ -4879,15 +4905,15 @@
       </c>
       <c r="F86" s="61">
         <f>SUM(F81,F73,F65,F57,F49,F41,F33,F25,F17,F9,M9,M17,M25,M33,M41,M49,M57,M65,M73,M81)</f>
-        <v>40.5</v>
+        <v>47</v>
       </c>
       <c r="G86" s="63">
         <f>SUM(D86:F86) + 9</f>
-        <v>232</v>
+        <v>238.5</v>
       </c>
       <c r="H86" s="64">
         <f>G86/400</f>
-        <v>0.57999999999999996</v>
+        <v>0.59624999999999995</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.25">
@@ -4906,7 +4932,7 @@
       <c r="F88" s="61"/>
       <c r="G88" s="58">
         <f>G86*50</f>
-        <v>11600</v>
+        <v>11925</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
@@ -4918,7 +4944,7 @@
       </c>
       <c r="E90" s="67">
         <f ca="1">G86/(DATEDIF("2020-01-06",TODAY(),"d")/7)</f>
-        <v>17.462365591397848</v>
+        <v>17.76063829787234</v>
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.25">
@@ -5052,7 +5078,7 @@
       </c>
       <c r="C108" s="8">
         <f>N33</f>
-        <v>9.5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="109" spans="2:3" x14ac:dyDescent="0.25">
@@ -5121,7 +5147,7 @@
       </c>
       <c r="C116" s="68">
         <f ca="1">E90</f>
-        <v>17.462365591397848</v>
+        <v>17.76063829787234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Additions to LitRev MoG
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Desktop\thesisWindows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A536B2-FB41-4D42-85C4-1A728BB57E61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{521A103B-9525-43FE-AD3A-A22DBA2906B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -553,10 +553,10 @@
     <t>9:00 - 11:00 12:30 - 13:30 14:30 - 15:00 17:00 - 18:30 19:45 - 20:45</t>
   </si>
   <si>
-    <t>9:00 - 11:00 12:30 - 14:30</t>
-  </si>
-  <si>
     <t>Clustering + MoG LitReview</t>
+  </si>
+  <si>
+    <t>9:00 - 11:00 12:30 - 14:30 15:30 - 17:00 17:30 - 18:00</t>
   </si>
 </sst>
 </file>
@@ -1281,7 +1281,7 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>16</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -1302,7 +1302,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0">
-                  <c:v>17.76063829787234</c:v>
+                  <c:v>17.909574468085108</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2222,8 +2222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G17" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3244,7 +3244,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
         <v>40</v>
       </c>
@@ -3263,15 +3263,15 @@
         <v>43930</v>
       </c>
       <c r="J29" s="32" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="K29" s="33"/>
       <c r="L29" s="33"/>
       <c r="M29" s="33">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="N29" s="70" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -3398,11 +3398,11 @@
       </c>
       <c r="M33" s="8">
         <f>SUM(M26:M32)</f>
-        <v>8.5</v>
+        <v>10.5</v>
       </c>
       <c r="N33" s="29">
         <f>SUM(K33:M33)</f>
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
@@ -4905,15 +4905,15 @@
       </c>
       <c r="F86" s="61">
         <f>SUM(F81,F73,F65,F57,F49,F41,F33,F25,F17,F9,M9,M17,M25,M33,M41,M49,M57,M65,M73,M81)</f>
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G86" s="63">
         <f>SUM(D86:F86) + 9</f>
-        <v>238.5</v>
+        <v>240.5</v>
       </c>
       <c r="H86" s="64">
         <f>G86/400</f>
-        <v>0.59624999999999995</v>
+        <v>0.60124999999999995</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.25">
@@ -4932,7 +4932,7 @@
       <c r="F88" s="61"/>
       <c r="G88" s="58">
         <f>G86*50</f>
-        <v>11925</v>
+        <v>12025</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
@@ -4944,7 +4944,7 @@
       </c>
       <c r="E90" s="67">
         <f ca="1">G86/(DATEDIF("2020-01-06",TODAY(),"d")/7)</f>
-        <v>17.76063829787234</v>
+        <v>17.909574468085108</v>
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.25">
@@ -5078,7 +5078,7 @@
       </c>
       <c r="C108" s="8">
         <f>N33</f>
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="109" spans="2:3" x14ac:dyDescent="0.25">
@@ -5147,7 +5147,7 @@
       </c>
       <c r="C116" s="68">
         <f ca="1">E90</f>
-        <v>17.76063829787234</v>
+        <v>17.909574468085108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LitRev: Adding to MoG
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Desktop\thesisWindows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D5963AE-D04A-4299-B066-7E15589D1AF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E4D06B-B059-4CCA-B229-862F4ADB082E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -559,10 +559,10 @@
     <t>9:00 - 11:00 12:30 - 14:30 15:30 - 17:00 17:30 - 18:00</t>
   </si>
   <si>
-    <t>9:30 - 11:30</t>
-  </si>
-  <si>
     <t>LitRev: Mog and Gauss</t>
+  </si>
+  <si>
+    <t>9:30 - 11:30 12:30 - 14:30 15:30 - 16:30</t>
   </si>
 </sst>
 </file>
@@ -1287,7 +1287,7 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>20</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -1308,7 +1308,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0">
-                  <c:v>17.868421052631579</c:v>
+                  <c:v>18.163157894736841</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2228,8 +2228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N31" sqref="N31"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G93" sqref="G93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3280,7 +3280,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="22" t="s">
         <v>44</v>
       </c>
@@ -3299,15 +3299,15 @@
         <v>43931</v>
       </c>
       <c r="J30" s="32" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="K30" s="33"/>
       <c r="L30" s="33"/>
       <c r="M30" s="33">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="N30" s="32" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -3410,11 +3410,11 @@
       </c>
       <c r="M33" s="8">
         <f>SUM(M26:M32)</f>
-        <v>12.5</v>
+        <v>16.5</v>
       </c>
       <c r="N33" s="29">
         <f>SUM(K33:M33)</f>
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
@@ -4917,15 +4917,15 @@
       </c>
       <c r="F86" s="61">
         <f>SUM(F81,F73,F65,F57,F49,F41,F33,F25,F17,F9,M9,M17,M25,M33,M41,M49,M57,M65,M73,M81)</f>
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="G86" s="63">
         <f>SUM(D86:F86) + 9</f>
-        <v>242.5</v>
+        <v>246.5</v>
       </c>
       <c r="H86" s="64">
         <f>G86/400</f>
-        <v>0.60624999999999996</v>
+        <v>0.61624999999999996</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.25">
@@ -4944,7 +4944,7 @@
       <c r="F88" s="61"/>
       <c r="G88" s="58">
         <f>G86*50</f>
-        <v>12125</v>
+        <v>12325</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
@@ -4956,7 +4956,7 @@
       </c>
       <c r="E90" s="67">
         <f ca="1">G86/(DATEDIF("2020-01-06",TODAY(),"d")/7)</f>
-        <v>17.868421052631579</v>
+        <v>18.163157894736841</v>
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.25">
@@ -5090,7 +5090,7 @@
       </c>
       <c r="C108" s="8">
         <f>N33</f>
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="109" spans="2:3" x14ac:dyDescent="0.25">
@@ -5159,7 +5159,7 @@
       </c>
       <c r="C116" s="68">
         <f ca="1">E90</f>
-        <v>17.868421052631579</v>
+        <v>18.163157894736841</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Trying to finish off MoG
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Desktop\thesisWindows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E4D06B-B059-4CCA-B229-862F4ADB082E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9ECB434-5C23-4F41-A0AF-8BFA0242EB32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="179">
   <si>
     <t>Date</t>
   </si>
@@ -563,6 +563,12 @@
   </si>
   <si>
     <t>9:30 - 11:30 12:30 - 14:30 15:30 - 16:30</t>
+  </si>
+  <si>
+    <t>MoG</t>
+  </si>
+  <si>
+    <t>10:00 - 12:00 15:00-17:00</t>
   </si>
 </sst>
 </file>
@@ -1290,7 +1296,7 @@
                   <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0</c:v>
@@ -1308,7 +1314,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0">
-                  <c:v>18.163157894736841</c:v>
+                  <c:v>17.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2228,8 +2234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G93" sqref="G93"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3417,7 +3423,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="22" t="s">
         <v>28</v>
       </c>
@@ -3439,11 +3445,17 @@
       <c r="I34" s="25">
         <v>43934</v>
       </c>
-      <c r="J34" s="24"/>
+      <c r="J34" s="24" t="s">
+        <v>178</v>
+      </c>
       <c r="K34" s="8"/>
       <c r="L34" s="8"/>
-      <c r="M34" s="8"/>
-      <c r="N34" s="7"/>
+      <c r="M34" s="8">
+        <v>2</v>
+      </c>
+      <c r="N34" s="7" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="22" t="s">
@@ -3649,11 +3661,11 @@
       </c>
       <c r="M41" s="8">
         <f>SUM(M34:M40)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N41" s="29">
         <f>SUM(K41:M41)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -4917,15 +4929,15 @@
       </c>
       <c r="F86" s="61">
         <f>SUM(F81,F73,F65,F57,F49,F41,F33,F25,F17,F9,M9,M17,M25,M33,M41,M49,M57,M65,M73,M81)</f>
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G86" s="63">
         <f>SUM(D86:F86) + 9</f>
-        <v>246.5</v>
+        <v>248.5</v>
       </c>
       <c r="H86" s="64">
         <f>G86/400</f>
-        <v>0.61624999999999996</v>
+        <v>0.62124999999999997</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.25">
@@ -4944,7 +4956,7 @@
       <c r="F88" s="61"/>
       <c r="G88" s="58">
         <f>G86*50</f>
-        <v>12325</v>
+        <v>12425</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
@@ -4956,7 +4968,7 @@
       </c>
       <c r="E90" s="67">
         <f ca="1">G86/(DATEDIF("2020-01-06",TODAY(),"d")/7)</f>
-        <v>18.163157894736841</v>
+        <v>17.75</v>
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.25">
@@ -5099,7 +5111,7 @@
       </c>
       <c r="C109" s="8">
         <f>N41</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="110" spans="2:3" x14ac:dyDescent="0.25">
@@ -5159,7 +5171,7 @@
       </c>
       <c r="C116" s="68">
         <f ca="1">E90</f>
-        <v>18.163157894736841</v>
+        <v>17.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MoG, need to read Bishop (2006)
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Desktop\thesisWindows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9ECB434-5C23-4F41-A0AF-8BFA0242EB32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EAE400D-3271-45FA-9C86-8CC6F80D6A5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -568,7 +568,7 @@
     <t>MoG</t>
   </si>
   <si>
-    <t>10:00 - 12:00 15:00-17:00</t>
+    <t xml:space="preserve">10:00 - 12:00 15:00-17:00 19:00 - 20:00 </t>
   </si>
 </sst>
 </file>
@@ -1296,7 +1296,7 @@
                   <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0</c:v>
@@ -1314,7 +1314,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0">
-                  <c:v>17.75</c:v>
+                  <c:v>17.964285714285715</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2234,8 +2234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView tabSelected="1" topLeftCell="B32" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3423,7 +3423,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="22" t="s">
         <v>28</v>
       </c>
@@ -3451,7 +3451,7 @@
       <c r="K34" s="8"/>
       <c r="L34" s="8"/>
       <c r="M34" s="8">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N34" s="7" t="s">
         <v>177</v>
@@ -3661,11 +3661,11 @@
       </c>
       <c r="M41" s="8">
         <f>SUM(M34:M40)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N41" s="29">
         <f>SUM(K41:M41)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -4929,15 +4929,15 @@
       </c>
       <c r="F86" s="61">
         <f>SUM(F81,F73,F65,F57,F49,F41,F33,F25,F17,F9,M9,M17,M25,M33,M41,M49,M57,M65,M73,M81)</f>
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="G86" s="63">
         <f>SUM(D86:F86) + 9</f>
-        <v>248.5</v>
+        <v>251.5</v>
       </c>
       <c r="H86" s="64">
         <f>G86/400</f>
-        <v>0.62124999999999997</v>
+        <v>0.62875000000000003</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.25">
@@ -4956,7 +4956,7 @@
       <c r="F88" s="61"/>
       <c r="G88" s="58">
         <f>G86*50</f>
-        <v>12425</v>
+        <v>12575</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
@@ -4968,7 +4968,7 @@
       </c>
       <c r="E90" s="67">
         <f ca="1">G86/(DATEDIF("2020-01-06",TODAY(),"d")/7)</f>
-        <v>17.75</v>
+        <v>17.964285714285715</v>
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.25">
@@ -5111,7 +5111,7 @@
       </c>
       <c r="C109" s="8">
         <f>N41</f>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="110" spans="2:3" x14ac:dyDescent="0.25">
@@ -5171,7 +5171,7 @@
       </c>
       <c r="C116" s="68">
         <f ca="1">E90</f>
-        <v>17.75</v>
+        <v>17.964285714285715</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commencing Network Initial Build
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Desktop\thesisWindows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F954D820-26D1-429E-B307-780318AF1C16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{213277DE-4253-4B54-BEB8-8083FF92865B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="183">
   <si>
     <t>Date</t>
   </si>
@@ -571,10 +571,16 @@
     <t xml:space="preserve">10:00 - 12:00 15:00-17:00 19:00 - 20:00 </t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>10:00 - 12:00 16:30 - 18:30</t>
+    <t>10:00 - 12:00 16:30 - 18:30 23:00 - 23:30</t>
+  </si>
+  <si>
+    <t>9:30 - 11:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12:00 - 14:00  17:00 - 19:00 </t>
+  </si>
+  <si>
+    <t>Planning and learning Django</t>
   </si>
 </sst>
 </file>
@@ -1302,7 +1308,7 @@
                   <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>8.5</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0</c:v>
@@ -1320,7 +1326,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0">
-                  <c:v>18.030303030303031</c:v>
+                  <c:v>18.054455445544555</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2240,8 +2246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B33" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+    <sheetView tabSelected="1" topLeftCell="C7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N39" sqref="N39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3463,7 +3469,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="22" t="s">
         <v>32</v>
       </c>
@@ -3486,7 +3492,7 @@
         <v>43935</v>
       </c>
       <c r="J35" s="24" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="K35" s="8"/>
       <c r="L35" s="8">
@@ -3521,11 +3527,17 @@
       <c r="I36" s="25">
         <v>43936</v>
       </c>
-      <c r="J36" s="24"/>
+      <c r="J36" s="24" t="s">
+        <v>180</v>
+      </c>
       <c r="K36" s="8"/>
       <c r="L36" s="8"/>
-      <c r="M36" s="8"/>
-      <c r="N36" s="7"/>
+      <c r="M36" s="8">
+        <v>2</v>
+      </c>
+      <c r="N36" s="7" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="37" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="22" t="s">
@@ -3549,12 +3561,16 @@
       <c r="I37" s="25">
         <v>43937</v>
       </c>
-      <c r="J37" s="24"/>
-      <c r="K37" s="8"/>
+      <c r="J37" s="24" t="s">
+        <v>181</v>
+      </c>
+      <c r="K37" s="8">
+        <v>3.5</v>
+      </c>
       <c r="L37" s="8"/>
       <c r="M37" s="8"/>
       <c r="N37" s="7" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
@@ -3669,7 +3685,7 @@
       <c r="J41" s="7"/>
       <c r="K41" s="8">
         <f>SUM(K34:K40)</f>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="L41" s="8">
         <f>SUM(L34:L40)</f>
@@ -3677,11 +3693,11 @@
       </c>
       <c r="M41" s="8">
         <f>SUM(M34:M40)</f>
-        <v>7.5</v>
+        <v>9.5</v>
       </c>
       <c r="N41" s="29">
         <f>SUM(K41:M41)</f>
-        <v>8.5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -4937,7 +4953,7 @@
       </c>
       <c r="D86" s="61">
         <f>SUM(D81,D73,D65,D57,D49,D41,D33,D25,D17,D9,K9,K17,K25,K33,K41,K49,K57,K65,K73,K81)</f>
-        <v>98.5</v>
+        <v>102</v>
       </c>
       <c r="E86" s="61">
         <f>SUM(E81,E73,E65,E57,E49,E41,E33,E25,E17,E9,L9,L17,L25,L33,L41,L49,L57,L65,L73,L81)</f>
@@ -4945,15 +4961,15 @@
       </c>
       <c r="F86" s="61">
         <f>SUM(F81,F73,F65,F57,F49,F41,F33,F25,F17,F9,M9,M17,M25,M33,M41,M49,M57,M65,M73,M81)</f>
-        <v>62.5</v>
+        <v>64.5</v>
       </c>
       <c r="G86" s="63">
         <f>SUM(D86:F86) + 9</f>
-        <v>255</v>
+        <v>260.5</v>
       </c>
       <c r="H86" s="64">
         <f>G86/400</f>
-        <v>0.63749999999999996</v>
+        <v>0.65125</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.25">
@@ -4972,7 +4988,7 @@
       <c r="F88" s="61"/>
       <c r="G88" s="58">
         <f>G86*50</f>
-        <v>12750</v>
+        <v>13025</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
@@ -4984,7 +5000,7 @@
       </c>
       <c r="E90" s="67">
         <f ca="1">G86/(DATEDIF("2020-01-06",TODAY(),"d")/7)</f>
-        <v>18.030303030303031</v>
+        <v>18.054455445544555</v>
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.25">
@@ -5127,7 +5143,7 @@
       </c>
       <c r="C109" s="8">
         <f>N41</f>
-        <v>8.5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="110" spans="2:3" x14ac:dyDescent="0.25">
@@ -5187,7 +5203,7 @@
       </c>
       <c r="C116" s="68">
         <f ca="1">E90</f>
-        <v>18.030303030303031</v>
+        <v>18.054455445544555</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding complexity to Django
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Desktop\thesisWindows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{213277DE-4253-4B54-BEB8-8083FF92865B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{700C6D2F-16A6-481B-9C6E-016AFF2B610F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="187">
   <si>
     <t>Date</t>
   </si>
@@ -577,10 +577,22 @@
     <t>9:30 - 11:30</t>
   </si>
   <si>
-    <t xml:space="preserve">12:00 - 14:00  17:00 - 19:00 </t>
-  </si>
-  <si>
     <t>Planning and learning Django</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12:00 - 13:30  17:00 - 19:00 </t>
+  </si>
+  <si>
+    <t>Learning Django Basics</t>
+  </si>
+  <si>
+    <t>9:00 - 11:00 11:30 - 13:30  16:00 - 16:30</t>
+  </si>
+  <si>
+    <t>Django</t>
+  </si>
+  <si>
+    <t>11:00 - 12:00 13:30 - 15:30</t>
   </si>
 </sst>
 </file>
@@ -1308,7 +1320,7 @@
                   <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14</c:v>
+                  <c:v>19.5</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0</c:v>
@@ -1326,7 +1338,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0">
-                  <c:v>18.054455445544555</c:v>
+                  <c:v>18.077669902912621</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2246,8 +2258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N39" sqref="N39"/>
+    <sheetView tabSelected="1" topLeftCell="C31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3562,7 +3574,7 @@
         <v>43937</v>
       </c>
       <c r="J37" s="24" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="K37" s="8">
         <v>3.5</v>
@@ -3570,10 +3582,10 @@
       <c r="L37" s="8"/>
       <c r="M37" s="8"/>
       <c r="N37" s="7" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="22" t="s">
         <v>44</v>
       </c>
@@ -3595,11 +3607,17 @@
       <c r="I38" s="25">
         <v>43938</v>
       </c>
-      <c r="J38" s="24"/>
-      <c r="K38" s="8"/>
+      <c r="J38" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="K38" s="8">
+        <v>3.5</v>
+      </c>
       <c r="L38" s="8"/>
       <c r="M38" s="8"/>
-      <c r="N38" s="7"/>
+      <c r="N38" s="7" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="39" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="22" t="s">
@@ -3623,11 +3641,17 @@
       <c r="I39" s="25">
         <v>43939</v>
       </c>
-      <c r="J39" s="24"/>
-      <c r="K39" s="8"/>
+      <c r="J39" s="24" t="s">
+        <v>186</v>
+      </c>
+      <c r="K39" s="8">
+        <v>2</v>
+      </c>
       <c r="L39" s="8"/>
       <c r="M39" s="8"/>
-      <c r="N39" s="7"/>
+      <c r="N39" s="7" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="22" t="s">
@@ -3685,7 +3709,7 @@
       <c r="J41" s="7"/>
       <c r="K41" s="8">
         <f>SUM(K34:K40)</f>
-        <v>3.5</v>
+        <v>9</v>
       </c>
       <c r="L41" s="8">
         <f>SUM(L34:L40)</f>
@@ -3697,7 +3721,7 @@
       </c>
       <c r="N41" s="29">
         <f>SUM(K41:M41)</f>
-        <v>14</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -4953,7 +4977,7 @@
       </c>
       <c r="D86" s="61">
         <f>SUM(D81,D73,D65,D57,D49,D41,D33,D25,D17,D9,K9,K17,K25,K33,K41,K49,K57,K65,K73,K81)</f>
-        <v>102</v>
+        <v>107.5</v>
       </c>
       <c r="E86" s="61">
         <f>SUM(E81,E73,E65,E57,E49,E41,E33,E25,E17,E9,L9,L17,L25,L33,L41,L49,L57,L65,L73,L81)</f>
@@ -4965,11 +4989,11 @@
       </c>
       <c r="G86" s="63">
         <f>SUM(D86:F86) + 9</f>
-        <v>260.5</v>
+        <v>266</v>
       </c>
       <c r="H86" s="64">
         <f>G86/400</f>
-        <v>0.65125</v>
+        <v>0.66500000000000004</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.25">
@@ -4988,7 +5012,7 @@
       <c r="F88" s="61"/>
       <c r="G88" s="58">
         <f>G86*50</f>
-        <v>13025</v>
+        <v>13300</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
@@ -5000,7 +5024,7 @@
       </c>
       <c r="E90" s="67">
         <f ca="1">G86/(DATEDIF("2020-01-06",TODAY(),"d")/7)</f>
-        <v>18.054455445544555</v>
+        <v>18.077669902912621</v>
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.25">
@@ -5143,7 +5167,7 @@
       </c>
       <c r="C109" s="8">
         <f>N41</f>
-        <v>14</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="110" spans="2:3" x14ac:dyDescent="0.25">
@@ -5203,7 +5227,7 @@
       </c>
       <c r="C116" s="68">
         <f ca="1">E90</f>
-        <v>18.054455445544555</v>
+        <v>18.077669902912621</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding tests to Django
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Desktop\thesisWindows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{700C6D2F-16A6-481B-9C6E-016AFF2B610F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D75CF807-6F1D-4AC5-A4E0-AAB66E256981}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="189">
   <si>
     <t>Date</t>
   </si>
@@ -593,6 +593,12 @@
   </si>
   <si>
     <t>11:00 - 12:00 13:30 - 15:30</t>
+  </si>
+  <si>
+    <t>22:30 - 23:30</t>
+  </si>
+  <si>
+    <t>12:30 - 13:00 21:30-22:30</t>
   </si>
 </sst>
 </file>
@@ -1320,10 +1326,10 @@
                   <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>19.5</c:v>
+                  <c:v>20.5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>0</c:v>
@@ -1338,7 +1344,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0">
-                  <c:v>18.077669902912621</c:v>
+                  <c:v>17.866666666666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2259,7 +2265,7 @@
   <dimension ref="A1:AMK116"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K40" sqref="K40"/>
+      <selection activeCell="N44" sqref="N44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3675,11 +3681,17 @@
       <c r="I40" s="25">
         <v>43940</v>
       </c>
-      <c r="J40" s="24"/>
-      <c r="K40" s="8"/>
+      <c r="J40" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="K40" s="8">
+        <v>1</v>
+      </c>
       <c r="L40" s="8"/>
       <c r="M40" s="8"/>
-      <c r="N40" s="7"/>
+      <c r="N40" s="7" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="28" t="s">
@@ -3709,7 +3721,7 @@
       <c r="J41" s="7"/>
       <c r="K41" s="8">
         <f>SUM(K34:K40)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L41" s="8">
         <f>SUM(L34:L40)</f>
@@ -3721,7 +3733,7 @@
       </c>
       <c r="N41" s="29">
         <f>SUM(K41:M41)</f>
-        <v>19.5</v>
+        <v>20.5</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -3748,8 +3760,12 @@
       <c r="I42" s="35">
         <v>43941</v>
       </c>
-      <c r="J42" s="32"/>
-      <c r="K42" s="33"/>
+      <c r="J42" s="32" t="s">
+        <v>188</v>
+      </c>
+      <c r="K42" s="33">
+        <v>1</v>
+      </c>
       <c r="L42" s="33"/>
       <c r="M42" s="33"/>
       <c r="N42" s="34"/>
@@ -3943,7 +3959,7 @@
       <c r="J49" s="32"/>
       <c r="K49" s="8">
         <f>SUM(K42:K48)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L49" s="8">
         <f>SUM(L42:L48)</f>
@@ -3955,7 +3971,7 @@
       </c>
       <c r="N49" s="29">
         <f>SUM(K49:M49)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
@@ -4977,7 +4993,7 @@
       </c>
       <c r="D86" s="61">
         <f>SUM(D81,D73,D65,D57,D49,D41,D33,D25,D17,D9,K9,K17,K25,K33,K41,K49,K57,K65,K73,K81)</f>
-        <v>107.5</v>
+        <v>109.5</v>
       </c>
       <c r="E86" s="61">
         <f>SUM(E81,E73,E65,E57,E49,E41,E33,E25,E17,E9,L9,L17,L25,L33,L41,L49,L57,L65,L73,L81)</f>
@@ -4989,11 +5005,11 @@
       </c>
       <c r="G86" s="63">
         <f>SUM(D86:F86) + 9</f>
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="H86" s="64">
         <f>G86/400</f>
-        <v>0.66500000000000004</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.25">
@@ -5012,7 +5028,7 @@
       <c r="F88" s="61"/>
       <c r="G88" s="58">
         <f>G86*50</f>
-        <v>13300</v>
+        <v>13400</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
@@ -5024,7 +5040,7 @@
       </c>
       <c r="E90" s="67">
         <f ca="1">G86/(DATEDIF("2020-01-06",TODAY(),"d")/7)</f>
-        <v>18.077669902912621</v>
+        <v>17.866666666666667</v>
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.25">
@@ -5167,7 +5183,7 @@
       </c>
       <c r="C109" s="8">
         <f>N41</f>
-        <v>19.5</v>
+        <v>20.5</v>
       </c>
     </row>
     <row r="110" spans="2:3" x14ac:dyDescent="0.25">
@@ -5176,7 +5192,7 @@
       </c>
       <c r="C110" s="8">
         <f>N49</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="111" spans="2:3" x14ac:dyDescent="0.25">
@@ -5227,7 +5243,7 @@
       </c>
       <c r="C116" s="68">
         <f ca="1">E90</f>
-        <v>18.077669902912621</v>
+        <v>17.866666666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sync up for pi
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Desktop\thesisWindows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D75CF807-6F1D-4AC5-A4E0-AAB66E256981}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA731CA9-8894-4BD6-871B-315ECCA4090F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="195">
   <si>
     <t>Date</t>
   </si>
@@ -599,6 +599,24 @@
   </si>
   <si>
     <t>12:30 - 13:00 21:30-22:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Django Site + Django Video </t>
+  </si>
+  <si>
+    <t>14:00 - 16:00 20:15 - 22:45</t>
+  </si>
+  <si>
+    <t>9:15 - 11:15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Streaming Video </t>
+  </si>
+  <si>
+    <t>19:00 - 20:00</t>
+  </si>
+  <si>
+    <t>Streaming Detection Results</t>
   </si>
 </sst>
 </file>
@@ -1329,7 +1347,7 @@
                   <c:v>20.5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>0</c:v>
@@ -1344,7 +1362,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0">
-                  <c:v>17.866666666666667</c:v>
+                  <c:v>17.726851851851851</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2264,8 +2282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N44" sqref="N44"/>
+    <sheetView tabSelected="1" topLeftCell="C33" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N46" sqref="N46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3770,7 +3788,7 @@
       <c r="M42" s="33"/>
       <c r="N42" s="34"/>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="22" t="s">
         <v>32</v>
       </c>
@@ -3788,11 +3806,17 @@
       <c r="I43" s="35">
         <v>43942</v>
       </c>
-      <c r="J43" s="32"/>
-      <c r="K43" s="33"/>
+      <c r="J43" s="32" t="s">
+        <v>190</v>
+      </c>
+      <c r="K43" s="33">
+        <v>4.5</v>
+      </c>
       <c r="L43" s="33"/>
       <c r="M43" s="33"/>
-      <c r="N43" s="34"/>
+      <c r="N43" s="34" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="44" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="22" t="s">
@@ -3818,11 +3842,17 @@
       <c r="I44" s="35">
         <v>43943</v>
       </c>
-      <c r="J44" s="32"/>
-      <c r="K44" s="33"/>
+      <c r="J44" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="K44" s="33">
+        <v>1</v>
+      </c>
       <c r="L44" s="33"/>
       <c r="M44" s="33"/>
-      <c r="N44" s="34"/>
+      <c r="N44" s="34" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="45" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="22" t="s">
@@ -3848,11 +3878,15 @@
       <c r="I45" s="35">
         <v>43944</v>
       </c>
-      <c r="J45" s="32"/>
+      <c r="J45" s="32" t="s">
+        <v>193</v>
+      </c>
       <c r="K45" s="33"/>
       <c r="L45" s="33"/>
       <c r="M45" s="33"/>
-      <c r="N45" s="34"/>
+      <c r="N45" s="34" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="22" t="s">
@@ -3959,7 +3993,7 @@
       <c r="J49" s="32"/>
       <c r="K49" s="8">
         <f>SUM(K42:K48)</f>
-        <v>1</v>
+        <v>6.5</v>
       </c>
       <c r="L49" s="8">
         <f>SUM(L42:L48)</f>
@@ -3971,7 +4005,7 @@
       </c>
       <c r="N49" s="29">
         <f>SUM(K49:M49)</f>
-        <v>1</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
@@ -4993,7 +5027,7 @@
       </c>
       <c r="D86" s="61">
         <f>SUM(D81,D73,D65,D57,D49,D41,D33,D25,D17,D9,K9,K17,K25,K33,K41,K49,K57,K65,K73,K81)</f>
-        <v>109.5</v>
+        <v>115</v>
       </c>
       <c r="E86" s="61">
         <f>SUM(E81,E73,E65,E57,E49,E41,E33,E25,E17,E9,L9,L17,L25,L33,L41,L49,L57,L65,L73,L81)</f>
@@ -5005,11 +5039,11 @@
       </c>
       <c r="G86" s="63">
         <f>SUM(D86:F86) + 9</f>
-        <v>268</v>
+        <v>273.5</v>
       </c>
       <c r="H86" s="64">
         <f>G86/400</f>
-        <v>0.67</v>
+        <v>0.68374999999999997</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.25">
@@ -5028,7 +5062,7 @@
       <c r="F88" s="61"/>
       <c r="G88" s="58">
         <f>G86*50</f>
-        <v>13400</v>
+        <v>13675</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
@@ -5040,7 +5074,7 @@
       </c>
       <c r="E90" s="67">
         <f ca="1">G86/(DATEDIF("2020-01-06",TODAY(),"d")/7)</f>
-        <v>17.866666666666667</v>
+        <v>17.726851851851851</v>
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.25">
@@ -5192,7 +5226,7 @@
       </c>
       <c r="C110" s="8">
         <f>N49</f>
-        <v>1</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="111" spans="2:3" x14ac:dyDescent="0.25">
@@ -5243,7 +5277,7 @@
       </c>
       <c r="C116" s="68">
         <f ca="1">E90</f>
-        <v>17.866666666666667</v>
+        <v>17.726851851851851</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Running Flask and Detection Simultaneously
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Desktop\thesisWindows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C736B8E0-14DF-4398-9C37-EA3CDAF72C67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0987F668-B8D3-4113-967F-45137B25B94B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -625,7 +625,7 @@
     <t>09:00 - 10:30 14:30 - 15:30 17:00 - 18:00 19:30 - 20:00 21:00 - 23:00</t>
   </si>
   <si>
-    <t>09:30-11:30</t>
+    <t>09:30-11:30 13:30 - 15:30</t>
   </si>
 </sst>
 </file>
@@ -1356,7 +1356,7 @@
                   <c:v>20.5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>14.5</c:v>
+                  <c:v>16.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>0</c:v>
@@ -1371,7 +1371,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0">
-                  <c:v>17.913636363636364</c:v>
+                  <c:v>18.040909090909093</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2291,8 +2291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C45" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N48" sqref="N48"/>
+    <sheetView tabSelected="1" topLeftCell="C87" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G92" sqref="G92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3929,7 +3929,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="22" t="s">
         <v>48</v>
       </c>
@@ -3950,7 +3950,9 @@
       <c r="J47" s="32" t="s">
         <v>197</v>
       </c>
-      <c r="K47" s="33"/>
+      <c r="K47" s="33">
+        <v>2</v>
+      </c>
       <c r="L47" s="33"/>
       <c r="M47" s="33"/>
       <c r="N47" s="32" t="s">
@@ -4014,7 +4016,7 @@
       <c r="J49" s="32"/>
       <c r="K49" s="8">
         <f>SUM(K42:K48)</f>
-        <v>14.5</v>
+        <v>16.5</v>
       </c>
       <c r="L49" s="8">
         <f>SUM(L42:L48)</f>
@@ -4026,7 +4028,7 @@
       </c>
       <c r="N49" s="29">
         <f>SUM(K49:M49)</f>
-        <v>14.5</v>
+        <v>16.5</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
@@ -5048,7 +5050,7 @@
       </c>
       <c r="D86" s="61">
         <f>SUM(D81,D73,D65,D57,D49,D41,D33,D25,D17,D9,K9,K17,K25,K33,K41,K49,K57,K65,K73,K81)</f>
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E86" s="61">
         <f>SUM(E81,E73,E65,E57,E49,E41,E33,E25,E17,E9,L9,L17,L25,L33,L41,L49,L57,L65,L73,L81)</f>
@@ -5060,11 +5062,11 @@
       </c>
       <c r="G86" s="63">
         <f>SUM(D86:F86) + 9</f>
-        <v>281.5</v>
+        <v>283.5</v>
       </c>
       <c r="H86" s="64">
         <f>G86/400</f>
-        <v>0.70374999999999999</v>
+        <v>0.70874999999999999</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.25">
@@ -5083,7 +5085,7 @@
       <c r="F88" s="61"/>
       <c r="G88" s="58">
         <f>G86*50</f>
-        <v>14075</v>
+        <v>14175</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
@@ -5095,7 +5097,7 @@
       </c>
       <c r="E90" s="67">
         <f ca="1">G86/(DATEDIF("2020-01-06",TODAY(),"d")/7)</f>
-        <v>17.913636363636364</v>
+        <v>18.040909090909093</v>
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.25">
@@ -5247,7 +5249,7 @@
       </c>
       <c r="C110" s="8">
         <f>N49</f>
-        <v>14.5</v>
+        <v>16.5</v>
       </c>
     </row>
     <row r="111" spans="2:3" x14ac:dyDescent="0.25">
@@ -5298,7 +5300,7 @@
       </c>
       <c r="C116" s="68">
         <f ca="1">E90</f>
-        <v>17.913636363636364</v>
+        <v>18.040909090909093</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Webstream begin integration, destruction?
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Desktop\thesisWindows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0987F668-B8D3-4113-967F-45137B25B94B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{563D3093-3F44-46E4-B7D4-477349E28A30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="201">
   <si>
     <t>Date</t>
   </si>
@@ -626,6 +626,15 @@
   </si>
   <si>
     <t>09:30-11:30 13:30 - 15:30</t>
+  </si>
+  <si>
+    <t>10:30 - 11:30</t>
+  </si>
+  <si>
+    <t>10:30-12:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flask </t>
   </si>
 </sst>
 </file>
@@ -1356,7 +1365,7 @@
                   <c:v>20.5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>16.5</c:v>
+                  <c:v>18.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>0</c:v>
@@ -1371,7 +1380,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0">
-                  <c:v>18.040909090909093</c:v>
+                  <c:v>17.84375</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2291,8 +2300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C87" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G92" sqref="G92"/>
+    <sheetView tabSelected="1" topLeftCell="C36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J51" sqref="J51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3951,7 +3960,7 @@
         <v>197</v>
       </c>
       <c r="K47" s="33">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L47" s="33"/>
       <c r="M47" s="33"/>
@@ -3983,11 +3992,17 @@
       <c r="I48" s="35">
         <v>43947</v>
       </c>
-      <c r="J48" s="32"/>
-      <c r="K48" s="33"/>
+      <c r="J48" s="32" t="s">
+        <v>198</v>
+      </c>
+      <c r="K48" s="33">
+        <v>1</v>
+      </c>
       <c r="L48" s="33"/>
       <c r="M48" s="33"/>
-      <c r="N48" s="32"/>
+      <c r="N48" s="32" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="28" t="s">
@@ -4016,7 +4031,7 @@
       <c r="J49" s="32"/>
       <c r="K49" s="8">
         <f>SUM(K42:K48)</f>
-        <v>16.5</v>
+        <v>18.5</v>
       </c>
       <c r="L49" s="8">
         <f>SUM(L42:L48)</f>
@@ -4028,7 +4043,7 @@
       </c>
       <c r="N49" s="29">
         <f>SUM(K49:M49)</f>
-        <v>16.5</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
@@ -4053,11 +4068,15 @@
       <c r="I50" s="25">
         <v>43948</v>
       </c>
-      <c r="J50" s="24"/>
+      <c r="J50" s="24" t="s">
+        <v>199</v>
+      </c>
       <c r="K50" s="8"/>
       <c r="L50" s="8"/>
       <c r="M50" s="8"/>
-      <c r="N50" s="7"/>
+      <c r="N50" s="7" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="51" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="22" t="s">
@@ -5050,7 +5069,7 @@
       </c>
       <c r="D86" s="61">
         <f>SUM(D81,D73,D65,D57,D49,D41,D33,D25,D17,D9,K9,K17,K25,K33,K41,K49,K57,K65,K73,K81)</f>
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E86" s="61">
         <f>SUM(E81,E73,E65,E57,E49,E41,E33,E25,E17,E9,L9,L17,L25,L33,L41,L49,L57,L65,L73,L81)</f>
@@ -5062,11 +5081,11 @@
       </c>
       <c r="G86" s="63">
         <f>SUM(D86:F86) + 9</f>
-        <v>283.5</v>
+        <v>285.5</v>
       </c>
       <c r="H86" s="64">
         <f>G86/400</f>
-        <v>0.70874999999999999</v>
+        <v>0.71375</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.25">
@@ -5085,7 +5104,7 @@
       <c r="F88" s="61"/>
       <c r="G88" s="58">
         <f>G86*50</f>
-        <v>14175</v>
+        <v>14275</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
@@ -5097,7 +5116,7 @@
       </c>
       <c r="E90" s="67">
         <f ca="1">G86/(DATEDIF("2020-01-06",TODAY(),"d")/7)</f>
-        <v>18.040909090909093</v>
+        <v>17.84375</v>
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.25">
@@ -5249,7 +5268,7 @@
       </c>
       <c r="C110" s="8">
         <f>N49</f>
-        <v>16.5</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="111" spans="2:3" x14ac:dyDescent="0.25">
@@ -5300,7 +5319,7 @@
       </c>
       <c r="C116" s="68">
         <f ca="1">E90</f>
-        <v>18.040909090909093</v>
+        <v>17.84375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Running on three threads
- Main: Handles instance creation and calling threads 
  for web and detection.
- Detection: The CV 
- Web Manger: Grabs frames and writes time stamp on them. Could probably cut this thread out.

As yet data is not shared between threads but they do function concurrently.
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Desktop\thesisWindows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E294A0-BD43-40EB-818A-A39129CABE2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1ECAA41-8E87-4FA7-8250-8B8D48B3A19C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="211">
   <si>
     <t>Date</t>
   </si>
@@ -640,7 +640,31 @@
     <t>Learning Flask</t>
   </si>
   <si>
-    <t>09:30 - 11:30 13:15 - 12:45 18:30 - 20:00</t>
+    <t>09:30 - 11:30 13:15 - 12:45 19:30 - 21:30</t>
+  </si>
+  <si>
+    <t>Implementing Flask App</t>
+  </si>
+  <si>
+    <t>09:00-11:00 13:30 - 15:30 20:00 - 22:00</t>
+  </si>
+  <si>
+    <t>Flask App</t>
+  </si>
+  <si>
+    <t>11:00 - 13:00 15:00 - 15:15 21:00 - 23:00</t>
+  </si>
+  <si>
+    <t>11:30 - 12:30</t>
+  </si>
+  <si>
+    <t>12:30 - 14:00</t>
+  </si>
+  <si>
+    <t>Flask App + Detection</t>
+  </si>
+  <si>
+    <t>10:30 - 11:30 17:00 - 19:00</t>
   </si>
 </sst>
 </file>
@@ -1374,10 +1398,10 @@
                   <c:v>18.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9.5</c:v>
+                  <c:v>24.5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0</c:v>
@@ -1386,7 +1410,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0">
-                  <c:v>18.274336283185843</c:v>
+                  <c:v>18.294117647058822</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2306,8 +2330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C42" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K51" sqref="K51"/>
+    <sheetView tabSelected="1" topLeftCell="C52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J59" sqref="J59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4112,7 +4136,7 @@
         <v>202</v>
       </c>
       <c r="K51" s="8">
-        <v>3.5</v>
+        <v>5.75</v>
       </c>
       <c r="L51" s="8"/>
       <c r="M51" s="8"/>
@@ -4120,7 +4144,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="22" t="s">
         <v>36</v>
       </c>
@@ -4142,13 +4166,19 @@
       <c r="I52" s="25">
         <v>43950</v>
       </c>
-      <c r="J52" s="24"/>
-      <c r="K52" s="8"/>
+      <c r="J52" s="24" t="s">
+        <v>204</v>
+      </c>
+      <c r="K52" s="8">
+        <v>6</v>
+      </c>
       <c r="L52" s="8"/>
       <c r="M52" s="8"/>
-      <c r="N52" s="7"/>
-    </row>
-    <row r="53" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="N52" s="7" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="22" t="s">
         <v>40</v>
       </c>
@@ -4170,11 +4200,17 @@
       <c r="I53" s="25">
         <v>43951</v>
       </c>
-      <c r="J53" s="41"/>
-      <c r="K53" s="8"/>
+      <c r="J53" s="41" t="s">
+        <v>206</v>
+      </c>
+      <c r="K53" s="8">
+        <v>4.25</v>
+      </c>
       <c r="L53" s="8"/>
       <c r="M53" s="8"/>
-      <c r="N53" s="7"/>
+      <c r="N53" s="7" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="54" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="22" t="s">
@@ -4198,11 +4234,17 @@
       <c r="I54" s="25">
         <v>43952</v>
       </c>
-      <c r="J54" s="41"/>
-      <c r="K54" s="8"/>
+      <c r="J54" s="41" t="s">
+        <v>207</v>
+      </c>
+      <c r="K54" s="8">
+        <v>1</v>
+      </c>
       <c r="L54" s="8"/>
       <c r="M54" s="8"/>
-      <c r="N54" s="7"/>
+      <c r="N54" s="7" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="22" t="s">
@@ -4248,11 +4290,17 @@
       <c r="I56" s="25">
         <v>43954</v>
       </c>
-      <c r="J56" s="24"/>
-      <c r="K56" s="8"/>
+      <c r="J56" s="24" t="s">
+        <v>208</v>
+      </c>
+      <c r="K56" s="8">
+        <v>1.5</v>
+      </c>
       <c r="L56" s="8"/>
       <c r="M56" s="8"/>
-      <c r="N56" s="7"/>
+      <c r="N56" s="7" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="28" t="s">
@@ -4282,7 +4330,7 @@
       <c r="J57" s="7"/>
       <c r="K57" s="8">
         <f>SUM(K50:K56)</f>
-        <v>9.5</v>
+        <v>24.5</v>
       </c>
       <c r="L57" s="8">
         <f>SUM(L50:L56)</f>
@@ -4294,10 +4342,10 @@
       </c>
       <c r="N57" s="29">
         <f>SUM(K57:M57)</f>
-        <v>9.5</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="22" t="s">
         <v>28</v>
       </c>
@@ -4323,11 +4371,17 @@
       <c r="I58" s="35">
         <v>43955</v>
       </c>
-      <c r="J58" s="32"/>
-      <c r="K58" s="33"/>
+      <c r="J58" s="32" t="s">
+        <v>210</v>
+      </c>
+      <c r="K58" s="33">
+        <v>1</v>
+      </c>
       <c r="L58" s="33"/>
       <c r="M58" s="33"/>
-      <c r="N58" s="34"/>
+      <c r="N58" s="34" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="22" t="s">
@@ -4528,7 +4582,7 @@
       <c r="J65" s="47"/>
       <c r="K65" s="8">
         <f>SUM(K58:K64)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L65" s="8">
         <f>SUM(L58:L64)</f>
@@ -4540,7 +4594,7 @@
       </c>
       <c r="N65" s="29">
         <f>SUM(K65:M65)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -5083,7 +5137,7 @@
       </c>
       <c r="D86" s="61">
         <f>SUM(D81,D73,D65,D57,D49,D41,D33,D25,D17,D9,K9,K17,K25,K33,K41,K49,K57,K65,K73,K81)</f>
-        <v>136.5</v>
+        <v>152.5</v>
       </c>
       <c r="E86" s="61">
         <f>SUM(E81,E73,E65,E57,E49,E41,E33,E25,E17,E9,L9,L17,L25,L33,L41,L49,L57,L65,L73,L81)</f>
@@ -5095,11 +5149,11 @@
       </c>
       <c r="G86" s="63">
         <f>SUM(D86:F86) + 9</f>
-        <v>295</v>
+        <v>311</v>
       </c>
       <c r="H86" s="64">
         <f>G86/400</f>
-        <v>0.73750000000000004</v>
+        <v>0.77749999999999997</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.25">
@@ -5118,7 +5172,7 @@
       <c r="F88" s="61"/>
       <c r="G88" s="58">
         <f>G86*50</f>
-        <v>14750</v>
+        <v>15550</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
@@ -5130,7 +5184,7 @@
       </c>
       <c r="E90" s="67">
         <f ca="1">G86/(DATEDIF("2020-01-06",TODAY(),"d")/7)</f>
-        <v>18.274336283185843</v>
+        <v>18.294117647058822</v>
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.25">
@@ -5291,7 +5345,7 @@
       </c>
       <c r="C111" s="8">
         <f>N57</f>
-        <v>9.5</v>
+        <v>24.5</v>
       </c>
     </row>
     <row r="112" spans="2:3" x14ac:dyDescent="0.25">
@@ -5300,7 +5354,7 @@
       </c>
       <c r="C112" s="8">
         <f>N65</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="113" spans="2:3" x14ac:dyDescent="0.25">
@@ -5333,7 +5387,7 @@
       </c>
       <c r="C116" s="68">
         <f ca="1">E90</f>
-        <v>18.274336283185843</v>
+        <v>18.294117647058822</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Decided to keep it local database, added time stamp to graphics.
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Desktop\thesisWindows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CDDDF0A-6F33-49C6-A1D5-A365D9692496}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B36447-E085-4CCE-8B82-CE55B0B18B75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="225">
   <si>
     <t>Date</t>
   </si>
@@ -701,6 +701,12 @@
   </si>
   <si>
     <t>10:00 - 12:00 13:00 - 15:00 19:30 - 21:30</t>
+  </si>
+  <si>
+    <t>Database Webhosting</t>
+  </si>
+  <si>
+    <t>10:45 - 13:45</t>
   </si>
 </sst>
 </file>
@@ -1525,7 +1531,7 @@
                   <c:v>24.5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>15</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0</c:v>
@@ -1534,7 +1540,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0">
-                  <c:v>18.647540983606557</c:v>
+                  <c:v>18.780487804878046</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2454,9 +2460,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK116"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J61" sqref="J61"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J63" sqref="J63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5274,7 +5280,7 @@
         <v>222</v>
       </c>
       <c r="K61" s="16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L61" s="16"/>
       <c r="M61" s="16"/>
@@ -5311,12 +5317,16 @@
       <c r="I62" s="15">
         <v>43959</v>
       </c>
-      <c r="J62" s="41"/>
-      <c r="K62" s="16"/>
+      <c r="J62" s="41" t="s">
+        <v>224</v>
+      </c>
+      <c r="K62" s="16">
+        <v>3</v>
+      </c>
       <c r="L62" s="16"/>
       <c r="M62" s="16"/>
       <c r="N62" s="41" t="s">
-        <v>211</v>
+        <v>223</v>
       </c>
       <c r="O62" s="35" t="s">
         <v>44</v>
@@ -5352,9 +5362,7 @@
       <c r="K63" s="16"/>
       <c r="L63" s="16"/>
       <c r="M63" s="16"/>
-      <c r="N63" s="41" t="s">
-        <v>211</v>
-      </c>
+      <c r="N63" s="41"/>
       <c r="O63" s="35" t="s">
         <v>48</v>
       </c>
@@ -5395,9 +5403,7 @@
       <c r="K64" s="16"/>
       <c r="L64" s="16"/>
       <c r="M64" s="16"/>
-      <c r="N64" s="41" t="s">
-        <v>211</v>
-      </c>
+      <c r="N64" s="41"/>
       <c r="O64" s="35" t="s">
         <v>52</v>
       </c>
@@ -5443,7 +5449,7 @@
       <c r="J65" s="55"/>
       <c r="K65" s="37">
         <f>SUM(K58:K64)</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="L65" s="37">
         <f>SUM(L58:L64)</f>
@@ -5455,7 +5461,7 @@
       </c>
       <c r="N65" s="40">
         <f>SUM(K65:M65)</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="O65" s="39"/>
       <c r="P65" s="71"/>
@@ -6146,7 +6152,7 @@
       </c>
       <c r="D86" s="64">
         <f>SUM(D81,D73,D65,D57,D49,D41,D33,D25,D17,D9,K9,K17,K25,K33,K41,K49,K57,K65,K73,K81)</f>
-        <v>166.5</v>
+        <v>171.5</v>
       </c>
       <c r="E86" s="64">
         <f>SUM(E81,E73,E65,E57,E49,E41,E33,E25,E17,E9,L9,L17,L25,L33,L41,L49,L57,L65,L73,L81)</f>
@@ -6158,11 +6164,11 @@
       </c>
       <c r="G86" s="25">
         <f>SUM(D86:F86) + 9</f>
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="H86" s="66">
         <f>G86/400</f>
-        <v>0.8125</v>
+        <v>0.82499999999999996</v>
       </c>
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.25">
@@ -6181,7 +6187,7 @@
       <c r="F88" s="64"/>
       <c r="G88" s="22">
         <f>G86*50</f>
-        <v>16250</v>
+        <v>16500</v>
       </c>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.25">
@@ -6193,7 +6199,7 @@
       </c>
       <c r="E90" s="28">
         <f ca="1">G86/(DATEDIF("2020-01-06",TODAY(),"d")/7)</f>
-        <v>18.647540983606557</v>
+        <v>18.780487804878046</v>
       </c>
     </row>
     <row r="94" spans="1:21" x14ac:dyDescent="0.25">
@@ -6363,7 +6369,7 @@
       </c>
       <c r="C112" s="7">
         <f>N65</f>
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="113" spans="2:3" x14ac:dyDescent="0.25">
@@ -6396,7 +6402,7 @@
       </c>
       <c r="C116" s="29">
         <f ca="1">E90</f>
-        <v>18.647540983606557</v>
+        <v>18.780487804878046</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Storing statistics in database at regular intervals.
Stores counts in database. Need to write function to store opposite traffic count as well.
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Desktop\thesisWindows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B36447-E085-4CCE-8B82-CE55B0B18B75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC0D578-7191-4406-847B-537F1E1DEE88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="228">
   <si>
     <t>Date</t>
   </si>
@@ -706,7 +706,16 @@
     <t>Database Webhosting</t>
   </si>
   <si>
-    <t>10:45 - 13:45</t>
+    <t>10:45 - 13:45 17:00 - 18:00</t>
+  </si>
+  <si>
+    <t>Database functionality</t>
+  </si>
+  <si>
+    <t>21:30 - 22:30</t>
+  </si>
+  <si>
+    <t>Integrating Database</t>
   </si>
 </sst>
 </file>
@@ -1531,7 +1540,7 @@
                   <c:v>24.5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>20</c:v>
+                  <c:v>22.5</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0</c:v>
@@ -1540,7 +1549,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0">
-                  <c:v>18.780487804878046</c:v>
+                  <c:v>18.77016129032258</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2461,8 +2470,8 @@
   <dimension ref="A1:AMK116"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J63" sqref="J63"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N65" sqref="N65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5299,7 +5308,7 @@
       <c r="T61" s="46"/>
       <c r="U61" s="46"/>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="35" t="s">
         <v>44</v>
       </c>
@@ -5321,7 +5330,7 @@
         <v>224</v>
       </c>
       <c r="K62" s="16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L62" s="16"/>
       <c r="M62" s="16"/>
@@ -5358,11 +5367,17 @@
       <c r="I63" s="15">
         <v>43960</v>
       </c>
-      <c r="J63" s="41"/>
-      <c r="K63" s="16"/>
+      <c r="J63" s="41" t="s">
+        <v>226</v>
+      </c>
+      <c r="K63" s="16">
+        <v>1.5</v>
+      </c>
       <c r="L63" s="16"/>
       <c r="M63" s="16"/>
-      <c r="N63" s="41"/>
+      <c r="N63" s="41" t="s">
+        <v>225</v>
+      </c>
       <c r="O63" s="35" t="s">
         <v>48</v>
       </c>
@@ -5403,7 +5418,9 @@
       <c r="K64" s="16"/>
       <c r="L64" s="16"/>
       <c r="M64" s="16"/>
-      <c r="N64" s="41"/>
+      <c r="N64" s="41" t="s">
+        <v>227</v>
+      </c>
       <c r="O64" s="35" t="s">
         <v>52</v>
       </c>
@@ -5449,7 +5466,7 @@
       <c r="J65" s="55"/>
       <c r="K65" s="37">
         <f>SUM(K58:K64)</f>
-        <v>20</v>
+        <v>22.5</v>
       </c>
       <c r="L65" s="37">
         <f>SUM(L58:L64)</f>
@@ -5461,7 +5478,7 @@
       </c>
       <c r="N65" s="40">
         <f>SUM(K65:M65)</f>
-        <v>20</v>
+        <v>22.5</v>
       </c>
       <c r="O65" s="39"/>
       <c r="P65" s="71"/>
@@ -6152,7 +6169,7 @@
       </c>
       <c r="D86" s="64">
         <f>SUM(D81,D73,D65,D57,D49,D41,D33,D25,D17,D9,K9,K17,K25,K33,K41,K49,K57,K65,K73,K81)</f>
-        <v>171.5</v>
+        <v>174</v>
       </c>
       <c r="E86" s="64">
         <f>SUM(E81,E73,E65,E57,E49,E41,E33,E25,E17,E9,L9,L17,L25,L33,L41,L49,L57,L65,L73,L81)</f>
@@ -6164,11 +6181,11 @@
       </c>
       <c r="G86" s="25">
         <f>SUM(D86:F86) + 9</f>
-        <v>330</v>
+        <v>332.5</v>
       </c>
       <c r="H86" s="66">
         <f>G86/400</f>
-        <v>0.82499999999999996</v>
+        <v>0.83125000000000004</v>
       </c>
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.25">
@@ -6187,7 +6204,7 @@
       <c r="F88" s="64"/>
       <c r="G88" s="22">
         <f>G86*50</f>
-        <v>16500</v>
+        <v>16625</v>
       </c>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.25">
@@ -6199,7 +6216,7 @@
       </c>
       <c r="E90" s="28">
         <f ca="1">G86/(DATEDIF("2020-01-06",TODAY(),"d")/7)</f>
-        <v>18.780487804878046</v>
+        <v>18.77016129032258</v>
       </c>
     </row>
     <row r="94" spans="1:21" x14ac:dyDescent="0.25">
@@ -6369,7 +6386,7 @@
       </c>
       <c r="C112" s="7">
         <f>N65</f>
-        <v>20</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="113" spans="2:3" x14ac:dyDescent="0.25">
@@ -6402,7 +6419,7 @@
       </c>
       <c r="C116" s="29">
         <f ca="1">E90</f>
-        <v>18.780487804878046</v>
+        <v>18.77016129032258</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added to Introduction and Refining LitRev
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Desktop\thesisWindows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{228B0669-3F25-4268-B320-94069F7C2F23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C202A1B-2F0D-4162-B239-DEB43D538F58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="248">
   <si>
     <t>Date</t>
   </si>
@@ -673,9 +673,6 @@
     <t>12:00 - 13:30 17:00 - 19:00 20:30 - 21:30</t>
   </si>
   <si>
-    <t xml:space="preserve">Report + Reassess Situation </t>
-  </si>
-  <si>
     <t>Wk22</t>
   </si>
   <si>
@@ -725,18 +722,73 @@
   </si>
   <si>
     <t>10:30 - 11:30 12:00 - 13:30 15:30 - 17:30</t>
+  </si>
+  <si>
+    <t>Web App</t>
+  </si>
+  <si>
+    <t>10:30 - 12:30 14:30 - 17:00 21:00 - 22:00</t>
+  </si>
+  <si>
+    <t>Plotting Matplotlib</t>
+  </si>
+  <si>
+    <t>16:00 - 18:30</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Due</t>
+  </si>
+  <si>
+    <t>Demo</t>
+  </si>
+  <si>
+    <t>WebApp Plotting</t>
+  </si>
+  <si>
+    <t>11:00 - 13:30 15:00 - 15:30 20:00 - 23:30</t>
+  </si>
+  <si>
+    <t>11:00 - 13:00 20:00 - 22:00</t>
+  </si>
+  <si>
+    <t>11:30 - 13:30 14:30 - 16:30 17:30 - 18:00 21:00 - 00:00</t>
+  </si>
+  <si>
+    <t>WebApp Form</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web App Plotting </t>
+  </si>
+  <si>
+    <t>12:00 - 15:00 17:00 - 19:00 21:00 - 00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Form Validation </t>
+  </si>
+  <si>
+    <t>11:30 - 13:00 20:30- 10:30</t>
+  </si>
+  <si>
+    <t>11:15 - 12:45 14:00 - 16:00 20:30 - 22:30</t>
+  </si>
+  <si>
+    <t>Report Introduction + Lit Review</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="d\-mmm"/>
     <numFmt numFmtId="165" formatCode="d/mm/yyyy"/>
     <numFmt numFmtId="166" formatCode="[$-409]d/mmm;@"/>
+    <numFmt numFmtId="167" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -789,6 +841,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFD9D9D9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFD9D9D9"/>
       <name val="Calibri"/>
@@ -995,7 +1054,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1217,6 +1276,15 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1552,13 +1620,13 @@
                   <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4.5</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0">
-                  <c:v>18.861111111111111</c:v>
+                  <c:v>19.651851851851852</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1754,50 +1822,6 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1209261</xdr:colOff>
-      <xdr:row>91</xdr:row>
-      <xdr:rowOff>149087</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>2563722</xdr:colOff>
-      <xdr:row>98</xdr:row>
-      <xdr:rowOff>101641</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{248EAB12-EBDB-4DD1-9A55-E1EBE5039240}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2749826" y="26819087"/>
-          <a:ext cx="4791744" cy="1286054"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2124,18 +2148,18 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="76" t="s">
+      <c r="G1" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
-      <c r="L1" s="76"/>
-      <c r="M1" s="76"/>
-      <c r="N1" s="76"/>
-      <c r="O1" s="76"/>
-      <c r="P1" s="76"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
+      <c r="L1" s="79"/>
+      <c r="M1" s="79"/>
+      <c r="N1" s="79"/>
+      <c r="O1" s="79"/>
+      <c r="P1" s="79"/>
       <c r="Q1" s="2"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -2478,9 +2502,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K71" sqref="K70:K71"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N77" sqref="N77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2488,7 +2512,8 @@
     <col min="1" max="1" width="11.5703125" style="67"/>
     <col min="2" max="2" width="11.5703125" style="5"/>
     <col min="3" max="3" width="19.28515625" style="6" customWidth="1"/>
-    <col min="4" max="5" width="11.5703125" style="7"/>
+    <col min="4" max="4" width="11.5703125" style="7"/>
+    <col min="5" max="5" width="21.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="7" customWidth="1"/>
     <col min="7" max="7" width="57.28515625" style="6" customWidth="1"/>
     <col min="8" max="8" width="29" style="61" customWidth="1"/>
@@ -2938,7 +2963,7 @@
         <v>17</v>
       </c>
       <c r="O9" s="39" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="P9" s="68" t="s">
         <v>55</v>
@@ -3282,7 +3307,7 @@
         <v>11.5</v>
       </c>
       <c r="O17" s="39" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="P17" s="48" t="s">
         <v>55</v>
@@ -3637,7 +3662,7 @@
         <v>15</v>
       </c>
       <c r="O25" s="39" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="P25" s="48"/>
       <c r="Q25" s="5"/>
@@ -3996,7 +4021,7 @@
         <v>24</v>
       </c>
       <c r="O33" s="39" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="P33" s="48" t="s">
         <v>55</v>
@@ -4383,7 +4408,7 @@
         <v>20.5</v>
       </c>
       <c r="O41" s="39" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="P41" s="48" t="s">
         <v>55</v>
@@ -4745,7 +4770,7 @@
         <v>18.5</v>
       </c>
       <c r="O49" s="39" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="P49" s="71" t="s">
         <v>55</v>
@@ -5118,7 +5143,7 @@
         <v>24.5</v>
       </c>
       <c r="O57" s="39" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="P57" s="48" t="s">
         <v>55</v>
@@ -5246,7 +5271,7 @@
         <v>43957</v>
       </c>
       <c r="J60" s="41" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K60" s="16">
         <v>3.5</v>
@@ -5295,7 +5320,7 @@
         <v>43958</v>
       </c>
       <c r="J61" s="41" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K61" s="16">
         <v>6</v>
@@ -5336,7 +5361,7 @@
         <v>43959</v>
       </c>
       <c r="J62" s="41" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K62" s="16">
         <v>4</v>
@@ -5344,7 +5369,7 @@
       <c r="L62" s="16"/>
       <c r="M62" s="16"/>
       <c r="N62" s="41" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="O62" s="35" t="s">
         <v>44</v>
@@ -5377,7 +5402,7 @@
         <v>43960</v>
       </c>
       <c r="J63" s="41" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="K63" s="16">
         <v>1.5</v>
@@ -5385,7 +5410,7 @@
       <c r="L63" s="16"/>
       <c r="M63" s="16"/>
       <c r="N63" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="O63" s="35" t="s">
         <v>48</v>
@@ -5424,7 +5449,7 @@
         <v>43961</v>
       </c>
       <c r="J64" s="41" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="K64" s="16">
         <v>2.5</v>
@@ -5432,7 +5457,7 @@
       <c r="L64" s="16"/>
       <c r="M64" s="16"/>
       <c r="N64" s="41" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="O64" s="35" t="s">
         <v>52</v>
@@ -5526,7 +5551,7 @@
         <v>43962</v>
       </c>
       <c r="J66" s="36" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="K66" s="37">
         <v>4.5</v>
@@ -5534,7 +5559,7 @@
       <c r="L66" s="37"/>
       <c r="M66" s="37"/>
       <c r="N66" s="38" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="O66" s="72"/>
       <c r="P66" s="73"/>
@@ -5544,7 +5569,7 @@
       <c r="T66" s="74"/>
       <c r="U66" s="74"/>
     </row>
-    <row r="67" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" s="35" t="s">
         <v>32</v>
       </c>
@@ -5568,12 +5593,16 @@
       <c r="I67" s="12">
         <v>43963</v>
       </c>
-      <c r="J67" s="36"/>
-      <c r="K67" s="37"/>
+      <c r="J67" s="36" t="s">
+        <v>231</v>
+      </c>
+      <c r="K67" s="37">
+        <v>6.5</v>
+      </c>
       <c r="L67" s="37"/>
       <c r="M67" s="37"/>
       <c r="N67" s="38" t="s">
-        <v>26</v>
+        <v>230</v>
       </c>
       <c r="O67" s="72"/>
       <c r="P67" s="73"/>
@@ -5607,12 +5636,16 @@
       <c r="I68" s="12">
         <v>43964</v>
       </c>
-      <c r="J68" s="36"/>
-      <c r="K68" s="37"/>
+      <c r="J68" s="36" t="s">
+        <v>233</v>
+      </c>
+      <c r="K68" s="37">
+        <v>1.5</v>
+      </c>
       <c r="L68" s="37"/>
       <c r="M68" s="37"/>
       <c r="N68" s="38" t="s">
-        <v>26</v>
+        <v>232</v>
       </c>
       <c r="O68" s="72"/>
       <c r="P68" s="73"/>
@@ -5622,7 +5655,7 @@
       <c r="T68" s="74"/>
       <c r="U68" s="74"/>
     </row>
-    <row r="69" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" s="35" t="s">
         <v>40</v>
       </c>
@@ -5646,12 +5679,16 @@
       <c r="I69" s="12">
         <v>43965</v>
       </c>
-      <c r="J69" s="36"/>
-      <c r="K69" s="37"/>
+      <c r="J69" s="36" t="s">
+        <v>238</v>
+      </c>
+      <c r="K69" s="37">
+        <v>6.5</v>
+      </c>
       <c r="L69" s="37"/>
       <c r="M69" s="37"/>
       <c r="N69" s="38" t="s">
-        <v>26</v>
+        <v>237</v>
       </c>
       <c r="O69" s="72"/>
       <c r="P69" s="73"/>
@@ -5661,7 +5698,7 @@
       <c r="T69" s="74"/>
       <c r="U69" s="74"/>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="35" t="s">
         <v>44</v>
       </c>
@@ -5685,12 +5722,16 @@
       <c r="I70" s="12">
         <v>43966</v>
       </c>
-      <c r="J70" s="36"/>
-      <c r="K70" s="37"/>
+      <c r="J70" s="36" t="s">
+        <v>239</v>
+      </c>
+      <c r="K70" s="37">
+        <v>4.5</v>
+      </c>
       <c r="L70" s="37"/>
       <c r="M70" s="37"/>
       <c r="N70" s="38" t="s">
-        <v>26</v>
+        <v>230</v>
       </c>
       <c r="O70" s="72"/>
       <c r="P70" s="73"/>
@@ -5700,7 +5741,7 @@
       <c r="T70" s="74"/>
       <c r="U70" s="74"/>
     </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A71" s="35" t="s">
         <v>48</v>
       </c>
@@ -5724,12 +5765,16 @@
       <c r="I71" s="12">
         <v>43967</v>
       </c>
-      <c r="J71" s="38"/>
-      <c r="K71" s="37"/>
+      <c r="J71" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="K71" s="37">
+        <v>7.5</v>
+      </c>
       <c r="L71" s="37"/>
       <c r="M71" s="37"/>
       <c r="N71" s="38" t="s">
-        <v>26</v>
+        <v>242</v>
       </c>
       <c r="O71" s="72"/>
       <c r="P71" s="73"/>
@@ -5767,9 +5812,7 @@
       <c r="K72" s="37"/>
       <c r="L72" s="37"/>
       <c r="M72" s="37"/>
-      <c r="N72" s="38" t="s">
-        <v>213</v>
-      </c>
+      <c r="N72" s="38"/>
       <c r="O72" s="72"/>
       <c r="P72" s="73"/>
       <c r="Q72" s="74"/>
@@ -5811,7 +5854,7 @@
       <c r="J73" s="38"/>
       <c r="K73" s="37">
         <f>SUM(K66:K72)</f>
-        <v>4.5</v>
+        <v>31</v>
       </c>
       <c r="L73" s="37">
         <f>SUM(L66:L72)</f>
@@ -5823,7 +5866,7 @@
       </c>
       <c r="N73" s="40">
         <f>SUM(K73:M73)</f>
-        <v>4.5</v>
+        <v>31</v>
       </c>
       <c r="O73" s="75"/>
       <c r="P73" s="73"/>
@@ -5833,7 +5876,7 @@
       <c r="T73" s="74"/>
       <c r="U73" s="74"/>
     </row>
-    <row r="74" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A74" s="35" t="s">
         <v>28</v>
       </c>
@@ -5857,11 +5900,17 @@
       <c r="I74" s="15">
         <v>43969</v>
       </c>
-      <c r="J74" s="41"/>
-      <c r="K74" s="16"/>
+      <c r="J74" s="41" t="s">
+        <v>243</v>
+      </c>
+      <c r="K74" s="16">
+        <v>8</v>
+      </c>
       <c r="L74" s="16"/>
       <c r="M74" s="16"/>
-      <c r="N74" s="42"/>
+      <c r="N74" s="42" t="s">
+        <v>241</v>
+      </c>
       <c r="O74" s="72"/>
       <c r="P74" s="73"/>
       <c r="Q74" s="74"/>
@@ -5894,11 +5943,17 @@
       <c r="I75" s="15">
         <v>43970</v>
       </c>
-      <c r="J75" s="41"/>
-      <c r="K75" s="16"/>
+      <c r="J75" s="41" t="s">
+        <v>245</v>
+      </c>
+      <c r="K75" s="16">
+        <v>1.5</v>
+      </c>
       <c r="L75" s="16"/>
       <c r="M75" s="16"/>
-      <c r="N75" s="42"/>
+      <c r="N75" s="42" t="s">
+        <v>244</v>
+      </c>
       <c r="O75" s="72"/>
       <c r="P75" s="73"/>
       <c r="Q75" s="74"/>
@@ -5907,7 +5962,7 @@
       <c r="T75" s="74"/>
       <c r="U75" s="74"/>
     </row>
-    <row r="76" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A76" s="35" t="s">
         <v>36</v>
       </c>
@@ -5931,11 +5986,17 @@
       <c r="I76" s="15">
         <v>43971</v>
       </c>
-      <c r="J76" s="41"/>
-      <c r="K76" s="16"/>
+      <c r="J76" s="41" t="s">
+        <v>246</v>
+      </c>
+      <c r="K76" s="16">
+        <v>3.5</v>
+      </c>
       <c r="L76" s="16"/>
       <c r="M76" s="16"/>
-      <c r="N76" s="42"/>
+      <c r="N76" s="42" t="s">
+        <v>247</v>
+      </c>
       <c r="O76" s="72"/>
       <c r="P76" s="73"/>
       <c r="Q76" s="74"/>
@@ -6109,7 +6170,7 @@
       <c r="J81" s="41"/>
       <c r="K81" s="37">
         <f>SUM(K74:K80)</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="L81" s="37">
         <f>SUM(L74:L80)</f>
@@ -6121,7 +6182,7 @@
       </c>
       <c r="N81" s="40">
         <f>SUM(K81:M81)</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="O81" s="74"/>
       <c r="P81" s="73"/>
@@ -6186,7 +6247,7 @@
       </c>
       <c r="D86" s="64">
         <f>SUM(D81,D73,D65,D57,D49,D41,D33,D25,D17,D9,K9,K17,K25,K33,K41,K49,K57,K65,K73,K81)</f>
-        <v>181</v>
+        <v>220.5</v>
       </c>
       <c r="E86" s="64">
         <f>SUM(E81,E73,E65,E57,E49,E41,E33,E25,E17,E9,L9,L17,L25,L33,L41,L49,L57,L65,L73,L81)</f>
@@ -6198,11 +6259,11 @@
       </c>
       <c r="G86" s="25">
         <f>SUM(D86:F86) + 9</f>
-        <v>339.5</v>
+        <v>379</v>
       </c>
       <c r="H86" s="66">
         <f>G86/400</f>
-        <v>0.84875</v>
+        <v>0.94750000000000001</v>
       </c>
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.25">
@@ -6221,7 +6282,7 @@
       <c r="F88" s="64"/>
       <c r="G88" s="22">
         <f>G86*50</f>
-        <v>16975</v>
+        <v>18950</v>
       </c>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.25">
@@ -6233,7 +6294,15 @@
       </c>
       <c r="E90" s="28">
         <f ca="1">G86/(DATEDIF("2020-01-06",TODAY(),"d")/7)</f>
-        <v>18.861111111111111</v>
+        <v>19.651851851851852</v>
+      </c>
+    </row>
+    <row r="93" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="D93" s="76" t="s">
+        <v>234</v>
+      </c>
+      <c r="E93" s="76" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="94" spans="1:21" x14ac:dyDescent="0.25">
@@ -6243,6 +6312,12 @@
       <c r="C94" s="7" t="s">
         <v>6</v>
       </c>
+      <c r="D94" s="77" t="s">
+        <v>26</v>
+      </c>
+      <c r="E94" s="78">
+        <v>44008</v>
+      </c>
     </row>
     <row r="95" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B95" s="7" t="s">
@@ -6252,6 +6327,12 @@
         <f>G9</f>
         <v>18.5</v>
       </c>
+      <c r="D95" s="77" t="s">
+        <v>236</v>
+      </c>
+      <c r="E95" s="78">
+        <v>44014</v>
+      </c>
     </row>
     <row r="96" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B96" s="7" t="s">
@@ -6412,7 +6493,7 @@
       </c>
       <c r="C113" s="7">
         <f>N73</f>
-        <v>4.5</v>
+        <v>31</v>
       </c>
     </row>
     <row r="114" spans="2:3" x14ac:dyDescent="0.25">
@@ -6421,7 +6502,7 @@
       </c>
       <c r="C114" s="7">
         <f>N81</f>
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.25">
@@ -6436,7 +6517,7 @@
       </c>
       <c r="C116" s="29">
         <f ca="1">E90</f>
-        <v>18.861111111111111</v>
+        <v>19.651851851851852</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added to Linear Filtering
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Desktop\thesisWindows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C202A1B-2F0D-4162-B239-DEB43D538F58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA90CA2D-F059-4A5E-8B19-94283AFD0286}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="250">
   <si>
     <t>Date</t>
   </si>
@@ -772,10 +772,16 @@
     <t>11:30 - 13:00 20:30- 10:30</t>
   </si>
   <si>
-    <t>11:15 - 12:45 14:00 - 16:00 20:30 - 22:30</t>
-  </si>
-  <si>
     <t>Report Introduction + Lit Review</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11:15 - 12:45 14:00 - 16:00 </t>
+  </si>
+  <si>
+    <t>01:00 - 02:00</t>
+  </si>
+  <si>
+    <t>Report: Lit Rev</t>
   </si>
 </sst>
 </file>
@@ -1623,10 +1629,10 @@
                   <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>13</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0">
-                  <c:v>19.651851851851852</c:v>
+                  <c:v>19.610294117647062</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2504,7 +2510,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N77" sqref="N77"/>
+      <selection pane="bottomLeft" activeCell="M78" sqref="M78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5962,7 +5968,7 @@
       <c r="T75" s="74"/>
       <c r="U75" s="74"/>
     </row>
-    <row r="76" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="35" t="s">
         <v>36</v>
       </c>
@@ -5987,15 +5993,15 @@
         <v>43971</v>
       </c>
       <c r="J76" s="41" t="s">
+        <v>247</v>
+      </c>
+      <c r="K76" s="16"/>
+      <c r="L76" s="16"/>
+      <c r="M76" s="16">
+        <v>3.5</v>
+      </c>
+      <c r="N76" s="42" t="s">
         <v>246</v>
-      </c>
-      <c r="K76" s="16">
-        <v>3.5</v>
-      </c>
-      <c r="L76" s="16"/>
-      <c r="M76" s="16"/>
-      <c r="N76" s="42" t="s">
-        <v>247</v>
       </c>
       <c r="O76" s="72"/>
       <c r="P76" s="73"/>
@@ -6029,11 +6035,17 @@
       <c r="I77" s="15">
         <v>43972</v>
       </c>
-      <c r="J77" s="41"/>
+      <c r="J77" s="41" t="s">
+        <v>248</v>
+      </c>
       <c r="K77" s="16"/>
       <c r="L77" s="16"/>
-      <c r="M77" s="16"/>
-      <c r="N77" s="42"/>
+      <c r="M77" s="16">
+        <v>2</v>
+      </c>
+      <c r="N77" s="42" t="s">
+        <v>249</v>
+      </c>
       <c r="O77" s="72"/>
       <c r="P77" s="73"/>
       <c r="Q77" s="74"/>
@@ -6170,7 +6182,7 @@
       <c r="J81" s="41"/>
       <c r="K81" s="37">
         <f>SUM(K74:K80)</f>
-        <v>13</v>
+        <v>9.5</v>
       </c>
       <c r="L81" s="37">
         <f>SUM(L74:L80)</f>
@@ -6178,11 +6190,11 @@
       </c>
       <c r="M81" s="37">
         <f>SUM(M74:M80)</f>
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="N81" s="40">
         <f>SUM(K81:M81)</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="O81" s="74"/>
       <c r="P81" s="73"/>
@@ -6247,7 +6259,7 @@
       </c>
       <c r="D86" s="64">
         <f>SUM(D81,D73,D65,D57,D49,D41,D33,D25,D17,D9,K9,K17,K25,K33,K41,K49,K57,K65,K73,K81)</f>
-        <v>220.5</v>
+        <v>217</v>
       </c>
       <c r="E86" s="64">
         <f>SUM(E81,E73,E65,E57,E49,E41,E33,E25,E17,E9,L9,L17,L25,L33,L41,L49,L57,L65,L73,L81)</f>
@@ -6255,15 +6267,15 @@
       </c>
       <c r="F86" s="64">
         <f>SUM(F81,F73,F65,F57,F49,F41,F33,F25,F17,F9,M9,M17,M25,M33,M41,M49,M57,M65,M73,M81)</f>
-        <v>64.5</v>
+        <v>70</v>
       </c>
       <c r="G86" s="25">
         <f>SUM(D86:F86) + 9</f>
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="H86" s="66">
         <f>G86/400</f>
-        <v>0.94750000000000001</v>
+        <v>0.95250000000000001</v>
       </c>
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.25">
@@ -6282,7 +6294,7 @@
       <c r="F88" s="64"/>
       <c r="G88" s="22">
         <f>G86*50</f>
-        <v>18950</v>
+        <v>19050</v>
       </c>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.25">
@@ -6294,7 +6306,7 @@
       </c>
       <c r="E90" s="28">
         <f ca="1">G86/(DATEDIF("2020-01-06",TODAY(),"d")/7)</f>
-        <v>19.651851851851852</v>
+        <v>19.610294117647062</v>
       </c>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.25">
@@ -6502,7 +6514,7 @@
       </c>
       <c r="C114" s="7">
         <f>N81</f>
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.25">
@@ -6517,7 +6529,7 @@
       </c>
       <c r="C116" s="29">
         <f ca="1">E90</f>
-        <v>19.651851851851852</v>
+        <v>19.610294117647062</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved on and added to litrev.
Improved INtroduction and linear filters. 
Addded nonlinear filters and morphology.
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Desktop\thesisWindows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA90CA2D-F059-4A5E-8B19-94283AFD0286}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B2376E9-470C-4AAB-A270-B2758198EF08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -778,10 +778,10 @@
     <t xml:space="preserve">11:15 - 12:45 14:00 - 16:00 </t>
   </si>
   <si>
-    <t>01:00 - 02:00</t>
-  </si>
-  <si>
     <t>Report: Lit Rev</t>
+  </si>
+  <si>
+    <t>01:00 - 02:00 13:00- 15:00 16:30 - 17:30 19:30 - 20:30</t>
   </si>
 </sst>
 </file>
@@ -1629,10 +1629,10 @@
                   <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>15</c:v>
+                  <c:v>19.5</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0">
-                  <c:v>19.610294117647062</c:v>
+                  <c:v>19.841911764705884</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2509,8 +2509,8 @@
   <dimension ref="A1:AMK116"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M78" sqref="M78"/>
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G99" sqref="G99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6011,7 +6011,7 @@
       <c r="T76" s="74"/>
       <c r="U76" s="74"/>
     </row>
-    <row r="77" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A77" s="35" t="s">
         <v>40</v>
       </c>
@@ -6036,15 +6036,15 @@
         <v>43972</v>
       </c>
       <c r="J77" s="41" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="K77" s="16"/>
       <c r="L77" s="16"/>
       <c r="M77" s="16">
-        <v>2</v>
+        <v>6.5</v>
       </c>
       <c r="N77" s="42" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="O77" s="72"/>
       <c r="P77" s="73"/>
@@ -6190,11 +6190,11 @@
       </c>
       <c r="M81" s="37">
         <f>SUM(M74:M80)</f>
-        <v>5.5</v>
+        <v>10</v>
       </c>
       <c r="N81" s="40">
         <f>SUM(K81:M81)</f>
-        <v>15</v>
+        <v>19.5</v>
       </c>
       <c r="O81" s="74"/>
       <c r="P81" s="73"/>
@@ -6267,15 +6267,15 @@
       </c>
       <c r="F86" s="64">
         <f>SUM(F81,F73,F65,F57,F49,F41,F33,F25,F17,F9,M9,M17,M25,M33,M41,M49,M57,M65,M73,M81)</f>
-        <v>70</v>
+        <v>74.5</v>
       </c>
       <c r="G86" s="25">
         <f>SUM(D86:F86) + 9</f>
-        <v>381</v>
+        <v>385.5</v>
       </c>
       <c r="H86" s="66">
         <f>G86/400</f>
-        <v>0.95250000000000001</v>
+        <v>0.96375</v>
       </c>
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.25">
@@ -6294,7 +6294,7 @@
       <c r="F88" s="64"/>
       <c r="G88" s="22">
         <f>G86*50</f>
-        <v>19050</v>
+        <v>19275</v>
       </c>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.25">
@@ -6306,7 +6306,7 @@
       </c>
       <c r="E90" s="28">
         <f ca="1">G86/(DATEDIF("2020-01-06",TODAY(),"d")/7)</f>
-        <v>19.610294117647062</v>
+        <v>19.841911764705884</v>
       </c>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.25">
@@ -6514,7 +6514,7 @@
       </c>
       <c r="C114" s="7">
         <f>N81</f>
-        <v>15</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.25">
@@ -6529,7 +6529,7 @@
       </c>
       <c r="C116" s="29">
         <f ca="1">E90</f>
-        <v>19.610294117647062</v>
+        <v>19.841911764705884</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nutting out design in report
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Desktop\thesisWindows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C32FAE87-3143-44F7-B6C6-6F03CD1F6942}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B5B665-1E22-4A40-A152-7FC3A43670C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="256">
   <si>
     <t>Date</t>
   </si>
@@ -791,6 +791,15 @@
   </si>
   <si>
     <t xml:space="preserve"> 20:30 - 21:30</t>
+  </si>
+  <si>
+    <t>Report: Design</t>
+  </si>
+  <si>
+    <t>20:00-22:00</t>
+  </si>
+  <si>
+    <t>11:00 - 13:00</t>
   </si>
 </sst>
 </file>
@@ -1638,10 +1647,13 @@
                   <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>25.5</c:v>
+                  <c:v>27.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0">
-                  <c:v>19.85869565217391</c:v>
+                  <c:v>19.725000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2517,9 +2529,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK116"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M79" sqref="M79"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2652,10 +2664,14 @@
       <c r="P2" s="68">
         <v>43976</v>
       </c>
-      <c r="Q2" s="69"/>
+      <c r="Q2" s="69" t="s">
+        <v>255</v>
+      </c>
       <c r="R2" s="69"/>
       <c r="S2" s="69"/>
-      <c r="T2" s="69"/>
+      <c r="T2" s="69">
+        <v>1</v>
+      </c>
       <c r="U2" s="69"/>
     </row>
     <row r="3" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2984,10 +3000,22 @@
         <v>55</v>
       </c>
       <c r="Q9" s="69"/>
-      <c r="R9" s="69"/>
-      <c r="S9" s="69"/>
-      <c r="T9" s="69"/>
-      <c r="U9" s="69"/>
+      <c r="R9" s="69">
+        <f>SUM(R2:R8)</f>
+        <v>0</v>
+      </c>
+      <c r="S9" s="69">
+        <f>SUM(S2:S8)</f>
+        <v>0</v>
+      </c>
+      <c r="T9" s="69">
+        <f>SUM(T2:T8)</f>
+        <v>1</v>
+      </c>
+      <c r="U9" s="69">
+        <f>SUM(R9:T9)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="35" t="s">
@@ -6132,7 +6160,9 @@
       <c r="M79" s="16">
         <v>1.5</v>
       </c>
-      <c r="N79" s="41"/>
+      <c r="N79" s="41" t="s">
+        <v>253</v>
+      </c>
       <c r="O79" s="72"/>
       <c r="P79" s="73"/>
       <c r="Q79" s="74"/>
@@ -6159,11 +6189,17 @@
       <c r="I80" s="15">
         <v>43975</v>
       </c>
-      <c r="J80" s="41"/>
+      <c r="J80" s="41" t="s">
+        <v>254</v>
+      </c>
       <c r="K80" s="16"/>
       <c r="L80" s="16"/>
-      <c r="M80" s="16"/>
-      <c r="N80" s="41"/>
+      <c r="M80" s="16">
+        <v>2</v>
+      </c>
+      <c r="N80" s="41" t="s">
+        <v>253</v>
+      </c>
       <c r="O80" s="72"/>
       <c r="P80" s="73"/>
       <c r="Q80" s="74"/>
@@ -6209,11 +6245,11 @@
       </c>
       <c r="M81" s="37">
         <f>SUM(M74:M80)</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="N81" s="40">
         <f>SUM(K81:M81)</f>
-        <v>25.5</v>
+        <v>27.5</v>
       </c>
       <c r="O81" s="74"/>
       <c r="P81" s="73"/>
@@ -6277,24 +6313,24 @@
         <v>147</v>
       </c>
       <c r="D86" s="64">
-        <f>SUM(D81,D73,D65,D57,D49,D41,D33,D25,D17,D9,K9,K17,K25,K33,K41,K49,K57,K65,K73,K81)</f>
+        <f>SUM(D81,D73,D65,D57,D49,D41,D33,D25,D17,D9,K9,K17,K25,K33,K41,K49,K57,K65,K73,K81,R9)</f>
         <v>217</v>
       </c>
       <c r="E86" s="64">
-        <f>SUM(E81,E73,E65,E57,E49,E41,E33,E25,E17,E9,L9,L17,L25,L33,L41,L49,L57,L65,L73,L81)</f>
+        <f>SUM(E81,E73,E65,E57,E49,E41,E33,E25,E17,E9,L9,L17,L25,L33,L41,L49,L57,L65,L73,L81,S9)</f>
         <v>85</v>
       </c>
       <c r="F86" s="64">
-        <f>SUM(F81,F73,F65,F57,F49,F41,F33,F25,F17,F9,M9,M17,M25,M33,M41,M49,M57,M65,M73,M81)</f>
-        <v>80.5</v>
+        <f>SUM(F81,F73,F65,F57,F49,F41,F33,F25,F17,F9,M9,M17,M25,M33,M41,M49,M57,M65,M73,M81,T9)</f>
+        <v>83.5</v>
       </c>
       <c r="G86" s="25">
         <f>SUM(D86:F86) + 9</f>
-        <v>391.5</v>
+        <v>394.5</v>
       </c>
       <c r="H86" s="66">
         <f>G86/400</f>
-        <v>0.97875000000000001</v>
+        <v>0.98624999999999996</v>
       </c>
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.25">
@@ -6313,7 +6349,7 @@
       <c r="F88" s="64"/>
       <c r="G88" s="22">
         <f>G86*50</f>
-        <v>19575</v>
+        <v>19725</v>
       </c>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.25">
@@ -6325,7 +6361,7 @@
       </c>
       <c r="E90" s="28">
         <f ca="1">G86/(DATEDIF("2020-01-06",TODAY(),"d")/7)</f>
-        <v>19.85869565217391</v>
+        <v>19.725000000000001</v>
       </c>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.25">
@@ -6536,14 +6572,17 @@
       </c>
       <c r="C114" s="7">
         <f>N81</f>
-        <v>25.5</v>
+        <v>27.5</v>
       </c>
     </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B115" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="C115" s="7"/>
+      <c r="C115" s="7">
+        <f>U9</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="116" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B116" s="5" t="s">
@@ -6551,7 +6590,7 @@
       </c>
       <c r="C116" s="29">
         <f ca="1">E90</f>
-        <v>19.85869565217391</v>
+        <v>19.725000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding to Design - Detection
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Desktop\thesisWindows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B5B665-1E22-4A40-A152-7FC3A43670C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5941E78A-22F1-4A0D-B359-1CA085BCFD33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="256">
   <si>
     <t>Date</t>
   </si>
@@ -799,7 +799,7 @@
     <t>20:00-22:00</t>
   </si>
   <si>
-    <t>11:00 - 13:00</t>
+    <t>11:00 - 13:30 15:00 - 17:00 17:30 - 19:00</t>
   </si>
 </sst>
 </file>
@@ -1078,7 +1078,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1309,6 +1309,21 @@
     </xf>
     <xf numFmtId="167" fontId="3" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1650,10 +1665,10 @@
                   <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0">
-                  <c:v>19.725000000000001</c:v>
+                  <c:v>19.975000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2175,18 +2190,18 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="79" t="s">
+      <c r="G1" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
-      <c r="L1" s="79"/>
-      <c r="M1" s="79"/>
-      <c r="N1" s="79"/>
-      <c r="O1" s="79"/>
-      <c r="P1" s="79"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
       <c r="Q1" s="2"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -2529,9 +2544,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T3" sqref="T3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J77" sqref="J77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2550,7 +2565,7 @@
     <col min="14" max="14" width="39.42578125" style="61" customWidth="1"/>
     <col min="15" max="15" width="6.7109375" style="61" customWidth="1"/>
     <col min="16" max="16" width="11.5703125" style="63"/>
-    <col min="17" max="17" width="16.28515625" style="61" customWidth="1"/>
+    <col min="17" max="17" width="16.28515625" style="6" customWidth="1"/>
     <col min="18" max="20" width="11.5703125" style="61"/>
     <col min="21" max="21" width="24.85546875" style="61" customWidth="1"/>
     <col min="22" max="22" width="11.5703125" style="33"/>
@@ -2623,7 +2638,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
         <v>28</v>
       </c>
@@ -2664,15 +2679,17 @@
       <c r="P2" s="68">
         <v>43976</v>
       </c>
-      <c r="Q2" s="69" t="s">
+      <c r="Q2" s="79" t="s">
         <v>255</v>
       </c>
       <c r="R2" s="69"/>
       <c r="S2" s="69"/>
       <c r="T2" s="69">
-        <v>1</v>
-      </c>
-      <c r="U2" s="69"/>
+        <v>6</v>
+      </c>
+      <c r="U2" s="69" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="3" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
@@ -2715,7 +2732,7 @@
       <c r="P3" s="68">
         <v>43977</v>
       </c>
-      <c r="Q3" s="70"/>
+      <c r="Q3" s="80"/>
       <c r="R3" s="70"/>
       <c r="S3" s="70"/>
       <c r="T3" s="69"/>
@@ -2764,7 +2781,7 @@
       <c r="P4" s="68">
         <v>43978</v>
       </c>
-      <c r="Q4" s="69"/>
+      <c r="Q4" s="79"/>
       <c r="R4" s="69"/>
       <c r="S4" s="69"/>
       <c r="T4" s="69"/>
@@ -2811,7 +2828,7 @@
       <c r="P5" s="68">
         <v>43979</v>
       </c>
-      <c r="Q5" s="69"/>
+      <c r="Q5" s="79"/>
       <c r="R5" s="69"/>
       <c r="S5" s="69"/>
       <c r="T5" s="69"/>
@@ -2856,7 +2873,7 @@
       <c r="P6" s="68">
         <v>43980</v>
       </c>
-      <c r="Q6" s="69"/>
+      <c r="Q6" s="79"/>
       <c r="R6" s="69"/>
       <c r="S6" s="69"/>
       <c r="T6" s="69"/>
@@ -2901,7 +2918,7 @@
       <c r="P7" s="68">
         <v>43981</v>
       </c>
-      <c r="Q7" s="69"/>
+      <c r="Q7" s="79"/>
       <c r="R7" s="69"/>
       <c r="S7" s="69"/>
       <c r="T7" s="69"/>
@@ -2940,7 +2957,7 @@
       <c r="P8" s="68">
         <v>43982</v>
       </c>
-      <c r="Q8" s="69"/>
+      <c r="Q8" s="79"/>
       <c r="R8" s="69"/>
       <c r="S8" s="69"/>
       <c r="T8" s="69"/>
@@ -2999,7 +3016,7 @@
       <c r="P9" s="68" t="s">
         <v>55</v>
       </c>
-      <c r="Q9" s="69"/>
+      <c r="Q9" s="79"/>
       <c r="R9" s="69">
         <f>SUM(R2:R8)</f>
         <v>0</v>
@@ -3010,11 +3027,11 @@
       </c>
       <c r="T9" s="69">
         <f>SUM(T2:T8)</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="U9" s="69">
         <f>SUM(R9:T9)</f>
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
@@ -3050,7 +3067,7 @@
       <c r="P10" s="43">
         <v>43983</v>
       </c>
-      <c r="Q10" s="44"/>
+      <c r="Q10" s="81"/>
       <c r="R10" s="44"/>
       <c r="S10" s="44"/>
       <c r="T10" s="45"/>
@@ -3095,7 +3112,7 @@
       <c r="P11" s="43">
         <v>43984</v>
       </c>
-      <c r="Q11" s="46"/>
+      <c r="Q11" s="82"/>
       <c r="R11" s="46"/>
       <c r="S11" s="46"/>
       <c r="T11" s="46"/>
@@ -3140,7 +3157,7 @@
       <c r="P12" s="43">
         <v>43985</v>
       </c>
-      <c r="Q12" s="46"/>
+      <c r="Q12" s="82"/>
       <c r="R12" s="46"/>
       <c r="S12" s="46"/>
       <c r="T12" s="46"/>
@@ -3179,7 +3196,7 @@
       <c r="P13" s="43">
         <v>43986</v>
       </c>
-      <c r="Q13" s="46"/>
+      <c r="Q13" s="82"/>
       <c r="R13" s="46"/>
       <c r="S13" s="46"/>
       <c r="T13" s="46"/>
@@ -3214,7 +3231,7 @@
       <c r="P14" s="43">
         <v>43987</v>
       </c>
-      <c r="Q14" s="46"/>
+      <c r="Q14" s="82"/>
       <c r="R14" s="46"/>
       <c r="S14" s="46"/>
       <c r="T14" s="46"/>
@@ -3255,7 +3272,7 @@
       <c r="P15" s="43">
         <v>43988</v>
       </c>
-      <c r="Q15" s="46"/>
+      <c r="Q15" s="82"/>
       <c r="R15" s="46"/>
       <c r="S15" s="46"/>
       <c r="T15" s="46"/>
@@ -3296,7 +3313,7 @@
       <c r="P16" s="43">
         <v>43989</v>
       </c>
-      <c r="Q16" s="46"/>
+      <c r="Q16" s="82"/>
       <c r="R16" s="46"/>
       <c r="S16" s="46"/>
       <c r="T16" s="46"/>
@@ -3355,7 +3372,7 @@
       <c r="P17" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="Q17" s="5"/>
+      <c r="Q17" s="38"/>
       <c r="R17" s="5"/>
       <c r="S17" s="5"/>
       <c r="T17" s="5"/>
@@ -3394,7 +3411,7 @@
       <c r="P18" s="48">
         <v>43990</v>
       </c>
-      <c r="Q18" s="5"/>
+      <c r="Q18" s="38"/>
       <c r="R18" s="5"/>
       <c r="S18" s="5"/>
       <c r="T18" s="5"/>
@@ -3441,7 +3458,7 @@
       <c r="P19" s="48">
         <v>43991</v>
       </c>
-      <c r="Q19" s="5"/>
+      <c r="Q19" s="38"/>
       <c r="R19" s="5"/>
       <c r="S19" s="5"/>
       <c r="T19" s="5"/>
@@ -3488,7 +3505,7 @@
       <c r="P20" s="48">
         <v>43992</v>
       </c>
-      <c r="Q20" s="5"/>
+      <c r="Q20" s="38"/>
       <c r="R20" s="5"/>
       <c r="S20" s="5"/>
       <c r="T20" s="5"/>
@@ -3535,7 +3552,7 @@
       <c r="P21" s="48">
         <v>43993</v>
       </c>
-      <c r="Q21" s="5"/>
+      <c r="Q21" s="38"/>
       <c r="R21" s="5"/>
       <c r="S21" s="5"/>
       <c r="T21" s="5"/>
@@ -3572,7 +3589,7 @@
       <c r="P22" s="48">
         <v>43994</v>
       </c>
-      <c r="Q22" s="5"/>
+      <c r="Q22" s="38"/>
       <c r="R22" s="5"/>
       <c r="S22" s="5"/>
       <c r="T22" s="5"/>
@@ -3613,7 +3630,7 @@
       <c r="P23" s="48">
         <v>43995</v>
       </c>
-      <c r="Q23" s="5"/>
+      <c r="Q23" s="38"/>
       <c r="R23" s="5"/>
       <c r="S23" s="5"/>
       <c r="T23" s="5"/>
@@ -3654,7 +3671,7 @@
       <c r="P24" s="48">
         <v>43996</v>
       </c>
-      <c r="Q24" s="5"/>
+      <c r="Q24" s="38"/>
       <c r="R24" s="5"/>
       <c r="S24" s="5"/>
       <c r="T24" s="5"/>
@@ -3708,7 +3725,7 @@
         <v>215</v>
       </c>
       <c r="P25" s="48"/>
-      <c r="Q25" s="5"/>
+      <c r="Q25" s="38"/>
       <c r="R25" s="5"/>
       <c r="S25" s="5"/>
       <c r="T25" s="5"/>
@@ -3757,7 +3774,7 @@
       <c r="P26" s="71">
         <v>43997</v>
       </c>
-      <c r="Q26" s="46"/>
+      <c r="Q26" s="82"/>
       <c r="R26" s="46"/>
       <c r="S26" s="46"/>
       <c r="T26" s="46"/>
@@ -3804,7 +3821,7 @@
       <c r="P27" s="71">
         <v>43998</v>
       </c>
-      <c r="Q27" s="46"/>
+      <c r="Q27" s="82"/>
       <c r="R27" s="46"/>
       <c r="S27" s="46"/>
       <c r="T27" s="46"/>
@@ -3847,7 +3864,7 @@
       <c r="P28" s="71">
         <v>43999</v>
       </c>
-      <c r="Q28" s="46"/>
+      <c r="Q28" s="82"/>
       <c r="R28" s="46"/>
       <c r="S28" s="46"/>
       <c r="T28" s="46"/>
@@ -3888,7 +3905,7 @@
       <c r="P29" s="71">
         <v>44000</v>
       </c>
-      <c r="Q29" s="46"/>
+      <c r="Q29" s="82"/>
       <c r="R29" s="46"/>
       <c r="S29" s="46"/>
       <c r="T29" s="46"/>
@@ -3929,7 +3946,7 @@
       <c r="P30" s="71">
         <v>44001</v>
       </c>
-      <c r="Q30" s="46"/>
+      <c r="Q30" s="82"/>
       <c r="R30" s="46"/>
       <c r="S30" s="46"/>
       <c r="T30" s="46"/>
@@ -3970,7 +3987,7 @@
       <c r="P31" s="71">
         <v>44002</v>
       </c>
-      <c r="Q31" s="46"/>
+      <c r="Q31" s="82"/>
       <c r="R31" s="46"/>
       <c r="S31" s="46"/>
       <c r="T31" s="46"/>
@@ -4011,7 +4028,7 @@
       <c r="P32" s="71">
         <v>44003</v>
       </c>
-      <c r="Q32" s="46"/>
+      <c r="Q32" s="82"/>
       <c r="R32" s="46"/>
       <c r="S32" s="46"/>
       <c r="T32" s="46"/>
@@ -4069,7 +4086,7 @@
       <c r="P33" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="Q33" s="5"/>
+      <c r="Q33" s="38"/>
       <c r="R33" s="5"/>
       <c r="S33" s="5"/>
       <c r="T33" s="5"/>
@@ -4116,7 +4133,7 @@
       <c r="P34" s="48">
         <v>44004</v>
       </c>
-      <c r="Q34" s="5"/>
+      <c r="Q34" s="38"/>
       <c r="R34" s="5"/>
       <c r="S34" s="5"/>
       <c r="T34" s="5"/>
@@ -4165,7 +4182,7 @@
       <c r="P35" s="48">
         <v>44005</v>
       </c>
-      <c r="Q35" s="5"/>
+      <c r="Q35" s="38"/>
       <c r="R35" s="5"/>
       <c r="S35" s="5"/>
       <c r="T35" s="5"/>
@@ -4212,7 +4229,7 @@
       <c r="P36" s="48">
         <v>44006</v>
       </c>
-      <c r="Q36" s="5"/>
+      <c r="Q36" s="38"/>
       <c r="R36" s="5"/>
       <c r="S36" s="5"/>
       <c r="T36" s="5"/>
@@ -4259,7 +4276,7 @@
       <c r="P37" s="48">
         <v>44007</v>
       </c>
-      <c r="Q37" s="5"/>
+      <c r="Q37" s="38"/>
       <c r="R37" s="5"/>
       <c r="S37" s="5"/>
       <c r="T37" s="5"/>
@@ -4306,7 +4323,7 @@
       <c r="P38" s="48">
         <v>44008</v>
       </c>
-      <c r="Q38" s="5"/>
+      <c r="Q38" s="38"/>
       <c r="R38" s="5"/>
       <c r="S38" s="5"/>
       <c r="T38" s="5"/>
@@ -4353,7 +4370,7 @@
       <c r="P39" s="48">
         <v>44009</v>
       </c>
-      <c r="Q39" s="5"/>
+      <c r="Q39" s="38"/>
       <c r="R39" s="5"/>
       <c r="S39" s="5"/>
       <c r="T39" s="5"/>
@@ -4400,7 +4417,7 @@
       <c r="P40" s="48">
         <v>44010</v>
       </c>
-      <c r="Q40" s="5"/>
+      <c r="Q40" s="38"/>
       <c r="R40" s="5"/>
       <c r="S40" s="5"/>
       <c r="T40" s="5"/>
@@ -4456,7 +4473,7 @@
       <c r="P41" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="Q41" s="5"/>
+      <c r="Q41" s="38"/>
       <c r="R41" s="5"/>
       <c r="S41" s="5"/>
       <c r="T41" s="5"/>
@@ -4501,7 +4518,7 @@
       <c r="P42" s="71">
         <v>44011</v>
       </c>
-      <c r="Q42" s="46"/>
+      <c r="Q42" s="82"/>
       <c r="R42" s="46"/>
       <c r="S42" s="46"/>
       <c r="T42" s="46"/>
@@ -4542,7 +4559,7 @@
       <c r="P43" s="71">
         <v>44012</v>
       </c>
-      <c r="Q43" s="46"/>
+      <c r="Q43" s="82"/>
       <c r="R43" s="46"/>
       <c r="S43" s="46"/>
       <c r="T43" s="46"/>
@@ -4589,7 +4606,7 @@
       <c r="P44" s="71">
         <v>44013</v>
       </c>
-      <c r="Q44" s="46"/>
+      <c r="Q44" s="82"/>
       <c r="R44" s="46"/>
       <c r="S44" s="46"/>
       <c r="T44" s="46"/>
@@ -4636,7 +4653,7 @@
       <c r="P45" s="71">
         <v>44014</v>
       </c>
-      <c r="Q45" s="46"/>
+      <c r="Q45" s="82"/>
       <c r="R45" s="46"/>
       <c r="S45" s="46"/>
       <c r="T45" s="46"/>
@@ -4677,7 +4694,7 @@
       <c r="P46" s="71">
         <v>44015</v>
       </c>
-      <c r="Q46" s="46"/>
+      <c r="Q46" s="82"/>
       <c r="R46" s="46"/>
       <c r="S46" s="46"/>
       <c r="T46" s="46"/>
@@ -4718,7 +4735,7 @@
       <c r="P47" s="71">
         <v>44016</v>
       </c>
-      <c r="Q47" s="46"/>
+      <c r="Q47" s="82"/>
       <c r="R47" s="46"/>
       <c r="S47" s="46"/>
       <c r="T47" s="46"/>
@@ -4765,7 +4782,7 @@
       <c r="P48" s="71">
         <v>44017</v>
       </c>
-      <c r="Q48" s="46"/>
+      <c r="Q48" s="82"/>
       <c r="R48" s="46"/>
       <c r="S48" s="46"/>
       <c r="T48" s="46"/>
@@ -4818,7 +4835,7 @@
       <c r="P49" s="71" t="s">
         <v>55</v>
       </c>
-      <c r="Q49" s="46"/>
+      <c r="Q49" s="82"/>
       <c r="R49" s="46"/>
       <c r="S49" s="46"/>
       <c r="T49" s="46"/>
@@ -4865,7 +4882,7 @@
       <c r="P50" s="48">
         <v>44018</v>
       </c>
-      <c r="Q50" s="5"/>
+      <c r="Q50" s="38"/>
       <c r="R50" s="5"/>
       <c r="S50" s="5"/>
       <c r="T50" s="5"/>
@@ -4912,7 +4929,7 @@
       <c r="P51" s="48">
         <v>44019</v>
       </c>
-      <c r="Q51" s="5"/>
+      <c r="Q51" s="38"/>
       <c r="R51" s="5"/>
       <c r="S51" s="5"/>
       <c r="T51" s="5"/>
@@ -4959,7 +4976,7 @@
       <c r="P52" s="48">
         <v>44020</v>
       </c>
-      <c r="Q52" s="5"/>
+      <c r="Q52" s="38"/>
       <c r="R52" s="5"/>
       <c r="S52" s="5"/>
       <c r="T52" s="5"/>
@@ -5006,7 +5023,7 @@
       <c r="P53" s="48">
         <v>44021</v>
       </c>
-      <c r="Q53" s="5"/>
+      <c r="Q53" s="38"/>
       <c r="R53" s="5"/>
       <c r="S53" s="5"/>
       <c r="T53" s="5"/>
@@ -5053,7 +5070,7 @@
       <c r="P54" s="48">
         <v>44022</v>
       </c>
-      <c r="Q54" s="5"/>
+      <c r="Q54" s="38"/>
       <c r="R54" s="5"/>
       <c r="S54" s="5"/>
       <c r="T54" s="5"/>
@@ -5094,7 +5111,7 @@
       <c r="P55" s="48">
         <v>44023</v>
       </c>
-      <c r="Q55" s="5"/>
+      <c r="Q55" s="38"/>
       <c r="R55" s="5"/>
       <c r="S55" s="5"/>
       <c r="T55" s="5"/>
@@ -5135,7 +5152,7 @@
       <c r="P56" s="48">
         <v>44024</v>
       </c>
-      <c r="Q56" s="5"/>
+      <c r="Q56" s="38"/>
       <c r="R56" s="5"/>
       <c r="S56" s="5"/>
       <c r="T56" s="5"/>
@@ -5191,7 +5208,7 @@
       <c r="P57" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="Q57" s="5"/>
+      <c r="Q57" s="38"/>
       <c r="R57" s="5"/>
       <c r="S57" s="5"/>
       <c r="T57" s="5"/>
@@ -5240,7 +5257,7 @@
       <c r="P58" s="71">
         <v>44025</v>
       </c>
-      <c r="Q58" s="46"/>
+      <c r="Q58" s="82"/>
       <c r="R58" s="46"/>
       <c r="S58" s="46"/>
       <c r="T58" s="46"/>
@@ -5283,7 +5300,7 @@
       <c r="P59" s="71">
         <v>44026</v>
       </c>
-      <c r="Q59" s="46"/>
+      <c r="Q59" s="82"/>
       <c r="R59" s="46"/>
       <c r="S59" s="46"/>
       <c r="T59" s="46"/>
@@ -5330,7 +5347,7 @@
       <c r="P60" s="71">
         <v>44027</v>
       </c>
-      <c r="Q60" s="46"/>
+      <c r="Q60" s="82"/>
       <c r="R60" s="46"/>
       <c r="S60" s="46"/>
       <c r="T60" s="46"/>
@@ -5379,7 +5396,7 @@
       <c r="P61" s="71">
         <v>44028</v>
       </c>
-      <c r="Q61" s="46"/>
+      <c r="Q61" s="82"/>
       <c r="R61" s="46"/>
       <c r="S61" s="46"/>
       <c r="T61" s="46"/>
@@ -5420,7 +5437,7 @@
       <c r="P62" s="71">
         <v>44029</v>
       </c>
-      <c r="Q62" s="46"/>
+      <c r="Q62" s="82"/>
       <c r="R62" s="46"/>
       <c r="S62" s="46"/>
       <c r="T62" s="46"/>
@@ -5461,7 +5478,7 @@
       <c r="P63" s="71">
         <v>44030</v>
       </c>
-      <c r="Q63" s="46"/>
+      <c r="Q63" s="82"/>
       <c r="R63" s="46"/>
       <c r="S63" s="46"/>
       <c r="T63" s="46"/>
@@ -5508,7 +5525,7 @@
       <c r="P64" s="71">
         <v>44031</v>
       </c>
-      <c r="Q64" s="46"/>
+      <c r="Q64" s="82"/>
       <c r="R64" s="46"/>
       <c r="S64" s="46"/>
       <c r="T64" s="46"/>
@@ -5563,7 +5580,7 @@
       </c>
       <c r="O65" s="39"/>
       <c r="P65" s="71"/>
-      <c r="Q65" s="46"/>
+      <c r="Q65" s="82"/>
       <c r="R65" s="46"/>
       <c r="S65" s="46"/>
       <c r="T65" s="46"/>
@@ -5606,7 +5623,7 @@
       </c>
       <c r="O66" s="72"/>
       <c r="P66" s="73"/>
-      <c r="Q66" s="74"/>
+      <c r="Q66" s="83"/>
       <c r="R66" s="74"/>
       <c r="S66" s="74"/>
       <c r="T66" s="74"/>
@@ -5649,7 +5666,7 @@
       </c>
       <c r="O67" s="72"/>
       <c r="P67" s="73"/>
-      <c r="Q67" s="74"/>
+      <c r="Q67" s="83"/>
       <c r="R67" s="74"/>
       <c r="S67" s="74"/>
       <c r="T67" s="74"/>
@@ -5692,7 +5709,7 @@
       </c>
       <c r="O68" s="72"/>
       <c r="P68" s="73"/>
-      <c r="Q68" s="74"/>
+      <c r="Q68" s="83"/>
       <c r="R68" s="74"/>
       <c r="S68" s="74"/>
       <c r="T68" s="74"/>
@@ -5735,7 +5752,7 @@
       </c>
       <c r="O69" s="72"/>
       <c r="P69" s="73"/>
-      <c r="Q69" s="74"/>
+      <c r="Q69" s="83"/>
       <c r="R69" s="74"/>
       <c r="S69" s="74"/>
       <c r="T69" s="74"/>
@@ -5778,7 +5795,7 @@
       </c>
       <c r="O70" s="72"/>
       <c r="P70" s="73"/>
-      <c r="Q70" s="74"/>
+      <c r="Q70" s="83"/>
       <c r="R70" s="74"/>
       <c r="S70" s="74"/>
       <c r="T70" s="74"/>
@@ -5821,7 +5838,7 @@
       </c>
       <c r="O71" s="72"/>
       <c r="P71" s="73"/>
-      <c r="Q71" s="74"/>
+      <c r="Q71" s="83"/>
       <c r="R71" s="74"/>
       <c r="S71" s="74"/>
       <c r="T71" s="74"/>
@@ -5858,7 +5875,7 @@
       <c r="N72" s="38"/>
       <c r="O72" s="72"/>
       <c r="P72" s="73"/>
-      <c r="Q72" s="74"/>
+      <c r="Q72" s="83"/>
       <c r="R72" s="74"/>
       <c r="S72" s="74"/>
       <c r="T72" s="74"/>
@@ -5913,7 +5930,7 @@
       </c>
       <c r="O73" s="75"/>
       <c r="P73" s="73"/>
-      <c r="Q73" s="74"/>
+      <c r="Q73" s="83"/>
       <c r="R73" s="74"/>
       <c r="S73" s="74"/>
       <c r="T73" s="74"/>
@@ -5956,7 +5973,7 @@
       </c>
       <c r="O74" s="72"/>
       <c r="P74" s="73"/>
-      <c r="Q74" s="74"/>
+      <c r="Q74" s="83"/>
       <c r="R74" s="74"/>
       <c r="S74" s="74"/>
       <c r="T74" s="74"/>
@@ -5999,7 +6016,7 @@
       </c>
       <c r="O75" s="72"/>
       <c r="P75" s="73"/>
-      <c r="Q75" s="74"/>
+      <c r="Q75" s="83"/>
       <c r="R75" s="74"/>
       <c r="S75" s="74"/>
       <c r="T75" s="74"/>
@@ -6042,7 +6059,7 @@
       </c>
       <c r="O76" s="72"/>
       <c r="P76" s="73"/>
-      <c r="Q76" s="74"/>
+      <c r="Q76" s="83"/>
       <c r="R76" s="74"/>
       <c r="S76" s="74"/>
       <c r="T76" s="74"/>
@@ -6085,7 +6102,7 @@
       </c>
       <c r="O77" s="72"/>
       <c r="P77" s="73"/>
-      <c r="Q77" s="74"/>
+      <c r="Q77" s="83"/>
       <c r="R77" s="74"/>
       <c r="S77" s="74"/>
       <c r="T77" s="74"/>
@@ -6128,7 +6145,7 @@
       </c>
       <c r="O78" s="72"/>
       <c r="P78" s="73"/>
-      <c r="Q78" s="74"/>
+      <c r="Q78" s="83"/>
       <c r="R78" s="74"/>
       <c r="S78" s="74"/>
       <c r="T78" s="74"/>
@@ -6165,7 +6182,7 @@
       </c>
       <c r="O79" s="72"/>
       <c r="P79" s="73"/>
-      <c r="Q79" s="74"/>
+      <c r="Q79" s="83"/>
       <c r="R79" s="74"/>
       <c r="S79" s="74"/>
       <c r="T79" s="74"/>
@@ -6202,7 +6219,7 @@
       </c>
       <c r="O80" s="72"/>
       <c r="P80" s="73"/>
-      <c r="Q80" s="74"/>
+      <c r="Q80" s="83"/>
       <c r="R80" s="74"/>
       <c r="S80" s="74"/>
       <c r="T80" s="74"/>
@@ -6253,7 +6270,7 @@
       </c>
       <c r="O81" s="74"/>
       <c r="P81" s="73"/>
-      <c r="Q81" s="74"/>
+      <c r="Q81" s="83"/>
       <c r="R81" s="74"/>
       <c r="S81" s="74"/>
       <c r="T81" s="74"/>
@@ -6322,15 +6339,15 @@
       </c>
       <c r="F86" s="64">
         <f>SUM(F81,F73,F65,F57,F49,F41,F33,F25,F17,F9,M9,M17,M25,M33,M41,M49,M57,M65,M73,M81,T9)</f>
-        <v>83.5</v>
+        <v>88.5</v>
       </c>
       <c r="G86" s="25">
         <f>SUM(D86:F86) + 9</f>
-        <v>394.5</v>
+        <v>399.5</v>
       </c>
       <c r="H86" s="66">
         <f>G86/400</f>
-        <v>0.98624999999999996</v>
+        <v>0.99875000000000003</v>
       </c>
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.25">
@@ -6349,7 +6366,7 @@
       <c r="F88" s="64"/>
       <c r="G88" s="22">
         <f>G86*50</f>
-        <v>19725</v>
+        <v>19975</v>
       </c>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.25">
@@ -6361,7 +6378,7 @@
       </c>
       <c r="E90" s="28">
         <f ca="1">G86/(DATEDIF("2020-01-06",TODAY(),"d")/7)</f>
-        <v>19.725000000000001</v>
+        <v>19.975000000000001</v>
       </c>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.25">
@@ -6581,7 +6598,7 @@
       </c>
       <c r="C115" s="7">
         <f>U9</f>
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="116" spans="2:3" x14ac:dyDescent="0.25">
@@ -6590,7 +6607,7 @@
       </c>
       <c r="C116" s="29">
         <f ca="1">E90</f>
-        <v>19.725000000000001</v>
+        <v>19.975000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nearly finished draft of design detection section.
Just need to add figure to tracking, do counting and speed section and finish calibration section.
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Desktop\thesisWindows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5941E78A-22F1-4A0D-B359-1CA085BCFD33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A8C4A0-4841-417E-A1CB-DA002EFCF5ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="257">
   <si>
     <t>Date</t>
   </si>
@@ -799,7 +799,10 @@
     <t>20:00-22:00</t>
   </si>
   <si>
-    <t>11:00 - 13:30 15:00 - 17:00 17:30 - 19:00</t>
+    <t>11:00 - 13:30 15:00 - 17:00 17:30 - 19:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11:00 - 13:00 19:30 - 21:30 </t>
   </si>
 </sst>
 </file>
@@ -1665,10 +1668,10 @@
                   <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>6</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0">
-                  <c:v>19.975000000000001</c:v>
+                  <c:v>20.056737588652481</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2544,9 +2547,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J77" sqref="J77"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N97" sqref="N97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2685,7 +2688,7 @@
       <c r="R2" s="69"/>
       <c r="S2" s="69"/>
       <c r="T2" s="69">
-        <v>6</v>
+        <v>6.5</v>
       </c>
       <c r="U2" s="69" t="s">
         <v>253</v>
@@ -2732,11 +2735,17 @@
       <c r="P3" s="68">
         <v>43977</v>
       </c>
-      <c r="Q3" s="80"/>
+      <c r="Q3" s="80" t="s">
+        <v>256</v>
+      </c>
       <c r="R3" s="70"/>
       <c r="S3" s="70"/>
-      <c r="T3" s="69"/>
-      <c r="U3" s="69"/>
+      <c r="T3" s="69">
+        <v>4</v>
+      </c>
+      <c r="U3" s="69" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="4" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
@@ -3027,11 +3036,11 @@
       </c>
       <c r="T9" s="69">
         <f>SUM(T2:T8)</f>
-        <v>6</v>
+        <v>10.5</v>
       </c>
       <c r="U9" s="69">
         <f>SUM(R9:T9)</f>
-        <v>6</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
@@ -6339,15 +6348,15 @@
       </c>
       <c r="F86" s="64">
         <f>SUM(F81,F73,F65,F57,F49,F41,F33,F25,F17,F9,M9,M17,M25,M33,M41,M49,M57,M65,M73,M81,T9)</f>
-        <v>88.5</v>
+        <v>93</v>
       </c>
       <c r="G86" s="25">
         <f>SUM(D86:F86) + 9</f>
-        <v>399.5</v>
+        <v>404</v>
       </c>
       <c r="H86" s="66">
         <f>G86/400</f>
-        <v>0.99875000000000003</v>
+        <v>1.01</v>
       </c>
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.25">
@@ -6366,7 +6375,7 @@
       <c r="F88" s="64"/>
       <c r="G88" s="22">
         <f>G86*50</f>
-        <v>19975</v>
+        <v>20200</v>
       </c>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.25">
@@ -6378,7 +6387,7 @@
       </c>
       <c r="E90" s="28">
         <f ca="1">G86/(DATEDIF("2020-01-06",TODAY(),"d")/7)</f>
-        <v>19.975000000000001</v>
+        <v>20.056737588652481</v>
       </c>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.25">
@@ -6598,7 +6607,7 @@
       </c>
       <c r="C115" s="7">
         <f>U9</f>
-        <v>6</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="116" spans="2:3" x14ac:dyDescent="0.25">
@@ -6607,7 +6616,7 @@
       </c>
       <c r="C116" s="29">
         <f ca="1">E90</f>
-        <v>19.975000000000001</v>
+        <v>20.056737588652481</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved centroid tracking so that consolidation works.
Will continue with report now and come back later to improve tracking some more. Want to not show centroids that have disappeared.
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Desktop\thesisWindows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A8C4A0-4841-417E-A1CB-DA002EFCF5ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77082B30-BC76-46B9-A6EF-3AA7D6DAF191}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="259">
   <si>
     <t>Date</t>
   </si>
@@ -802,7 +802,13 @@
     <t>11:00 - 13:30 15:00 - 17:00 17:30 - 19:30</t>
   </si>
   <si>
-    <t xml:space="preserve">11:00 - 13:00 19:30 - 21:30 </t>
+    <t>11:00 - 13:00 19:30 - 21:30 22:00 - 01:00</t>
+  </si>
+  <si>
+    <t>12:00 - 14:00</t>
+  </si>
+  <si>
+    <t>Improving Tracker</t>
   </si>
 </sst>
 </file>
@@ -1668,10 +1674,10 @@
                   <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>10.5</c:v>
+                  <c:v>16.5</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0">
-                  <c:v>20.056737588652481</c:v>
+                  <c:v>20.211267605633804</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2547,9 +2553,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N97" sqref="N97"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2694,7 +2700,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
         <v>32</v>
       </c>
@@ -2741,7 +2747,7 @@
       <c r="R3" s="70"/>
       <c r="S3" s="70"/>
       <c r="T3" s="69">
-        <v>4</v>
+        <v>7.5</v>
       </c>
       <c r="U3" s="69" t="s">
         <v>253</v>
@@ -2790,11 +2796,17 @@
       <c r="P4" s="68">
         <v>43978</v>
       </c>
-      <c r="Q4" s="79"/>
-      <c r="R4" s="69"/>
+      <c r="Q4" s="79" t="s">
+        <v>257</v>
+      </c>
+      <c r="R4" s="69">
+        <v>2.5</v>
+      </c>
       <c r="S4" s="69"/>
       <c r="T4" s="69"/>
-      <c r="U4" s="69"/>
+      <c r="U4" s="69" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="35" t="s">
@@ -3028,7 +3040,7 @@
       <c r="Q9" s="79"/>
       <c r="R9" s="69">
         <f>SUM(R2:R8)</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="S9" s="69">
         <f>SUM(S2:S8)</f>
@@ -3036,11 +3048,11 @@
       </c>
       <c r="T9" s="69">
         <f>SUM(T2:T8)</f>
-        <v>10.5</v>
+        <v>14</v>
       </c>
       <c r="U9" s="69">
         <f>SUM(R9:T9)</f>
-        <v>10.5</v>
+        <v>16.5</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
@@ -6340,7 +6352,7 @@
       </c>
       <c r="D86" s="64">
         <f>SUM(D81,D73,D65,D57,D49,D41,D33,D25,D17,D9,K9,K17,K25,K33,K41,K49,K57,K65,K73,K81,R9)</f>
-        <v>217</v>
+        <v>219.5</v>
       </c>
       <c r="E86" s="64">
         <f>SUM(E81,E73,E65,E57,E49,E41,E33,E25,E17,E9,L9,L17,L25,L33,L41,L49,L57,L65,L73,L81,S9)</f>
@@ -6348,15 +6360,15 @@
       </c>
       <c r="F86" s="64">
         <f>SUM(F81,F73,F65,F57,F49,F41,F33,F25,F17,F9,M9,M17,M25,M33,M41,M49,M57,M65,M73,M81,T9)</f>
-        <v>93</v>
+        <v>96.5</v>
       </c>
       <c r="G86" s="25">
         <f>SUM(D86:F86) + 9</f>
-        <v>404</v>
+        <v>410</v>
       </c>
       <c r="H86" s="66">
         <f>G86/400</f>
-        <v>1.01</v>
+        <v>1.0249999999999999</v>
       </c>
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.25">
@@ -6375,7 +6387,7 @@
       <c r="F88" s="64"/>
       <c r="G88" s="22">
         <f>G86*50</f>
-        <v>20200</v>
+        <v>20500</v>
       </c>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.25">
@@ -6387,7 +6399,7 @@
       </c>
       <c r="E90" s="28">
         <f ca="1">G86/(DATEDIF("2020-01-06",TODAY(),"d")/7)</f>
-        <v>20.056737588652481</v>
+        <v>20.211267605633804</v>
       </c>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.25">
@@ -6607,7 +6619,7 @@
       </c>
       <c r="C115" s="7">
         <f>U9</f>
-        <v>10.5</v>
+        <v>16.5</v>
       </c>
     </row>
     <row r="116" spans="2:3" x14ac:dyDescent="0.25">
@@ -6616,7 +6628,7 @@
       </c>
       <c r="C116" s="29">
         <f ca="1">E90</f>
-        <v>20.056737588652481</v>
+        <v>20.211267605633804</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished draft of Design Detection section aside from calibration.
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Desktop\thesisWindows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77082B30-BC76-46B9-A6EF-3AA7D6DAF191}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84BDAFA4-BA8C-4ACD-B534-F457F66A8DD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -805,10 +805,10 @@
     <t>11:00 - 13:00 19:30 - 21:30 22:00 - 01:00</t>
   </si>
   <si>
-    <t>12:00 - 14:00</t>
-  </si>
-  <si>
-    <t>Improving Tracker</t>
+    <t>Improving Tracker + Report: Design</t>
+  </si>
+  <si>
+    <t>12:00 - 14:00 18:00 - 20:00 22:00 - 23:00</t>
   </si>
 </sst>
 </file>
@@ -1674,10 +1674,10 @@
                   <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>16.5</c:v>
+                  <c:v>19.5</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0">
-                  <c:v>20.211267605633804</c:v>
+                  <c:v>20.359154929577464</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2555,7 +2555,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R5" sqref="R5"/>
+      <selection pane="bottomLeft" activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2576,7 +2576,7 @@
     <col min="16" max="16" width="11.5703125" style="63"/>
     <col min="17" max="17" width="16.28515625" style="6" customWidth="1"/>
     <col min="18" max="20" width="11.5703125" style="61"/>
-    <col min="21" max="21" width="24.85546875" style="61" customWidth="1"/>
+    <col min="21" max="21" width="24.85546875" style="6" customWidth="1"/>
     <col min="22" max="22" width="11.5703125" style="33"/>
     <col min="23" max="1025" width="11.5703125" style="34"/>
     <col min="1026" max="16384" width="9.140625" style="2"/>
@@ -2696,7 +2696,7 @@
       <c r="T2" s="69">
         <v>6.5</v>
       </c>
-      <c r="U2" s="69" t="s">
+      <c r="U2" s="79" t="s">
         <v>253</v>
       </c>
     </row>
@@ -2749,7 +2749,7 @@
       <c r="T3" s="69">
         <v>7.5</v>
       </c>
-      <c r="U3" s="69" t="s">
+      <c r="U3" s="79" t="s">
         <v>253</v>
       </c>
     </row>
@@ -2797,15 +2797,17 @@
         <v>43978</v>
       </c>
       <c r="Q4" s="79" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="R4" s="69">
         <v>2.5</v>
       </c>
       <c r="S4" s="69"/>
-      <c r="T4" s="69"/>
-      <c r="U4" s="69" t="s">
-        <v>258</v>
+      <c r="T4" s="69">
+        <v>3</v>
+      </c>
+      <c r="U4" s="79" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
@@ -2853,7 +2855,7 @@
       <c r="R5" s="69"/>
       <c r="S5" s="69"/>
       <c r="T5" s="69"/>
-      <c r="U5" s="69"/>
+      <c r="U5" s="79"/>
     </row>
     <row r="6" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="35" t="s">
@@ -2898,7 +2900,7 @@
       <c r="R6" s="69"/>
       <c r="S6" s="69"/>
       <c r="T6" s="69"/>
-      <c r="U6" s="69"/>
+      <c r="U6" s="79"/>
     </row>
     <row r="7" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="35" t="s">
@@ -2943,7 +2945,7 @@
       <c r="R7" s="69"/>
       <c r="S7" s="69"/>
       <c r="T7" s="69"/>
-      <c r="U7" s="69"/>
+      <c r="U7" s="79"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="35" t="s">
@@ -2982,7 +2984,7 @@
       <c r="R8" s="69"/>
       <c r="S8" s="69"/>
       <c r="T8" s="69"/>
-      <c r="U8" s="69"/>
+      <c r="U8" s="79"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="39" t="s">
@@ -3048,11 +3050,11 @@
       </c>
       <c r="T9" s="69">
         <f>SUM(T2:T8)</f>
-        <v>14</v>
-      </c>
-      <c r="U9" s="69">
+        <v>17</v>
+      </c>
+      <c r="U9" s="79">
         <f>SUM(R9:T9)</f>
-        <v>16.5</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
@@ -3092,7 +3094,7 @@
       <c r="R10" s="44"/>
       <c r="S10" s="44"/>
       <c r="T10" s="45"/>
-      <c r="U10" s="44"/>
+      <c r="U10" s="81"/>
     </row>
     <row r="11" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="35" t="s">
@@ -3137,7 +3139,7 @@
       <c r="R11" s="46"/>
       <c r="S11" s="46"/>
       <c r="T11" s="46"/>
-      <c r="U11" s="46"/>
+      <c r="U11" s="82"/>
     </row>
     <row r="12" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="35" t="s">
@@ -3182,7 +3184,7 @@
       <c r="R12" s="46"/>
       <c r="S12" s="46"/>
       <c r="T12" s="46"/>
-      <c r="U12" s="46"/>
+      <c r="U12" s="82"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="35" t="s">
@@ -3221,7 +3223,7 @@
       <c r="R13" s="46"/>
       <c r="S13" s="46"/>
       <c r="T13" s="46"/>
-      <c r="U13" s="46"/>
+      <c r="U13" s="82"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="35" t="s">
@@ -3256,7 +3258,7 @@
       <c r="R14" s="46"/>
       <c r="S14" s="46"/>
       <c r="T14" s="46"/>
-      <c r="U14" s="46"/>
+      <c r="U14" s="82"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="35" t="s">
@@ -3297,7 +3299,7 @@
       <c r="R15" s="46"/>
       <c r="S15" s="46"/>
       <c r="T15" s="46"/>
-      <c r="U15" s="46"/>
+      <c r="U15" s="82"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="35" t="s">
@@ -3338,7 +3340,7 @@
       <c r="R16" s="46"/>
       <c r="S16" s="46"/>
       <c r="T16" s="46"/>
-      <c r="U16" s="46"/>
+      <c r="U16" s="82"/>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="39" t="s">
@@ -3397,7 +3399,7 @@
       <c r="R17" s="5"/>
       <c r="S17" s="5"/>
       <c r="T17" s="5"/>
-      <c r="U17" s="5"/>
+      <c r="U17" s="38"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="35" t="s">
@@ -3436,7 +3438,7 @@
       <c r="R18" s="5"/>
       <c r="S18" s="5"/>
       <c r="T18" s="5"/>
-      <c r="U18" s="5"/>
+      <c r="U18" s="38"/>
     </row>
     <row r="19" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="35" t="s">
@@ -3483,7 +3485,7 @@
       <c r="R19" s="5"/>
       <c r="S19" s="5"/>
       <c r="T19" s="5"/>
-      <c r="U19" s="5"/>
+      <c r="U19" s="38"/>
     </row>
     <row r="20" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="35" t="s">
@@ -3530,7 +3532,7 @@
       <c r="R20" s="5"/>
       <c r="S20" s="5"/>
       <c r="T20" s="5"/>
-      <c r="U20" s="5"/>
+      <c r="U20" s="38"/>
     </row>
     <row r="21" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="35" t="s">
@@ -3577,7 +3579,7 @@
       <c r="R21" s="5"/>
       <c r="S21" s="5"/>
       <c r="T21" s="5"/>
-      <c r="U21" s="5"/>
+      <c r="U21" s="38"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="35" t="s">
@@ -3614,7 +3616,7 @@
       <c r="R22" s="5"/>
       <c r="S22" s="5"/>
       <c r="T22" s="5"/>
-      <c r="U22" s="5"/>
+      <c r="U22" s="38"/>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="35" t="s">
@@ -3655,7 +3657,7 @@
       <c r="R23" s="5"/>
       <c r="S23" s="5"/>
       <c r="T23" s="5"/>
-      <c r="U23" s="5"/>
+      <c r="U23" s="38"/>
     </row>
     <row r="24" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="35" t="s">
@@ -3696,7 +3698,7 @@
       <c r="R24" s="5"/>
       <c r="S24" s="5"/>
       <c r="T24" s="5"/>
-      <c r="U24" s="5"/>
+      <c r="U24" s="38"/>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="39" t="s">
@@ -3750,7 +3752,7 @@
       <c r="R25" s="5"/>
       <c r="S25" s="5"/>
       <c r="T25" s="5"/>
-      <c r="U25" s="5"/>
+      <c r="U25" s="38"/>
     </row>
     <row r="26" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="35" t="s">
@@ -3799,7 +3801,7 @@
       <c r="R26" s="46"/>
       <c r="S26" s="46"/>
       <c r="T26" s="46"/>
-      <c r="U26" s="46"/>
+      <c r="U26" s="82"/>
     </row>
     <row r="27" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="35" t="s">
@@ -3846,7 +3848,7 @@
       <c r="R27" s="46"/>
       <c r="S27" s="46"/>
       <c r="T27" s="46"/>
-      <c r="U27" s="46"/>
+      <c r="U27" s="82"/>
     </row>
     <row r="28" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" s="35" t="s">
@@ -3889,7 +3891,7 @@
       <c r="R28" s="46"/>
       <c r="S28" s="46"/>
       <c r="T28" s="46"/>
-      <c r="U28" s="46"/>
+      <c r="U28" s="82"/>
     </row>
     <row r="29" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="35" t="s">
@@ -3930,7 +3932,7 @@
       <c r="R29" s="46"/>
       <c r="S29" s="46"/>
       <c r="T29" s="46"/>
-      <c r="U29" s="46"/>
+      <c r="U29" s="82"/>
     </row>
     <row r="30" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="35" t="s">
@@ -3971,7 +3973,7 @@
       <c r="R30" s="46"/>
       <c r="S30" s="46"/>
       <c r="T30" s="46"/>
-      <c r="U30" s="46"/>
+      <c r="U30" s="82"/>
     </row>
     <row r="31" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="35" t="s">
@@ -4012,7 +4014,7 @@
       <c r="R31" s="46"/>
       <c r="S31" s="46"/>
       <c r="T31" s="46"/>
-      <c r="U31" s="46"/>
+      <c r="U31" s="82"/>
     </row>
     <row r="32" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="35" t="s">
@@ -4053,7 +4055,7 @@
       <c r="R32" s="46"/>
       <c r="S32" s="46"/>
       <c r="T32" s="46"/>
-      <c r="U32" s="46"/>
+      <c r="U32" s="82"/>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="39" t="s">
@@ -4111,7 +4113,7 @@
       <c r="R33" s="5"/>
       <c r="S33" s="5"/>
       <c r="T33" s="5"/>
-      <c r="U33" s="5"/>
+      <c r="U33" s="38"/>
     </row>
     <row r="34" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="35" t="s">
@@ -4158,7 +4160,7 @@
       <c r="R34" s="5"/>
       <c r="S34" s="5"/>
       <c r="T34" s="5"/>
-      <c r="U34" s="5"/>
+      <c r="U34" s="38"/>
     </row>
     <row r="35" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="35" t="s">
@@ -4207,7 +4209,7 @@
       <c r="R35" s="5"/>
       <c r="S35" s="5"/>
       <c r="T35" s="5"/>
-      <c r="U35" s="5"/>
+      <c r="U35" s="38"/>
     </row>
     <row r="36" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="35" t="s">
@@ -4254,7 +4256,7 @@
       <c r="R36" s="5"/>
       <c r="S36" s="5"/>
       <c r="T36" s="5"/>
-      <c r="U36" s="5"/>
+      <c r="U36" s="38"/>
     </row>
     <row r="37" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="35" t="s">
@@ -4301,7 +4303,7 @@
       <c r="R37" s="5"/>
       <c r="S37" s="5"/>
       <c r="T37" s="5"/>
-      <c r="U37" s="5"/>
+      <c r="U37" s="38"/>
     </row>
     <row r="38" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="35" t="s">
@@ -4348,7 +4350,7 @@
       <c r="R38" s="5"/>
       <c r="S38" s="5"/>
       <c r="T38" s="5"/>
-      <c r="U38" s="5"/>
+      <c r="U38" s="38"/>
     </row>
     <row r="39" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="35" t="s">
@@ -4395,7 +4397,7 @@
       <c r="R39" s="5"/>
       <c r="S39" s="5"/>
       <c r="T39" s="5"/>
-      <c r="U39" s="5"/>
+      <c r="U39" s="38"/>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" s="35" t="s">
@@ -4442,7 +4444,7 @@
       <c r="R40" s="5"/>
       <c r="S40" s="5"/>
       <c r="T40" s="5"/>
-      <c r="U40" s="5"/>
+      <c r="U40" s="38"/>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" s="39" t="s">
@@ -4498,7 +4500,7 @@
       <c r="R41" s="5"/>
       <c r="S41" s="5"/>
       <c r="T41" s="5"/>
-      <c r="U41" s="5"/>
+      <c r="U41" s="38"/>
     </row>
     <row r="42" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="35" t="s">
@@ -4543,7 +4545,7 @@
       <c r="R42" s="46"/>
       <c r="S42" s="46"/>
       <c r="T42" s="46"/>
-      <c r="U42" s="46"/>
+      <c r="U42" s="82"/>
     </row>
     <row r="43" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="35" t="s">
@@ -4584,7 +4586,7 @@
       <c r="R43" s="46"/>
       <c r="S43" s="46"/>
       <c r="T43" s="46"/>
-      <c r="U43" s="46"/>
+      <c r="U43" s="82"/>
     </row>
     <row r="44" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="35" t="s">
@@ -4631,7 +4633,7 @@
       <c r="R44" s="46"/>
       <c r="S44" s="46"/>
       <c r="T44" s="46"/>
-      <c r="U44" s="46"/>
+      <c r="U44" s="82"/>
     </row>
     <row r="45" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="35" t="s">
@@ -4678,7 +4680,7 @@
       <c r="R45" s="46"/>
       <c r="S45" s="46"/>
       <c r="T45" s="46"/>
-      <c r="U45" s="46"/>
+      <c r="U45" s="82"/>
     </row>
     <row r="46" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A46" s="35" t="s">
@@ -4719,7 +4721,7 @@
       <c r="R46" s="46"/>
       <c r="S46" s="46"/>
       <c r="T46" s="46"/>
-      <c r="U46" s="46"/>
+      <c r="U46" s="82"/>
     </row>
     <row r="47" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="35" t="s">
@@ -4760,7 +4762,7 @@
       <c r="R47" s="46"/>
       <c r="S47" s="46"/>
       <c r="T47" s="46"/>
-      <c r="U47" s="46"/>
+      <c r="U47" s="82"/>
     </row>
     <row r="48" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="35" t="s">
@@ -4807,7 +4809,7 @@
       <c r="R48" s="46"/>
       <c r="S48" s="46"/>
       <c r="T48" s="46"/>
-      <c r="U48" s="46"/>
+      <c r="U48" s="82"/>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" s="39" t="s">
@@ -4860,7 +4862,7 @@
       <c r="R49" s="46"/>
       <c r="S49" s="46"/>
       <c r="T49" s="46"/>
-      <c r="U49" s="46"/>
+      <c r="U49" s="82"/>
     </row>
     <row r="50" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="35" t="s">
@@ -4907,7 +4909,7 @@
       <c r="R50" s="5"/>
       <c r="S50" s="5"/>
       <c r="T50" s="5"/>
-      <c r="U50" s="5"/>
+      <c r="U50" s="38"/>
     </row>
     <row r="51" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="35" t="s">
@@ -4954,7 +4956,7 @@
       <c r="R51" s="5"/>
       <c r="S51" s="5"/>
       <c r="T51" s="5"/>
-      <c r="U51" s="5"/>
+      <c r="U51" s="38"/>
     </row>
     <row r="52" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="35" t="s">
@@ -5001,7 +5003,7 @@
       <c r="R52" s="5"/>
       <c r="S52" s="5"/>
       <c r="T52" s="5"/>
-      <c r="U52" s="5"/>
+      <c r="U52" s="38"/>
     </row>
     <row r="53" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="35" t="s">
@@ -5048,7 +5050,7 @@
       <c r="R53" s="5"/>
       <c r="S53" s="5"/>
       <c r="T53" s="5"/>
-      <c r="U53" s="5"/>
+      <c r="U53" s="38"/>
     </row>
     <row r="54" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="35" t="s">
@@ -5095,7 +5097,7 @@
       <c r="R54" s="5"/>
       <c r="S54" s="5"/>
       <c r="T54" s="5"/>
-      <c r="U54" s="5"/>
+      <c r="U54" s="38"/>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55" s="35" t="s">
@@ -5136,7 +5138,7 @@
       <c r="R55" s="5"/>
       <c r="S55" s="5"/>
       <c r="T55" s="5"/>
-      <c r="U55" s="5"/>
+      <c r="U55" s="38"/>
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A56" s="35" t="s">
@@ -5177,7 +5179,7 @@
       <c r="R56" s="5"/>
       <c r="S56" s="5"/>
       <c r="T56" s="5"/>
-      <c r="U56" s="5"/>
+      <c r="U56" s="38"/>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A57" s="39" t="s">
@@ -5233,7 +5235,7 @@
       <c r="R57" s="5"/>
       <c r="S57" s="5"/>
       <c r="T57" s="5"/>
-      <c r="U57" s="5"/>
+      <c r="U57" s="38"/>
     </row>
     <row r="58" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A58" s="35" t="s">
@@ -5282,7 +5284,7 @@
       <c r="R58" s="46"/>
       <c r="S58" s="46"/>
       <c r="T58" s="46"/>
-      <c r="U58" s="46"/>
+      <c r="U58" s="82"/>
     </row>
     <row r="59" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" s="35" t="s">
@@ -5325,7 +5327,7 @@
       <c r="R59" s="46"/>
       <c r="S59" s="46"/>
       <c r="T59" s="46"/>
-      <c r="U59" s="46"/>
+      <c r="U59" s="82"/>
     </row>
     <row r="60" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="35" t="s">
@@ -5372,7 +5374,7 @@
       <c r="R60" s="46"/>
       <c r="S60" s="46"/>
       <c r="T60" s="46"/>
-      <c r="U60" s="46"/>
+      <c r="U60" s="82"/>
     </row>
     <row r="61" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="35" t="s">
@@ -5421,7 +5423,7 @@
       <c r="R61" s="46"/>
       <c r="S61" s="46"/>
       <c r="T61" s="46"/>
-      <c r="U61" s="46"/>
+      <c r="U61" s="82"/>
     </row>
     <row r="62" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="35" t="s">
@@ -5462,7 +5464,7 @@
       <c r="R62" s="46"/>
       <c r="S62" s="46"/>
       <c r="T62" s="46"/>
-      <c r="U62" s="46"/>
+      <c r="U62" s="82"/>
     </row>
     <row r="63" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A63" s="35" t="s">
@@ -5503,7 +5505,7 @@
       <c r="R63" s="46"/>
       <c r="S63" s="46"/>
       <c r="T63" s="46"/>
-      <c r="U63" s="46"/>
+      <c r="U63" s="82"/>
     </row>
     <row r="64" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="35" t="s">
@@ -5550,7 +5552,7 @@
       <c r="R64" s="46"/>
       <c r="S64" s="46"/>
       <c r="T64" s="46"/>
-      <c r="U64" s="46"/>
+      <c r="U64" s="82"/>
     </row>
     <row r="65" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A65" s="39" t="s">
@@ -5605,7 +5607,7 @@
       <c r="R65" s="46"/>
       <c r="S65" s="46"/>
       <c r="T65" s="46"/>
-      <c r="U65" s="46"/>
+      <c r="U65" s="82"/>
     </row>
     <row r="66" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A66" s="35" t="s">
@@ -5648,7 +5650,7 @@
       <c r="R66" s="74"/>
       <c r="S66" s="74"/>
       <c r="T66" s="74"/>
-      <c r="U66" s="74"/>
+      <c r="U66" s="83"/>
     </row>
     <row r="67" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" s="35" t="s">
@@ -5691,7 +5693,7 @@
       <c r="R67" s="74"/>
       <c r="S67" s="74"/>
       <c r="T67" s="74"/>
-      <c r="U67" s="74"/>
+      <c r="U67" s="83"/>
     </row>
     <row r="68" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="35" t="s">
@@ -5734,7 +5736,7 @@
       <c r="R68" s="74"/>
       <c r="S68" s="74"/>
       <c r="T68" s="74"/>
-      <c r="U68" s="74"/>
+      <c r="U68" s="83"/>
     </row>
     <row r="69" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" s="35" t="s">
@@ -5777,7 +5779,7 @@
       <c r="R69" s="74"/>
       <c r="S69" s="74"/>
       <c r="T69" s="74"/>
-      <c r="U69" s="74"/>
+      <c r="U69" s="83"/>
     </row>
     <row r="70" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="35" t="s">
@@ -5820,7 +5822,7 @@
       <c r="R70" s="74"/>
       <c r="S70" s="74"/>
       <c r="T70" s="74"/>
-      <c r="U70" s="74"/>
+      <c r="U70" s="83"/>
     </row>
     <row r="71" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A71" s="35" t="s">
@@ -5863,7 +5865,7 @@
       <c r="R71" s="74"/>
       <c r="S71" s="74"/>
       <c r="T71" s="74"/>
-      <c r="U71" s="74"/>
+      <c r="U71" s="83"/>
     </row>
     <row r="72" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="35" t="s">
@@ -5900,7 +5902,7 @@
       <c r="R72" s="74"/>
       <c r="S72" s="74"/>
       <c r="T72" s="74"/>
-      <c r="U72" s="74"/>
+      <c r="U72" s="83"/>
     </row>
     <row r="73" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A73" s="39" t="s">
@@ -5955,7 +5957,7 @@
       <c r="R73" s="74"/>
       <c r="S73" s="74"/>
       <c r="T73" s="74"/>
-      <c r="U73" s="74"/>
+      <c r="U73" s="83"/>
     </row>
     <row r="74" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A74" s="35" t="s">
@@ -5998,7 +6000,7 @@
       <c r="R74" s="74"/>
       <c r="S74" s="74"/>
       <c r="T74" s="74"/>
-      <c r="U74" s="74"/>
+      <c r="U74" s="83"/>
     </row>
     <row r="75" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="35" t="s">
@@ -6041,7 +6043,7 @@
       <c r="R75" s="74"/>
       <c r="S75" s="74"/>
       <c r="T75" s="74"/>
-      <c r="U75" s="74"/>
+      <c r="U75" s="83"/>
     </row>
     <row r="76" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="35" t="s">
@@ -6084,7 +6086,7 @@
       <c r="R76" s="74"/>
       <c r="S76" s="74"/>
       <c r="T76" s="74"/>
-      <c r="U76" s="74"/>
+      <c r="U76" s="83"/>
     </row>
     <row r="77" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A77" s="35" t="s">
@@ -6127,7 +6129,7 @@
       <c r="R77" s="74"/>
       <c r="S77" s="74"/>
       <c r="T77" s="74"/>
-      <c r="U77" s="74"/>
+      <c r="U77" s="83"/>
     </row>
     <row r="78" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A78" s="35" t="s">
@@ -6170,7 +6172,7 @@
       <c r="R78" s="74"/>
       <c r="S78" s="74"/>
       <c r="T78" s="74"/>
-      <c r="U78" s="74"/>
+      <c r="U78" s="83"/>
     </row>
     <row r="79" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A79" s="35" t="s">
@@ -6207,7 +6209,7 @@
       <c r="R79" s="74"/>
       <c r="S79" s="74"/>
       <c r="T79" s="74"/>
-      <c r="U79" s="74"/>
+      <c r="U79" s="83"/>
     </row>
     <row r="80" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A80" s="35" t="s">
@@ -6244,7 +6246,7 @@
       <c r="R80" s="74"/>
       <c r="S80" s="74"/>
       <c r="T80" s="74"/>
-      <c r="U80" s="74"/>
+      <c r="U80" s="83"/>
     </row>
     <row r="81" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A81" s="58"/>
@@ -6295,7 +6297,7 @@
       <c r="R81" s="74"/>
       <c r="S81" s="74"/>
       <c r="T81" s="74"/>
-      <c r="U81" s="74"/>
+      <c r="U81" s="83"/>
     </row>
     <row r="82" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A82" s="59"/>
@@ -6360,15 +6362,15 @@
       </c>
       <c r="F86" s="64">
         <f>SUM(F81,F73,F65,F57,F49,F41,F33,F25,F17,F9,M9,M17,M25,M33,M41,M49,M57,M65,M73,M81,T9)</f>
-        <v>96.5</v>
+        <v>99.5</v>
       </c>
       <c r="G86" s="25">
         <f>SUM(D86:F86) + 9</f>
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="H86" s="66">
         <f>G86/400</f>
-        <v>1.0249999999999999</v>
+        <v>1.0325</v>
       </c>
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.25">
@@ -6387,7 +6389,7 @@
       <c r="F88" s="64"/>
       <c r="G88" s="22">
         <f>G86*50</f>
-        <v>20500</v>
+        <v>20650</v>
       </c>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.25">
@@ -6399,7 +6401,7 @@
       </c>
       <c r="E90" s="28">
         <f ca="1">G86/(DATEDIF("2020-01-06",TODAY(),"d")/7)</f>
-        <v>20.211267605633804</v>
+        <v>20.359154929577464</v>
       </c>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.25">
@@ -6619,7 +6621,7 @@
       </c>
       <c r="C115" s="7">
         <f>U9</f>
-        <v>16.5</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="116" spans="2:3" x14ac:dyDescent="0.25">
@@ -6628,7 +6630,7 @@
       </c>
       <c r="C116" s="29">
         <f ca="1">E90</f>
-        <v>20.211267605633804</v>
+        <v>20.359154929577464</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Design raw draft complete.
Need to read over, improve and add to. Thereafter, large sections to complete are only results and conclusion.
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Desktop\thesisWindows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92EC5C3-E882-4C07-9538-1CFE2CBD9AA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF3E3081-9627-4D0C-B5F8-B99AC025FDC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="263">
   <si>
     <t>Date</t>
   </si>
@@ -812,6 +812,15 @@
   </si>
   <si>
     <t>Report: Design/Calibration</t>
+  </si>
+  <si>
+    <t>19:00 - 21:30</t>
+  </si>
+  <si>
+    <t>11:00 - 13:00 15:30 - 17:30 20:30 - 21:30 22:00 - 23:00</t>
+  </si>
+  <si>
+    <t>10:30 - 13:00 14:30 - 15:30</t>
   </si>
 </sst>
 </file>
@@ -1474,12 +1483,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1300" b="0" strike="noStrike" spc="-1">
+              <a:defRPr sz="1300" b="1" strike="noStrike" spc="-1">
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1300" b="0" strike="noStrike" spc="-1">
+              <a:rPr lang="en-US" sz="1300" b="1" strike="noStrike" spc="-1">
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>Weekly Totals</a:t>
@@ -1538,9 +1547,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$B$95:$B$116</c:f>
+              <c:f>Sheet2!$B$95:$B$120</c:f>
               <c:strCache>
-                <c:ptCount val="22"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>Wk1</c:v>
                 </c:pt>
@@ -1605,6 +1614,18 @@
                   <c:v>Wk21</c:v>
                 </c:pt>
                 <c:pt idx="21">
+                  <c:v>Wk22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Wk23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Wk24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Wk25</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>Average</c:v>
                 </c:pt>
               </c:strCache>
@@ -1612,10 +1633,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$C$95:$C$116</c:f>
+              <c:f>Sheet2!$C$95:$C$120</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>18.5</c:v>
                 </c:pt>
@@ -1677,10 +1698,22 @@
                   <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>22.5</c:v>
+                  <c:v>29.5</c:v>
                 </c:pt>
-                <c:pt idx="21" formatCode="0">
-                  <c:v>20.363636363636367</c:v>
+                <c:pt idx="21" formatCode="General">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25" formatCode="0">
+                  <c:v>20.30952380952381</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1844,16 +1877,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>468076</xdr:colOff>
-      <xdr:row>87</xdr:row>
-      <xdr:rowOff>79174</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>658575</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>56762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>623429</xdr:colOff>
-      <xdr:row>111</xdr:row>
-      <xdr:rowOff>78454</xdr:rowOff>
+      <xdr:colOff>493058</xdr:colOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>33618</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2554,11 +2587,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AMK116"/>
+  <dimension ref="A1:AMK120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S5" sqref="S5"/>
+      <selection pane="bottomLeft" activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2855,7 +2888,7 @@
         <v>43979</v>
       </c>
       <c r="Q5" s="79" t="s">
-        <v>194</v>
+        <v>260</v>
       </c>
       <c r="R5" s="69"/>
       <c r="S5" s="69"/>
@@ -2866,7 +2899,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="35" t="s">
         <v>44</v>
       </c>
@@ -2905,11 +2938,17 @@
       <c r="P6" s="68">
         <v>43980</v>
       </c>
-      <c r="Q6" s="79"/>
+      <c r="Q6" s="79" t="s">
+        <v>261</v>
+      </c>
       <c r="R6" s="69"/>
       <c r="S6" s="69"/>
-      <c r="T6" s="69"/>
-      <c r="U6" s="79"/>
+      <c r="T6" s="69">
+        <v>5</v>
+      </c>
+      <c r="U6" s="79" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="7" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="35" t="s">
@@ -2953,7 +2992,9 @@
       <c r="Q7" s="79"/>
       <c r="R7" s="69"/>
       <c r="S7" s="69"/>
-      <c r="T7" s="69"/>
+      <c r="T7" s="69">
+        <v>2</v>
+      </c>
       <c r="U7" s="79"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
@@ -3059,14 +3100,14 @@
       </c>
       <c r="T9" s="69">
         <f>SUM(T2:T8)</f>
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="U9" s="79">
         <f>SUM(R9:T9)</f>
-        <v>22.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+        <v>29.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="35" t="s">
         <v>28</v>
       </c>
@@ -3099,11 +3140,17 @@
       <c r="P10" s="43">
         <v>43983</v>
       </c>
-      <c r="Q10" s="81"/>
+      <c r="Q10" s="81" t="s">
+        <v>262</v>
+      </c>
       <c r="R10" s="44"/>
       <c r="S10" s="44"/>
-      <c r="T10" s="45"/>
-      <c r="U10" s="81"/>
+      <c r="T10" s="45">
+        <v>3.5</v>
+      </c>
+      <c r="U10" s="81" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="11" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="35" t="s">
@@ -3144,7 +3191,9 @@
       <c r="P11" s="43">
         <v>43984</v>
       </c>
-      <c r="Q11" s="82"/>
+      <c r="Q11" s="82" t="s">
+        <v>250</v>
+      </c>
       <c r="R11" s="46"/>
       <c r="S11" s="46"/>
       <c r="T11" s="46"/>
@@ -3405,10 +3454,22 @@
         <v>55</v>
       </c>
       <c r="Q17" s="38"/>
-      <c r="R17" s="5"/>
-      <c r="S17" s="5"/>
-      <c r="T17" s="5"/>
-      <c r="U17" s="38"/>
+      <c r="R17" s="5">
+        <f>SUM(R10:R16)</f>
+        <v>0</v>
+      </c>
+      <c r="S17" s="5">
+        <f>SUM(S10:S16)</f>
+        <v>0</v>
+      </c>
+      <c r="T17" s="5">
+        <f>SUM(T10:T16)</f>
+        <v>3.5</v>
+      </c>
+      <c r="U17" s="38">
+        <f>SUM(R17:T17)</f>
+        <v>3.5</v>
+      </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="35" t="s">
@@ -6362,24 +6423,24 @@
         <v>147</v>
       </c>
       <c r="D86" s="64">
-        <f>SUM(D81,D73,D65,D57,D49,D41,D33,D25,D17,D9,K9,K17,K25,K33,K41,K49,K57,K65,K73,K81,R9)</f>
+        <f>SUM(D81,D73,D65,D57,D49,D41,D33,D25,D17,D9,K9,K17,K25,K33,K41,K49,K57,K65,K73,K81,R9, R17)</f>
         <v>219.5</v>
       </c>
       <c r="E86" s="64">
-        <f>SUM(E81,E73,E65,E57,E49,E41,E33,E25,E17,E9,L9,L17,L25,L33,L41,L49,L57,L65,L73,L81,S9)</f>
+        <f>SUM(E81,E73,E65,E57,E49,E41,E33,E25,E17,E9,L9,L17,L25,L33,L41,L49,L57,L65,L73,L81,S9, S17)</f>
         <v>85</v>
       </c>
       <c r="F86" s="64">
-        <f>SUM(F81,F73,F65,F57,F49,F41,F33,F25,F17,F9,M9,M17,M25,M33,M41,M49,M57,M65,M73,M81,T9)</f>
-        <v>102.5</v>
+        <f>SUM(F81,F73,F65,F57,F49,F41,F33,F25,F17,F9,M9,M17,M25,M33,M41,M49,M57,M65,M73,M81,T9, T17)</f>
+        <v>113</v>
       </c>
       <c r="G86" s="25">
         <f>SUM(D86:F86) + 9</f>
-        <v>416</v>
+        <v>426.5</v>
       </c>
       <c r="H86" s="66">
         <f>G86/400</f>
-        <v>1.04</v>
+        <v>1.0662499999999999</v>
       </c>
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.25">
@@ -6398,7 +6459,7 @@
       <c r="F88" s="64"/>
       <c r="G88" s="22">
         <f>G86*50</f>
-        <v>20800</v>
+        <v>21325</v>
       </c>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.25">
@@ -6410,7 +6471,7 @@
       </c>
       <c r="E90" s="28">
         <f ca="1">G86/(DATEDIF("2020-01-06",TODAY(),"d")/7)</f>
-        <v>20.363636363636367</v>
+        <v>20.30952380952381</v>
       </c>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.25">
@@ -6630,16 +6691,52 @@
       </c>
       <c r="C115" s="7">
         <f>U9</f>
-        <v>22.5</v>
+        <v>29.5</v>
       </c>
     </row>
     <row r="116" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B116" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="C116" s="6">
+        <f>U17</f>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B117" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="C117" s="7">
+        <f>U25</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B118" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="C118" s="6">
+        <f>U33</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B119" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="C119" s="6">
+        <f>U41</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B120" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="C116" s="29">
+      <c r="C120" s="29">
         <f ca="1">E90</f>
-        <v>20.363636363636367</v>
+        <v>20.30952380952381</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Design Revision 90% Done
Only need to read over user interface
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Desktop\thesisWindows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF3E3081-9627-4D0C-B5F8-B99AC025FDC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD89CF5-BEA2-480B-9A79-ADC55D963907}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="266">
   <si>
     <t>Date</t>
   </si>
@@ -821,6 +821,15 @@
   </si>
   <si>
     <t>10:30 - 13:00 14:30 - 15:30</t>
+  </si>
+  <si>
+    <t>Meeting + Report</t>
+  </si>
+  <si>
+    <t>11:00 - 12:30 14:00 - 16:00 22:00 - 00:00</t>
+  </si>
+  <si>
+    <t>12:00 - 14:30 16:00 - 18:00</t>
   </si>
 </sst>
 </file>
@@ -1701,7 +1710,7 @@
                   <c:v>29.5</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="General">
-                  <c:v>3.5</c:v>
+                  <c:v>11.5</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>0</c:v>
@@ -1713,7 +1722,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0">
-                  <c:v>20.30952380952381</c:v>
+                  <c:v>20.412751677852349</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2589,9 +2598,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R14" sqref="R14"/>
+      <selection pane="bottomLeft" activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3152,7 +3161,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="35" t="s">
         <v>32</v>
       </c>
@@ -3192,12 +3201,18 @@
         <v>43984</v>
       </c>
       <c r="Q11" s="82" t="s">
-        <v>250</v>
-      </c>
-      <c r="R11" s="46"/>
+        <v>264</v>
+      </c>
+      <c r="R11" s="46">
+        <v>1.5</v>
+      </c>
       <c r="S11" s="46"/>
-      <c r="T11" s="46"/>
-      <c r="U11" s="82"/>
+      <c r="T11" s="46">
+        <v>4</v>
+      </c>
+      <c r="U11" s="82" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="12" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="35" t="s">
@@ -3238,11 +3253,17 @@
       <c r="P12" s="43">
         <v>43985</v>
       </c>
-      <c r="Q12" s="82"/>
+      <c r="Q12" s="82" t="s">
+        <v>265</v>
+      </c>
       <c r="R12" s="46"/>
       <c r="S12" s="46"/>
-      <c r="T12" s="46"/>
-      <c r="U12" s="82"/>
+      <c r="T12" s="46">
+        <v>2.5</v>
+      </c>
+      <c r="U12" s="82" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="35" t="s">
@@ -3456,7 +3477,7 @@
       <c r="Q17" s="38"/>
       <c r="R17" s="5">
         <f>SUM(R10:R16)</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="S17" s="5">
         <f>SUM(S10:S16)</f>
@@ -3464,11 +3485,11 @@
       </c>
       <c r="T17" s="5">
         <f>SUM(T10:T16)</f>
-        <v>3.5</v>
+        <v>10</v>
       </c>
       <c r="U17" s="38">
         <f>SUM(R17:T17)</f>
-        <v>3.5</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
@@ -6424,7 +6445,7 @@
       </c>
       <c r="D86" s="64">
         <f>SUM(D81,D73,D65,D57,D49,D41,D33,D25,D17,D9,K9,K17,K25,K33,K41,K49,K57,K65,K73,K81,R9, R17)</f>
-        <v>219.5</v>
+        <v>221</v>
       </c>
       <c r="E86" s="64">
         <f>SUM(E81,E73,E65,E57,E49,E41,E33,E25,E17,E9,L9,L17,L25,L33,L41,L49,L57,L65,L73,L81,S9, S17)</f>
@@ -6432,15 +6453,15 @@
       </c>
       <c r="F86" s="64">
         <f>SUM(F81,F73,F65,F57,F49,F41,F33,F25,F17,F9,M9,M17,M25,M33,M41,M49,M57,M65,M73,M81,T9, T17)</f>
-        <v>113</v>
+        <v>119.5</v>
       </c>
       <c r="G86" s="25">
         <f>SUM(D86:F86) + 9</f>
-        <v>426.5</v>
+        <v>434.5</v>
       </c>
       <c r="H86" s="66">
         <f>G86/400</f>
-        <v>1.0662499999999999</v>
+        <v>1.0862499999999999</v>
       </c>
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.25">
@@ -6459,7 +6480,7 @@
       <c r="F88" s="64"/>
       <c r="G88" s="22">
         <f>G86*50</f>
-        <v>21325</v>
+        <v>21725</v>
       </c>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.25">
@@ -6471,7 +6492,7 @@
       </c>
       <c r="E90" s="28">
         <f ca="1">G86/(DATEDIF("2020-01-06",TODAY(),"d")/7)</f>
-        <v>20.30952380952381</v>
+        <v>20.412751677852349</v>
       </c>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.25">
@@ -6700,7 +6721,7 @@
       </c>
       <c r="C116" s="6">
         <f>U17</f>
-        <v>3.5</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="117" spans="2:3" x14ac:dyDescent="0.25">
@@ -6736,7 +6757,7 @@
       </c>
       <c r="C120" s="29">
         <f ca="1">E90</f>
-        <v>20.30952380952381</v>
+        <v>20.412751677852349</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Design 100% looked over
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Desktop\thesisWindows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD89CF5-BEA2-480B-9A79-ADC55D963907}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C15084-1447-4AC8-90F7-ACADF79A4540}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="265">
   <si>
     <t>Date</t>
   </si>
@@ -827,9 +827,6 @@
   </si>
   <si>
     <t>11:00 - 12:30 14:00 - 16:00 22:00 - 00:00</t>
-  </si>
-  <si>
-    <t>12:00 - 14:30 16:00 - 18:00</t>
   </si>
 </sst>
 </file>
@@ -1710,7 +1707,7 @@
                   <c:v>29.5</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="General">
-                  <c:v>11.5</c:v>
+                  <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>0</c:v>
@@ -1722,7 +1719,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0">
-                  <c:v>20.412751677852349</c:v>
+                  <c:v>20.506711409395972</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2600,7 +2597,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q13" sqref="Q13"/>
+      <selection pane="bottomLeft" activeCell="O11" sqref="O11:P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3254,12 +3251,12 @@
         <v>43985</v>
       </c>
       <c r="Q12" s="82" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="R12" s="46"/>
       <c r="S12" s="46"/>
       <c r="T12" s="46">
-        <v>2.5</v>
+        <v>4.5</v>
       </c>
       <c r="U12" s="82" t="s">
         <v>26</v>
@@ -3485,11 +3482,11 @@
       </c>
       <c r="T17" s="5">
         <f>SUM(T10:T16)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="U17" s="38">
         <f>SUM(R17:T17)</f>
-        <v>11.5</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
@@ -6453,15 +6450,15 @@
       </c>
       <c r="F86" s="64">
         <f>SUM(F81,F73,F65,F57,F49,F41,F33,F25,F17,F9,M9,M17,M25,M33,M41,M49,M57,M65,M73,M81,T9, T17)</f>
-        <v>119.5</v>
+        <v>121.5</v>
       </c>
       <c r="G86" s="25">
         <f>SUM(D86:F86) + 9</f>
-        <v>434.5</v>
+        <v>436.5</v>
       </c>
       <c r="H86" s="66">
         <f>G86/400</f>
-        <v>1.0862499999999999</v>
+        <v>1.0912500000000001</v>
       </c>
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.25">
@@ -6480,7 +6477,7 @@
       <c r="F88" s="64"/>
       <c r="G88" s="22">
         <f>G86*50</f>
-        <v>21725</v>
+        <v>21825</v>
       </c>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.25">
@@ -6492,7 +6489,7 @@
       </c>
       <c r="E90" s="28">
         <f ca="1">G86/(DATEDIF("2020-01-06",TODAY(),"d")/7)</f>
-        <v>20.412751677852349</v>
+        <v>20.506711409395972</v>
       </c>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.25">
@@ -6721,7 +6718,7 @@
       </c>
       <c r="C116" s="6">
         <f>U17</f>
-        <v>11.5</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="117" spans="2:3" x14ac:dyDescent="0.25">
@@ -6757,7 +6754,7 @@
       </c>
       <c r="C120" s="29">
         <f ca="1">E90</f>
-        <v>20.412751677852349</v>
+        <v>20.506711409395972</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started to build config file parser.
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Desktop\thesisWindows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C15084-1447-4AC8-90F7-ACADF79A4540}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B76C5F-4573-4F6B-9C9C-87CC3ED82941}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="267">
   <si>
     <t>Date</t>
   </si>
@@ -823,10 +823,16 @@
     <t>10:30 - 13:00 14:30 - 15:30</t>
   </si>
   <si>
-    <t>Meeting + Report</t>
-  </si>
-  <si>
     <t>11:00 - 12:30 14:00 - 16:00 22:00 - 00:00</t>
+  </si>
+  <si>
+    <t>Meeting + Report + Setup File Calibration</t>
+  </si>
+  <si>
+    <t>Report + Config File</t>
+  </si>
+  <si>
+    <t>12:00 - 14:30 16:00 - 18:00 21:00 - 22:00</t>
   </si>
 </sst>
 </file>
@@ -1105,7 +1111,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1354,6 +1360,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="3" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1707,7 +1716,7 @@
                   <c:v>29.5</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="General">
-                  <c:v>13.5</c:v>
+                  <c:v>14.5</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>0</c:v>
@@ -1719,7 +1728,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0">
-                  <c:v>20.506711409395972</c:v>
+                  <c:v>20.553691275167786</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2597,7 +2606,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O11" sqref="O11:P11"/>
+      <selection pane="bottomLeft" activeCell="U14" sqref="U14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3198,7 +3207,7 @@
         <v>43984</v>
       </c>
       <c r="Q11" s="82" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="R11" s="46">
         <v>1.5</v>
@@ -3208,7 +3217,7 @@
         <v>4</v>
       </c>
       <c r="U11" s="82" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="45" x14ac:dyDescent="0.25">
@@ -3250,16 +3259,18 @@
       <c r="P12" s="43">
         <v>43985</v>
       </c>
-      <c r="Q12" s="82" t="s">
-        <v>250</v>
-      </c>
-      <c r="R12" s="46"/>
+      <c r="Q12" s="85" t="s">
+        <v>266</v>
+      </c>
+      <c r="R12" s="46">
+        <v>1</v>
+      </c>
       <c r="S12" s="46"/>
       <c r="T12" s="46">
         <v>4.5</v>
       </c>
       <c r="U12" s="82" t="s">
-        <v>26</v>
+        <v>265</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
@@ -3474,7 +3485,7 @@
       <c r="Q17" s="38"/>
       <c r="R17" s="5">
         <f>SUM(R10:R16)</f>
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="S17" s="5">
         <f>SUM(S10:S16)</f>
@@ -3486,7 +3497,7 @@
       </c>
       <c r="U17" s="38">
         <f>SUM(R17:T17)</f>
-        <v>13.5</v>
+        <v>14.5</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
@@ -6442,7 +6453,7 @@
       </c>
       <c r="D86" s="64">
         <f>SUM(D81,D73,D65,D57,D49,D41,D33,D25,D17,D9,K9,K17,K25,K33,K41,K49,K57,K65,K73,K81,R9, R17)</f>
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E86" s="64">
         <f>SUM(E81,E73,E65,E57,E49,E41,E33,E25,E17,E9,L9,L17,L25,L33,L41,L49,L57,L65,L73,L81,S9, S17)</f>
@@ -6454,11 +6465,11 @@
       </c>
       <c r="G86" s="25">
         <f>SUM(D86:F86) + 9</f>
-        <v>436.5</v>
+        <v>437.5</v>
       </c>
       <c r="H86" s="66">
         <f>G86/400</f>
-        <v>1.0912500000000001</v>
+        <v>1.09375</v>
       </c>
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.25">
@@ -6477,7 +6488,7 @@
       <c r="F88" s="64"/>
       <c r="G88" s="22">
         <f>G86*50</f>
-        <v>21825</v>
+        <v>21875</v>
       </c>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.25">
@@ -6489,7 +6500,7 @@
       </c>
       <c r="E90" s="28">
         <f ca="1">G86/(DATEDIF("2020-01-06",TODAY(),"d")/7)</f>
-        <v>20.506711409395972</v>
+        <v>20.553691275167786</v>
       </c>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.25">
@@ -6718,7 +6729,7 @@
       </c>
       <c r="C116" s="6">
         <f>U17</f>
-        <v>13.5</v>
+        <v>14.5</v>
       </c>
     </row>
     <row r="117" spans="2:3" x14ac:dyDescent="0.25">
@@ -6754,7 +6765,7 @@
       </c>
       <c r="C120" s="29">
         <f ca="1">E90</f>
-        <v>20.506711409395972</v>
+        <v>20.553691275167786</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Parsing calibrations from file into parse object.
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Desktop\thesisWindows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B76C5F-4573-4F6B-9C9C-87CC3ED82941}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24AF60B0-2D54-4ABF-8B7D-A9A11011C4DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="269">
   <si>
     <t>Date</t>
   </si>
@@ -833,6 +833,12 @@
   </si>
   <si>
     <t>12:00 - 14:30 16:00 - 18:00 21:00 - 22:00</t>
+  </si>
+  <si>
+    <t>12:00 - 14:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Config File </t>
   </si>
 </sst>
 </file>
@@ -1716,7 +1722,7 @@
                   <c:v>29.5</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="General">
-                  <c:v>14.5</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>0</c:v>
@@ -1728,7 +1734,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0">
-                  <c:v>20.553691275167786</c:v>
+                  <c:v>20.533333333333335</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2606,7 +2612,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U14" sqref="U14"/>
+      <selection pane="bottomLeft" activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3306,11 +3312,17 @@
       <c r="P13" s="43">
         <v>43986</v>
       </c>
-      <c r="Q13" s="82"/>
-      <c r="R13" s="46"/>
+      <c r="Q13" s="82" t="s">
+        <v>267</v>
+      </c>
+      <c r="R13" s="46">
+        <v>2.5</v>
+      </c>
       <c r="S13" s="46"/>
       <c r="T13" s="46"/>
-      <c r="U13" s="82"/>
+      <c r="U13" s="82" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="35" t="s">
@@ -3485,7 +3497,7 @@
       <c r="Q17" s="38"/>
       <c r="R17" s="5">
         <f>SUM(R10:R16)</f>
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="S17" s="5">
         <f>SUM(S10:S16)</f>
@@ -3497,7 +3509,7 @@
       </c>
       <c r="U17" s="38">
         <f>SUM(R17:T17)</f>
-        <v>14.5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
@@ -6453,7 +6465,7 @@
       </c>
       <c r="D86" s="64">
         <f>SUM(D81,D73,D65,D57,D49,D41,D33,D25,D17,D9,K9,K17,K25,K33,K41,K49,K57,K65,K73,K81,R9, R17)</f>
-        <v>222</v>
+        <v>224.5</v>
       </c>
       <c r="E86" s="64">
         <f>SUM(E81,E73,E65,E57,E49,E41,E33,E25,E17,E9,L9,L17,L25,L33,L41,L49,L57,L65,L73,L81,S9, S17)</f>
@@ -6465,11 +6477,11 @@
       </c>
       <c r="G86" s="25">
         <f>SUM(D86:F86) + 9</f>
-        <v>437.5</v>
+        <v>440</v>
       </c>
       <c r="H86" s="66">
         <f>G86/400</f>
-        <v>1.09375</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.25">
@@ -6488,7 +6500,7 @@
       <c r="F88" s="64"/>
       <c r="G88" s="22">
         <f>G86*50</f>
-        <v>21875</v>
+        <v>22000</v>
       </c>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.25">
@@ -6500,7 +6512,7 @@
       </c>
       <c r="E90" s="28">
         <f ca="1">G86/(DATEDIF("2020-01-06",TODAY(),"d")/7)</f>
-        <v>20.553691275167786</v>
+        <v>20.533333333333335</v>
       </c>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.25">
@@ -6729,7 +6741,7 @@
       </c>
       <c r="C116" s="6">
         <f>U17</f>
-        <v>14.5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="117" spans="2:3" x14ac:dyDescent="0.25">
@@ -6765,7 +6777,7 @@
       </c>
       <c r="C120" s="29">
         <f ca="1">E90</f>
-        <v>20.553691275167786</v>
+        <v>20.533333333333335</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Configuration File Parser 90% Integrated
Just need to to add count and speed line integration.
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Desktop\thesisWindows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24AF60B0-2D54-4ABF-8B7D-A9A11011C4DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F67F284A-C2A2-48E0-8919-A7A5D65F626E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -835,10 +835,10 @@
     <t>12:00 - 14:30 16:00 - 18:00 21:00 - 22:00</t>
   </si>
   <si>
-    <t>12:00 - 14:00</t>
-  </si>
-  <si>
     <t xml:space="preserve">Config File </t>
+  </si>
+  <si>
+    <t>12:00 - 14:30 18:15 - 18:45 21:00 - 23:00 23:30 - 00:30</t>
   </si>
 </sst>
 </file>
@@ -1364,11 +1364,11 @@
     <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="20" fontId="3" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="3" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1722,7 +1722,7 @@
                   <c:v>29.5</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="General">
-                  <c:v>17</c:v>
+                  <c:v>19.5</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>0</c:v>
@@ -1734,7 +1734,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0">
-                  <c:v>20.533333333333335</c:v>
+                  <c:v>20.650000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2256,18 +2256,18 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="84" t="s">
+      <c r="G1" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84"/>
-      <c r="K1" s="84"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="84"/>
-      <c r="P1" s="84"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
+      <c r="L1" s="85"/>
+      <c r="M1" s="85"/>
+      <c r="N1" s="85"/>
+      <c r="O1" s="85"/>
+      <c r="P1" s="85"/>
       <c r="Q1" s="2"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -2610,9 +2610,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R14" sqref="R14"/>
+      <selection pane="bottomLeft" activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3265,7 +3265,7 @@
       <c r="P12" s="43">
         <v>43985</v>
       </c>
-      <c r="Q12" s="85" t="s">
+      <c r="Q12" s="84" t="s">
         <v>266</v>
       </c>
       <c r="R12" s="46">
@@ -3279,7 +3279,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="35" t="s">
         <v>40</v>
       </c>
@@ -3313,15 +3313,15 @@
         <v>43986</v>
       </c>
       <c r="Q13" s="82" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="R13" s="46">
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="S13" s="46"/>
       <c r="T13" s="46"/>
       <c r="U13" s="82" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
@@ -3497,7 +3497,7 @@
       <c r="Q17" s="38"/>
       <c r="R17" s="5">
         <f>SUM(R10:R16)</f>
-        <v>5</v>
+        <v>7.5</v>
       </c>
       <c r="S17" s="5">
         <f>SUM(S10:S16)</f>
@@ -3509,7 +3509,7 @@
       </c>
       <c r="U17" s="38">
         <f>SUM(R17:T17)</f>
-        <v>17</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
@@ -6465,7 +6465,7 @@
       </c>
       <c r="D86" s="64">
         <f>SUM(D81,D73,D65,D57,D49,D41,D33,D25,D17,D9,K9,K17,K25,K33,K41,K49,K57,K65,K73,K81,R9, R17)</f>
-        <v>224.5</v>
+        <v>227</v>
       </c>
       <c r="E86" s="64">
         <f>SUM(E81,E73,E65,E57,E49,E41,E33,E25,E17,E9,L9,L17,L25,L33,L41,L49,L57,L65,L73,L81,S9, S17)</f>
@@ -6477,11 +6477,11 @@
       </c>
       <c r="G86" s="25">
         <f>SUM(D86:F86) + 9</f>
-        <v>440</v>
+        <v>442.5</v>
       </c>
       <c r="H86" s="66">
         <f>G86/400</f>
-        <v>1.1000000000000001</v>
+        <v>1.10625</v>
       </c>
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.25">
@@ -6500,7 +6500,7 @@
       <c r="F88" s="64"/>
       <c r="G88" s="22">
         <f>G86*50</f>
-        <v>22000</v>
+        <v>22125</v>
       </c>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.25">
@@ -6512,7 +6512,7 @@
       </c>
       <c r="E90" s="28">
         <f ca="1">G86/(DATEDIF("2020-01-06",TODAY(),"d")/7)</f>
-        <v>20.533333333333335</v>
+        <v>20.650000000000002</v>
       </c>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.25">
@@ -6741,7 +6741,7 @@
       </c>
       <c r="C116" s="6">
         <f>U17</f>
-        <v>17</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="117" spans="2:3" x14ac:dyDescent="0.25">
@@ -6777,7 +6777,7 @@
       </c>
       <c r="C120" s="29">
         <f ca="1">E90</f>
-        <v>20.533333333333335</v>
+        <v>20.650000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete configuration file integration
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Desktop\thesisWindows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F67F284A-C2A2-48E0-8919-A7A5D65F626E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C559426-91E3-4685-937A-A371C389CAD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="271">
   <si>
     <t>Date</t>
   </si>
@@ -835,10 +835,16 @@
     <t>12:00 - 14:30 16:00 - 18:00 21:00 - 22:00</t>
   </si>
   <si>
-    <t xml:space="preserve">Config File </t>
-  </si>
-  <si>
     <t>12:00 - 14:30 18:15 - 18:45 21:00 - 23:00 23:30 - 00:30</t>
+  </si>
+  <si>
+    <t>Config File Integration</t>
+  </si>
+  <si>
+    <t>Config + Calibration</t>
+  </si>
+  <si>
+    <t>12:00 - 14:00 14:30</t>
   </si>
 </sst>
 </file>
@@ -1722,7 +1728,7 @@
                   <c:v>29.5</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="General">
-                  <c:v>19.5</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>0</c:v>
@@ -1734,7 +1740,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0">
-                  <c:v>20.650000000000002</c:v>
+                  <c:v>20.493421052631579</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2610,9 +2616,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK120"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q14" sqref="Q14"/>
+      <selection pane="bottomLeft" activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3313,15 +3319,15 @@
         <v>43986</v>
       </c>
       <c r="Q13" s="82" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="R13" s="46">
-        <v>5</v>
+        <v>5.5</v>
       </c>
       <c r="S13" s="46"/>
       <c r="T13" s="46"/>
       <c r="U13" s="82" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
@@ -3359,7 +3365,7 @@
       <c r="T14" s="46"/>
       <c r="U14" s="82"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="35" t="s">
         <v>48</v>
       </c>
@@ -3394,11 +3400,17 @@
       <c r="P15" s="43">
         <v>43988</v>
       </c>
-      <c r="Q15" s="82"/>
-      <c r="R15" s="46"/>
+      <c r="Q15" s="82" t="s">
+        <v>270</v>
+      </c>
+      <c r="R15" s="46">
+        <v>2</v>
+      </c>
       <c r="S15" s="46"/>
       <c r="T15" s="46"/>
-      <c r="U15" s="82"/>
+      <c r="U15" s="82" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="35" t="s">
@@ -3497,7 +3509,7 @@
       <c r="Q17" s="38"/>
       <c r="R17" s="5">
         <f>SUM(R10:R16)</f>
-        <v>7.5</v>
+        <v>10</v>
       </c>
       <c r="S17" s="5">
         <f>SUM(S10:S16)</f>
@@ -3509,7 +3521,7 @@
       </c>
       <c r="U17" s="38">
         <f>SUM(R17:T17)</f>
-        <v>19.5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
@@ -6465,7 +6477,7 @@
       </c>
       <c r="D86" s="64">
         <f>SUM(D81,D73,D65,D57,D49,D41,D33,D25,D17,D9,K9,K17,K25,K33,K41,K49,K57,K65,K73,K81,R9, R17)</f>
-        <v>227</v>
+        <v>229.5</v>
       </c>
       <c r="E86" s="64">
         <f>SUM(E81,E73,E65,E57,E49,E41,E33,E25,E17,E9,L9,L17,L25,L33,L41,L49,L57,L65,L73,L81,S9, S17)</f>
@@ -6477,11 +6489,11 @@
       </c>
       <c r="G86" s="25">
         <f>SUM(D86:F86) + 9</f>
-        <v>442.5</v>
+        <v>445</v>
       </c>
       <c r="H86" s="66">
         <f>G86/400</f>
-        <v>1.10625</v>
+        <v>1.1125</v>
       </c>
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.25">
@@ -6500,7 +6512,7 @@
       <c r="F88" s="64"/>
       <c r="G88" s="22">
         <f>G86*50</f>
-        <v>22125</v>
+        <v>22250</v>
       </c>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.25">
@@ -6512,7 +6524,7 @@
       </c>
       <c r="E90" s="28">
         <f ca="1">G86/(DATEDIF("2020-01-06",TODAY(),"d")/7)</f>
-        <v>20.650000000000002</v>
+        <v>20.493421052631579</v>
       </c>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.25">
@@ -6741,7 +6753,7 @@
       </c>
       <c r="C116" s="6">
         <f>U17</f>
-        <v>19.5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="117" spans="2:3" x14ac:dyDescent="0.25">
@@ -6777,7 +6789,7 @@
       </c>
       <c r="C120" s="29">
         <f ca="1">E90</f>
-        <v>20.650000000000002</v>
+        <v>20.493421052631579</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented more config setting and (w,h) graphics for boxes.
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Desktop\thesisWindows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C559426-91E3-4685-937A-A371C389CAD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39FA9FBA-CEB6-4B91-B4B4-19C60FFE02FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="273">
   <si>
     <t>Date</t>
   </si>
@@ -845,6 +845,12 @@
   </si>
   <si>
     <t>12:00 - 14:00 14:30</t>
+  </si>
+  <si>
+    <t>Calibrating Specific scene</t>
+  </si>
+  <si>
+    <t>15:00 - 17:00</t>
   </si>
 </sst>
 </file>
@@ -1728,7 +1734,7 @@
                   <c:v>29.5</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="General">
-                  <c:v>22</c:v>
+                  <c:v>24.5</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>0</c:v>
@@ -1740,7 +1746,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0">
-                  <c:v>20.493421052631579</c:v>
+                  <c:v>20.473856209150327</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2616,9 +2622,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q16" sqref="Q16"/>
+      <selection pane="bottomLeft" activeCell="U16" sqref="U16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3404,7 +3410,7 @@
         <v>270</v>
       </c>
       <c r="R15" s="46">
-        <v>2</v>
+        <v>4.5</v>
       </c>
       <c r="S15" s="46"/>
       <c r="T15" s="46"/>
@@ -3447,11 +3453,15 @@
       <c r="P16" s="43">
         <v>43989</v>
       </c>
-      <c r="Q16" s="82"/>
+      <c r="Q16" s="82" t="s">
+        <v>272</v>
+      </c>
       <c r="R16" s="46"/>
       <c r="S16" s="46"/>
       <c r="T16" s="46"/>
-      <c r="U16" s="82"/>
+      <c r="U16" s="82" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="39" t="s">
@@ -3509,7 +3519,7 @@
       <c r="Q17" s="38"/>
       <c r="R17" s="5">
         <f>SUM(R10:R16)</f>
-        <v>10</v>
+        <v>12.5</v>
       </c>
       <c r="S17" s="5">
         <f>SUM(S10:S16)</f>
@@ -3521,7 +3531,7 @@
       </c>
       <c r="U17" s="38">
         <f>SUM(R17:T17)</f>
-        <v>22</v>
+        <v>24.5</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
@@ -6477,7 +6487,7 @@
       </c>
       <c r="D86" s="64">
         <f>SUM(D81,D73,D65,D57,D49,D41,D33,D25,D17,D9,K9,K17,K25,K33,K41,K49,K57,K65,K73,K81,R9, R17)</f>
-        <v>229.5</v>
+        <v>232</v>
       </c>
       <c r="E86" s="64">
         <f>SUM(E81,E73,E65,E57,E49,E41,E33,E25,E17,E9,L9,L17,L25,L33,L41,L49,L57,L65,L73,L81,S9, S17)</f>
@@ -6489,11 +6499,11 @@
       </c>
       <c r="G86" s="25">
         <f>SUM(D86:F86) + 9</f>
-        <v>445</v>
+        <v>447.5</v>
       </c>
       <c r="H86" s="66">
         <f>G86/400</f>
-        <v>1.1125</v>
+        <v>1.1187499999999999</v>
       </c>
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.25">
@@ -6512,7 +6522,7 @@
       <c r="F88" s="64"/>
       <c r="G88" s="22">
         <f>G86*50</f>
-        <v>22250</v>
+        <v>22375</v>
       </c>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.25">
@@ -6524,7 +6534,7 @@
       </c>
       <c r="E90" s="28">
         <f ca="1">G86/(DATEDIF("2020-01-06",TODAY(),"d")/7)</f>
-        <v>20.493421052631579</v>
+        <v>20.473856209150327</v>
       </c>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.25">
@@ -6753,7 +6763,7 @@
       </c>
       <c r="C116" s="6">
         <f>U17</f>
-        <v>22</v>
+        <v>24.5</v>
       </c>
     </row>
     <row r="117" spans="2:3" x14ac:dyDescent="0.25">
@@ -6789,7 +6799,7 @@
       </c>
       <c r="C120" s="29">
         <f ca="1">E90</f>
-        <v>20.493421052631579</v>
+        <v>20.473856209150327</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected Issues with vehicle counting system.
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Desktop\thesisWindows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39FA9FBA-CEB6-4B91-B4B4-19C60FFE02FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5453AC0A-161E-4F35-8A54-413DEFE47A38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -850,7 +850,7 @@
     <t>Calibrating Specific scene</t>
   </si>
   <si>
-    <t>15:00 - 17:00</t>
+    <t>15:00 - 18:30 20:30 - 20:00</t>
   </si>
 </sst>
 </file>
@@ -1507,7 +1507,14 @@
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
-  <c:style val="2"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1734,7 +1741,7 @@
                   <c:v>29.5</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="General">
-                  <c:v>24.5</c:v>
+                  <c:v>31.5</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>0</c:v>
@@ -1746,14 +1753,14 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0">
-                  <c:v>20.473856209150327</c:v>
+                  <c:v>20.794117647058822</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D9DD-450D-AC55-7D0387D3E7B6}"/>
+              <c16:uniqueId val="{00000000-8E41-4BB0-A2B7-E17F5F724986}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1910,27 +1917,29 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>658575</xdr:colOff>
-      <xdr:row>90</xdr:row>
-      <xdr:rowOff>56762</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>297957</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>110658</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>493058</xdr:colOff>
-      <xdr:row>127</xdr:row>
-      <xdr:rowOff>33618</xdr:rowOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>525876</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>66434</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE8AD8B8-3645-4531-A246-A1F358F41A64}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2622,7 +2631,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="U16" sqref="U16"/>
     </sheetView>
@@ -3418,7 +3427,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="35" t="s">
         <v>52</v>
       </c>
@@ -3456,7 +3465,9 @@
       <c r="Q16" s="82" t="s">
         <v>272</v>
       </c>
-      <c r="R16" s="46"/>
+      <c r="R16" s="46">
+        <v>7</v>
+      </c>
       <c r="S16" s="46"/>
       <c r="T16" s="46"/>
       <c r="U16" s="82" t="s">
@@ -3519,7 +3530,7 @@
       <c r="Q17" s="38"/>
       <c r="R17" s="5">
         <f>SUM(R10:R16)</f>
-        <v>12.5</v>
+        <v>19.5</v>
       </c>
       <c r="S17" s="5">
         <f>SUM(S10:S16)</f>
@@ -3531,7 +3542,7 @@
       </c>
       <c r="U17" s="38">
         <f>SUM(R17:T17)</f>
-        <v>24.5</v>
+        <v>31.5</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
@@ -6487,7 +6498,7 @@
       </c>
       <c r="D86" s="64">
         <f>SUM(D81,D73,D65,D57,D49,D41,D33,D25,D17,D9,K9,K17,K25,K33,K41,K49,K57,K65,K73,K81,R9, R17)</f>
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="E86" s="64">
         <f>SUM(E81,E73,E65,E57,E49,E41,E33,E25,E17,E9,L9,L17,L25,L33,L41,L49,L57,L65,L73,L81,S9, S17)</f>
@@ -6499,11 +6510,11 @@
       </c>
       <c r="G86" s="25">
         <f>SUM(D86:F86) + 9</f>
-        <v>447.5</v>
+        <v>454.5</v>
       </c>
       <c r="H86" s="66">
         <f>G86/400</f>
-        <v>1.1187499999999999</v>
+        <v>1.13625</v>
       </c>
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.25">
@@ -6522,7 +6533,7 @@
       <c r="F88" s="64"/>
       <c r="G88" s="22">
         <f>G86*50</f>
-        <v>22375</v>
+        <v>22725</v>
       </c>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.25">
@@ -6534,7 +6545,7 @@
       </c>
       <c r="E90" s="28">
         <f ca="1">G86/(DATEDIF("2020-01-06",TODAY(),"d")/7)</f>
-        <v>20.473856209150327</v>
+        <v>20.794117647058822</v>
       </c>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.25">
@@ -6763,7 +6774,7 @@
       </c>
       <c r="C116" s="6">
         <f>U17</f>
-        <v>24.5</v>
+        <v>31.5</v>
       </c>
     </row>
     <row r="117" spans="2:3" x14ac:dyDescent="0.25">
@@ -6799,7 +6810,7 @@
       </c>
       <c r="C120" s="29">
         <f ca="1">E90</f>
-        <v>20.473856209150327</v>
+        <v>20.794117647058822</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Simplified line crossing logic
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Desktop\thesisWindows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5453AC0A-161E-4F35-8A54-413DEFE47A38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6177086E-E38A-4C3E-B984-F60799517463}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="275">
   <si>
     <t>Date</t>
   </si>
@@ -851,6 +851,12 @@
   </si>
   <si>
     <t>15:00 - 18:30 20:30 - 20:00</t>
+  </si>
+  <si>
+    <t>Generating Results</t>
+  </si>
+  <si>
+    <t>14:30 - 16:30</t>
   </si>
 </sst>
 </file>
@@ -1753,7 +1759,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0">
-                  <c:v>20.794117647058822</c:v>
+                  <c:v>20.65909090909091</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2633,7 +2639,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U16" sqref="U16"/>
+      <selection pane="bottomLeft" activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3578,11 +3584,15 @@
       <c r="P18" s="48">
         <v>43990</v>
       </c>
-      <c r="Q18" s="38"/>
+      <c r="Q18" s="38" t="s">
+        <v>274</v>
+      </c>
       <c r="R18" s="5"/>
       <c r="S18" s="5"/>
       <c r="T18" s="5"/>
-      <c r="U18" s="38"/>
+      <c r="U18" s="38" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="19" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="35" t="s">
@@ -6545,7 +6555,7 @@
       </c>
       <c r="E90" s="28">
         <f ca="1">G86/(DATEDIF("2020-01-06",TODAY(),"d")/7)</f>
-        <v>20.794117647058822</v>
+        <v>20.65909090909091</v>
       </c>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.25">
@@ -6810,7 +6820,7 @@
       </c>
       <c r="C120" s="29">
         <f ca="1">E90</f>
-        <v>20.794117647058822</v>
+        <v>20.65909090909091</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added two count_line functionality.
Doesn't look like it broke everything else because I tested it on previously tested samples and they behaved the same as before.
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Desktop\thesisWindows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6177086E-E38A-4C3E-B984-F60799517463}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31A9374-5FB2-44BC-BF66-D121889ACDBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -853,10 +853,10 @@
     <t>15:00 - 18:30 20:30 - 20:00</t>
   </si>
   <si>
-    <t>Generating Results</t>
-  </si>
-  <si>
-    <t>14:30 - 16:30</t>
+    <t>Generating Results + Improving Counting Logic</t>
+  </si>
+  <si>
+    <t>14:30 - 16:30 19:00 - 21:00 22:00 - 01:00</t>
   </si>
 </sst>
 </file>
@@ -1750,7 +1750,7 @@
                   <c:v>31.5</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="23" formatCode="General">
                   <c:v>0</c:v>
@@ -1759,7 +1759,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0">
-                  <c:v>20.65909090909091</c:v>
+                  <c:v>20.525806451612905</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2637,9 +2637,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q19" sqref="Q19"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U18" sqref="U18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3551,7 +3551,7 @@
         <v>31.5</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="35" t="s">
         <v>28</v>
       </c>
@@ -3587,7 +3587,9 @@
       <c r="Q18" s="38" t="s">
         <v>274</v>
       </c>
-      <c r="R18" s="5"/>
+      <c r="R18" s="5">
+        <v>7</v>
+      </c>
       <c r="S18" s="5"/>
       <c r="T18" s="5"/>
       <c r="U18" s="38" t="s">
@@ -3903,10 +3905,22 @@
       </c>
       <c r="P25" s="48"/>
       <c r="Q25" s="38"/>
-      <c r="R25" s="5"/>
-      <c r="S25" s="5"/>
-      <c r="T25" s="5"/>
-      <c r="U25" s="38"/>
+      <c r="R25" s="5">
+        <f>SUM(R18:R24)</f>
+        <v>7</v>
+      </c>
+      <c r="S25" s="5">
+        <f>SUM(S18:S24)</f>
+        <v>0</v>
+      </c>
+      <c r="T25" s="5">
+        <f>SUM(T18:T24)</f>
+        <v>0</v>
+      </c>
+      <c r="U25" s="38">
+        <f>SUM(R25:T25)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="26" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="35" t="s">
@@ -6555,7 +6569,7 @@
       </c>
       <c r="E90" s="28">
         <f ca="1">G86/(DATEDIF("2020-01-06",TODAY(),"d")/7)</f>
-        <v>20.65909090909091</v>
+        <v>20.525806451612905</v>
       </c>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.25">
@@ -6793,7 +6807,7 @@
       </c>
       <c r="C117" s="7">
         <f>U25</f>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="118" spans="2:3" x14ac:dyDescent="0.25">
@@ -6820,7 +6834,7 @@
       </c>
       <c r="C120" s="29">
         <f ca="1">E90</f>
-        <v>20.65909090909091</v>
+        <v>20.525806451612905</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added rotation functionality in case video is from mobile.
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Desktop\thesisWindows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A7D4313-062F-4282-9D7A-D30D289448F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADBEFBFD-244E-4340-9A93-50AC1CE00265}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -859,10 +859,10 @@
     <t>14:30 - 16:30 19:00 - 21:00 22:00 - 01:00</t>
   </si>
   <si>
-    <t>12:00 - 14:30</t>
-  </si>
-  <si>
-    <t>Calibration for scene 3</t>
+    <t>Calibration for scene 3 Collecting more samples</t>
+  </si>
+  <si>
+    <t>12:00 - 14:30 15:30 - 16:30 20:00 - 20:30</t>
   </si>
 </sst>
 </file>
@@ -1756,7 +1756,7 @@
                   <c:v>31.5</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>9.5</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="23" formatCode="General">
                   <c:v>0</c:v>
@@ -2644,8 +2644,8 @@
   <dimension ref="A1:AMK120"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L21" sqref="L21"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3602,7 +3602,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="35" t="s">
         <v>32</v>
       </c>
@@ -3644,15 +3644,15 @@
         <v>43991</v>
       </c>
       <c r="Q19" s="38" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="R19" s="5">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="S19" s="5"/>
       <c r="T19" s="5"/>
       <c r="U19" s="38" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="45" x14ac:dyDescent="0.25">
@@ -3919,7 +3919,7 @@
       <c r="Q25" s="38"/>
       <c r="R25" s="5">
         <f>SUM(R18:R24)</f>
-        <v>9.5</v>
+        <v>10.5</v>
       </c>
       <c r="S25" s="5">
         <f>SUM(S18:S24)</f>
@@ -3931,7 +3931,7 @@
       </c>
       <c r="U25" s="38">
         <f>SUM(R25:T25)</f>
-        <v>9.5</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="45" x14ac:dyDescent="0.25">
@@ -6819,7 +6819,7 @@
       </c>
       <c r="C117" s="7">
         <f>U25</f>
-        <v>9.5</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="118" spans="2:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Set up for android video as well with rotation function
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Desktop\thesisWindows\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\c3175\Desktop\thesisWindows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADBEFBFD-244E-4340-9A93-50AC1CE00265}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7C4FF24-FCB6-4165-8B36-2DD74419FC40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="278">
   <si>
     <t>Date</t>
   </si>
@@ -859,21 +859,22 @@
     <t>14:30 - 16:30 19:00 - 21:00 22:00 - 01:00</t>
   </si>
   <si>
-    <t>Calibration for scene 3 Collecting more samples</t>
-  </si>
-  <si>
-    <t>12:00 - 14:30 15:30 - 16:30 20:00 - 20:30</t>
+    <t>12:00 - 14:30 15:30 - 16:30 20:00 - 20:30 22:30 - 23:00</t>
+  </si>
+  <si>
+    <t>Calibration for scene 3 + Collecting more samples + Setting up laptop for demo</t>
+  </si>
+  <si>
+    <t>12:30 - 14:30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="d\-mmm"/>
-    <numFmt numFmtId="165" formatCode="d/mm/yyyy"/>
-    <numFmt numFmtId="166" formatCode="[$-409]d/mmm;@"/>
-    <numFmt numFmtId="167" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="[$-409]d/mmm;@"/>
+    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -1147,7 +1148,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1169,120 +1170,120 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="16" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="6" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1292,7 +1293,7 @@
     <xf numFmtId="20" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1301,7 +1302,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="3" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1325,7 +1326,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1340,22 +1341,22 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="7" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1370,13 +1371,13 @@
     <xf numFmtId="2" fontId="3" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="7" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1756,7 +1757,7 @@
                   <c:v>31.5</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>10.5</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="23" formatCode="General">
                   <c:v>0</c:v>
@@ -1765,7 +1766,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0">
-                  <c:v>20.525806451612905</c:v>
+                  <c:v>20.39423076923077</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2269,17 +2270,17 @@
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" customWidth="1"/>
-    <col min="4" max="16" width="10.7109375" customWidth="1"/>
-    <col min="17" max="17" width="37.28515625" customWidth="1"/>
-    <col min="18" max="1025" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" customWidth="1"/>
+    <col min="3" max="3" width="21.44140625" customWidth="1"/>
+    <col min="4" max="16" width="10.6640625" customWidth="1"/>
+    <col min="17" max="17" width="37.33203125" customWidth="1"/>
+    <col min="18" max="1025" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2303,7 +2304,7 @@
       <c r="P1" s="85"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2347,7 +2348,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -2369,7 +2370,7 @@
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -2391,7 +2392,7 @@
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -2407,7 +2408,7 @@
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -2429,7 +2430,7 @@
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -2451,7 +2452,7 @@
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -2473,7 +2474,7 @@
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -2489,7 +2490,7 @@
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -2511,7 +2512,7 @@
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -2533,7 +2534,7 @@
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -2546,7 +2547,7 @@
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -2559,7 +2560,7 @@
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -2572,7 +2573,7 @@
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -2585,7 +2586,7 @@
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -2598,7 +2599,7 @@
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.3">
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -2611,7 +2612,7 @@
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
@@ -2624,7 +2625,7 @@
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B22">
         <f>SUM(B2:B21)</f>
         <v>9.5</v>
@@ -2643,36 +2644,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T19" sqref="T19"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AC20" sqref="AC20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" style="67"/>
-    <col min="2" max="2" width="11.5703125" style="5"/>
-    <col min="3" max="3" width="19.28515625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="7"/>
-    <col min="5" max="5" width="21.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="7" customWidth="1"/>
-    <col min="7" max="7" width="57.28515625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" style="67"/>
+    <col min="2" max="2" width="11.5546875" style="5"/>
+    <col min="3" max="3" width="19.33203125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="7"/>
+    <col min="5" max="5" width="21.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="7" customWidth="1"/>
+    <col min="7" max="7" width="57.33203125" style="6" customWidth="1"/>
     <col min="8" max="8" width="29" style="61" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" style="62"/>
-    <col min="10" max="10" width="14.42578125" style="6" customWidth="1"/>
-    <col min="11" max="13" width="11.5703125" style="61"/>
-    <col min="14" max="14" width="39.42578125" style="61" customWidth="1"/>
-    <col min="15" max="15" width="6.7109375" style="61" customWidth="1"/>
-    <col min="16" max="16" width="11.5703125" style="63"/>
-    <col min="17" max="17" width="16.28515625" style="6" customWidth="1"/>
-    <col min="18" max="20" width="11.5703125" style="61"/>
-    <col min="21" max="21" width="24.85546875" style="6" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="33"/>
-    <col min="23" max="1025" width="11.5703125" style="34"/>
-    <col min="1026" max="16384" width="9.140625" style="2"/>
+    <col min="9" max="9" width="11.5546875" style="62"/>
+    <col min="10" max="10" width="14.44140625" style="6" customWidth="1"/>
+    <col min="11" max="13" width="11.5546875" style="61"/>
+    <col min="14" max="14" width="39.44140625" style="61" customWidth="1"/>
+    <col min="15" max="15" width="6.6640625" style="61" customWidth="1"/>
+    <col min="16" max="16" width="11.5546875" style="63"/>
+    <col min="17" max="17" width="16.33203125" style="6" customWidth="1"/>
+    <col min="18" max="20" width="11.5546875" style="61"/>
+    <col min="21" max="21" width="24.88671875" style="6" customWidth="1"/>
+    <col min="22" max="22" width="11.5546875" style="33"/>
+    <col min="23" max="1025" width="11.5546875" style="34"/>
+    <col min="1026" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
         <v>23</v>
       </c>
@@ -2737,7 +2738,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="35" t="s">
         <v>28</v>
       </c>
@@ -2790,7 +2791,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="35" t="s">
         <v>32</v>
       </c>
@@ -2843,7 +2844,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="35" t="s">
         <v>36</v>
       </c>
@@ -2900,7 +2901,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="35" t="s">
         <v>40</v>
       </c>
@@ -2953,7 +2954,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="35" t="s">
         <v>44</v>
       </c>
@@ -3004,7 +3005,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="35" t="s">
         <v>48</v>
       </c>
@@ -3051,7 +3052,7 @@
       </c>
       <c r="U7" s="79"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="35" t="s">
         <v>52</v>
       </c>
@@ -3090,7 +3091,7 @@
       <c r="T8" s="69"/>
       <c r="U8" s="79"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="39" t="s">
         <v>54</v>
       </c>
@@ -3161,7 +3162,7 @@
         <v>29.5</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="35" t="s">
         <v>28</v>
       </c>
@@ -3206,7 +3207,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="35" t="s">
         <v>32</v>
       </c>
@@ -3259,7 +3260,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="35" t="s">
         <v>36</v>
       </c>
@@ -3312,7 +3313,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="35" t="s">
         <v>40</v>
       </c>
@@ -3357,7 +3358,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" s="35" t="s">
         <v>44</v>
       </c>
@@ -3392,7 +3393,7 @@
       <c r="T14" s="46"/>
       <c r="U14" s="82"/>
     </row>
-    <row r="15" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="35" t="s">
         <v>48</v>
       </c>
@@ -3439,7 +3440,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="35" t="s">
         <v>52</v>
       </c>
@@ -3486,7 +3487,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" s="39" t="s">
         <v>68</v>
       </c>
@@ -3557,7 +3558,7 @@
         <v>31.5</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="35" t="s">
         <v>28</v>
       </c>
@@ -3602,7 +3603,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="35" t="s">
         <v>32</v>
       </c>
@@ -3644,18 +3645,18 @@
         <v>43991</v>
       </c>
       <c r="Q19" s="38" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="R19" s="5">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="S19" s="5"/>
       <c r="T19" s="5"/>
       <c r="U19" s="38" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="35" t="s">
         <v>36</v>
       </c>
@@ -3696,13 +3697,17 @@
       <c r="P20" s="48">
         <v>43992</v>
       </c>
-      <c r="Q20" s="38"/>
-      <c r="R20" s="5"/>
+      <c r="Q20" s="38" t="s">
+        <v>277</v>
+      </c>
+      <c r="R20" s="5">
+        <v>2</v>
+      </c>
       <c r="S20" s="5"/>
       <c r="T20" s="5"/>
       <c r="U20" s="38"/>
     </row>
-    <row r="21" spans="1:21" ht="75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" ht="72" x14ac:dyDescent="0.3">
       <c r="A21" s="35" t="s">
         <v>40</v>
       </c>
@@ -3749,7 +3754,7 @@
       <c r="T21" s="5"/>
       <c r="U21" s="38"/>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22" s="35" t="s">
         <v>44</v>
       </c>
@@ -3786,7 +3791,7 @@
       <c r="T22" s="5"/>
       <c r="U22" s="38"/>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A23" s="35" t="s">
         <v>48</v>
       </c>
@@ -3827,7 +3832,7 @@
       <c r="T23" s="5"/>
       <c r="U23" s="38"/>
     </row>
-    <row r="24" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="35" t="s">
         <v>52</v>
       </c>
@@ -3868,7 +3873,7 @@
       <c r="T24" s="5"/>
       <c r="U24" s="38"/>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A25" s="39" t="s">
         <v>78</v>
       </c>
@@ -3919,7 +3924,7 @@
       <c r="Q25" s="38"/>
       <c r="R25" s="5">
         <f>SUM(R18:R24)</f>
-        <v>10.5</v>
+        <v>13</v>
       </c>
       <c r="S25" s="5">
         <f>SUM(S18:S24)</f>
@@ -3931,10 +3936,10 @@
       </c>
       <c r="U25" s="38">
         <f>SUM(R25:T25)</f>
-        <v>10.5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="35" t="s">
         <v>28</v>
       </c>
@@ -3983,7 +3988,7 @@
       <c r="T26" s="46"/>
       <c r="U26" s="82"/>
     </row>
-    <row r="27" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="35" t="s">
         <v>32</v>
       </c>
@@ -4030,7 +4035,7 @@
       <c r="T27" s="46"/>
       <c r="U27" s="82"/>
     </row>
-    <row r="28" spans="1:21" ht="75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" ht="72" x14ac:dyDescent="0.3">
       <c r="A28" s="35" t="s">
         <v>36</v>
       </c>
@@ -4073,7 +4078,7 @@
       <c r="T28" s="46"/>
       <c r="U28" s="82"/>
     </row>
-    <row r="29" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A29" s="35" t="s">
         <v>40</v>
       </c>
@@ -4114,7 +4119,7 @@
       <c r="T29" s="46"/>
       <c r="U29" s="82"/>
     </row>
-    <row r="30" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" s="35" t="s">
         <v>44</v>
       </c>
@@ -4155,7 +4160,7 @@
       <c r="T30" s="46"/>
       <c r="U30" s="82"/>
     </row>
-    <row r="31" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="35" t="s">
         <v>48</v>
       </c>
@@ -4196,7 +4201,7 @@
       <c r="T31" s="46"/>
       <c r="U31" s="82"/>
     </row>
-    <row r="32" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="35" t="s">
         <v>52</v>
       </c>
@@ -4237,7 +4242,7 @@
       <c r="T32" s="46"/>
       <c r="U32" s="82"/>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A33" s="39" t="s">
         <v>83</v>
       </c>
@@ -4295,7 +4300,7 @@
       <c r="T33" s="5"/>
       <c r="U33" s="38"/>
     </row>
-    <row r="34" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34" s="35" t="s">
         <v>28</v>
       </c>
@@ -4342,7 +4347,7 @@
       <c r="T34" s="5"/>
       <c r="U34" s="38"/>
     </row>
-    <row r="35" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35" s="35" t="s">
         <v>32</v>
       </c>
@@ -4391,7 +4396,7 @@
       <c r="T35" s="5"/>
       <c r="U35" s="38"/>
     </row>
-    <row r="36" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="35" t="s">
         <v>36</v>
       </c>
@@ -4438,7 +4443,7 @@
       <c r="T36" s="5"/>
       <c r="U36" s="38"/>
     </row>
-    <row r="37" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A37" s="35" t="s">
         <v>40</v>
       </c>
@@ -4485,7 +4490,7 @@
       <c r="T37" s="5"/>
       <c r="U37" s="38"/>
     </row>
-    <row r="38" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A38" s="35" t="s">
         <v>44</v>
       </c>
@@ -4532,7 +4537,7 @@
       <c r="T38" s="5"/>
       <c r="U38" s="38"/>
     </row>
-    <row r="39" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="35" t="s">
         <v>48</v>
       </c>
@@ -4579,7 +4584,7 @@
       <c r="T39" s="5"/>
       <c r="U39" s="38"/>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A40" s="35" t="s">
         <v>52</v>
       </c>
@@ -4626,7 +4631,7 @@
       <c r="T40" s="5"/>
       <c r="U40" s="38"/>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A41" s="39" t="s">
         <v>92</v>
       </c>
@@ -4682,7 +4687,7 @@
       <c r="T41" s="5"/>
       <c r="U41" s="38"/>
     </row>
-    <row r="42" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="35" t="s">
         <v>28</v>
       </c>
@@ -4727,7 +4732,7 @@
       <c r="T42" s="46"/>
       <c r="U42" s="82"/>
     </row>
-    <row r="43" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="35" t="s">
         <v>32</v>
       </c>
@@ -4768,7 +4773,7 @@
       <c r="T43" s="46"/>
       <c r="U43" s="82"/>
     </row>
-    <row r="44" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="35" t="s">
         <v>36</v>
       </c>
@@ -4815,7 +4820,7 @@
       <c r="T44" s="46"/>
       <c r="U44" s="82"/>
     </row>
-    <row r="45" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" s="35" t="s">
         <v>40</v>
       </c>
@@ -4862,7 +4867,7 @@
       <c r="T45" s="46"/>
       <c r="U45" s="82"/>
     </row>
-    <row r="46" spans="1:21" ht="75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" ht="72" x14ac:dyDescent="0.3">
       <c r="A46" s="35" t="s">
         <v>44</v>
       </c>
@@ -4903,7 +4908,7 @@
       <c r="T46" s="46"/>
       <c r="U46" s="82"/>
     </row>
-    <row r="47" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="35" t="s">
         <v>48</v>
       </c>
@@ -4944,7 +4949,7 @@
       <c r="T47" s="46"/>
       <c r="U47" s="82"/>
     </row>
-    <row r="48" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="35" t="s">
         <v>52</v>
       </c>
@@ -4991,7 +4996,7 @@
       <c r="T48" s="46"/>
       <c r="U48" s="82"/>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49" s="39" t="s">
         <v>97</v>
       </c>
@@ -5044,7 +5049,7 @@
       <c r="T49" s="46"/>
       <c r="U49" s="82"/>
     </row>
-    <row r="50" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A50" s="35" t="s">
         <v>28</v>
       </c>
@@ -5091,7 +5096,7 @@
       <c r="T50" s="5"/>
       <c r="U50" s="38"/>
     </row>
-    <row r="51" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A51" s="35" t="s">
         <v>32</v>
       </c>
@@ -5138,7 +5143,7 @@
       <c r="T51" s="5"/>
       <c r="U51" s="38"/>
     </row>
-    <row r="52" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A52" s="35" t="s">
         <v>36</v>
       </c>
@@ -5185,7 +5190,7 @@
       <c r="T52" s="5"/>
       <c r="U52" s="38"/>
     </row>
-    <row r="53" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A53" s="35" t="s">
         <v>40</v>
       </c>
@@ -5232,7 +5237,7 @@
       <c r="T53" s="5"/>
       <c r="U53" s="38"/>
     </row>
-    <row r="54" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" s="35" t="s">
         <v>44</v>
       </c>
@@ -5279,7 +5284,7 @@
       <c r="T54" s="5"/>
       <c r="U54" s="38"/>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A55" s="35" t="s">
         <v>48</v>
       </c>
@@ -5320,7 +5325,7 @@
       <c r="T55" s="5"/>
       <c r="U55" s="38"/>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A56" s="35" t="s">
         <v>52</v>
       </c>
@@ -5361,7 +5366,7 @@
       <c r="T56" s="5"/>
       <c r="U56" s="38"/>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A57" s="39" t="s">
         <v>110</v>
       </c>
@@ -5417,7 +5422,7 @@
       <c r="T57" s="5"/>
       <c r="U57" s="38"/>
     </row>
-    <row r="58" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A58" s="35" t="s">
         <v>28</v>
       </c>
@@ -5466,7 +5471,7 @@
       <c r="T58" s="46"/>
       <c r="U58" s="82"/>
     </row>
-    <row r="59" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A59" s="35" t="s">
         <v>32</v>
       </c>
@@ -5509,7 +5514,7 @@
       <c r="T59" s="46"/>
       <c r="U59" s="82"/>
     </row>
-    <row r="60" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A60" s="35" t="s">
         <v>36</v>
       </c>
@@ -5556,7 +5561,7 @@
       <c r="T60" s="46"/>
       <c r="U60" s="82"/>
     </row>
-    <row r="61" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A61" s="35" t="s">
         <v>40</v>
       </c>
@@ -5605,7 +5610,7 @@
       <c r="T61" s="46"/>
       <c r="U61" s="82"/>
     </row>
-    <row r="62" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A62" s="35" t="s">
         <v>44</v>
       </c>
@@ -5646,7 +5651,7 @@
       <c r="T62" s="46"/>
       <c r="U62" s="82"/>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A63" s="35" t="s">
         <v>48</v>
       </c>
@@ -5687,7 +5692,7 @@
       <c r="T63" s="46"/>
       <c r="U63" s="82"/>
     </row>
-    <row r="64" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A64" s="35" t="s">
         <v>52</v>
       </c>
@@ -5734,7 +5739,7 @@
       <c r="T64" s="46"/>
       <c r="U64" s="82"/>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A65" s="39" t="s">
         <v>118</v>
       </c>
@@ -5789,7 +5794,7 @@
       <c r="T65" s="46"/>
       <c r="U65" s="82"/>
     </row>
-    <row r="66" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A66" s="35" t="s">
         <v>28</v>
       </c>
@@ -5832,7 +5837,7 @@
       <c r="T66" s="74"/>
       <c r="U66" s="83"/>
     </row>
-    <row r="67" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A67" s="35" t="s">
         <v>32</v>
       </c>
@@ -5875,7 +5880,7 @@
       <c r="T67" s="74"/>
       <c r="U67" s="83"/>
     </row>
-    <row r="68" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A68" s="35" t="s">
         <v>36</v>
       </c>
@@ -5918,7 +5923,7 @@
       <c r="T68" s="74"/>
       <c r="U68" s="83"/>
     </row>
-    <row r="69" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A69" s="35" t="s">
         <v>40</v>
       </c>
@@ -5961,7 +5966,7 @@
       <c r="T69" s="74"/>
       <c r="U69" s="83"/>
     </row>
-    <row r="70" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A70" s="35" t="s">
         <v>44</v>
       </c>
@@ -6004,7 +6009,7 @@
       <c r="T70" s="74"/>
       <c r="U70" s="83"/>
     </row>
-    <row r="71" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A71" s="35" t="s">
         <v>48</v>
       </c>
@@ -6047,7 +6052,7 @@
       <c r="T71" s="74"/>
       <c r="U71" s="83"/>
     </row>
-    <row r="72" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A72" s="35" t="s">
         <v>52</v>
       </c>
@@ -6084,7 +6089,7 @@
       <c r="T72" s="74"/>
       <c r="U72" s="83"/>
     </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A73" s="39" t="s">
         <v>133</v>
       </c>
@@ -6139,7 +6144,7 @@
       <c r="T73" s="74"/>
       <c r="U73" s="83"/>
     </row>
-    <row r="74" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A74" s="35" t="s">
         <v>28</v>
       </c>
@@ -6182,7 +6187,7 @@
       <c r="T74" s="74"/>
       <c r="U74" s="83"/>
     </row>
-    <row r="75" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A75" s="35" t="s">
         <v>32</v>
       </c>
@@ -6225,7 +6230,7 @@
       <c r="T75" s="74"/>
       <c r="U75" s="83"/>
     </row>
-    <row r="76" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A76" s="35" t="s">
         <v>36</v>
       </c>
@@ -6268,7 +6273,7 @@
       <c r="T76" s="74"/>
       <c r="U76" s="83"/>
     </row>
-    <row r="77" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A77" s="35" t="s">
         <v>40</v>
       </c>
@@ -6311,7 +6316,7 @@
       <c r="T77" s="74"/>
       <c r="U77" s="83"/>
     </row>
-    <row r="78" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A78" s="35" t="s">
         <v>44</v>
       </c>
@@ -6354,7 +6359,7 @@
       <c r="T78" s="74"/>
       <c r="U78" s="83"/>
     </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A79" s="35" t="s">
         <v>48</v>
       </c>
@@ -6391,7 +6396,7 @@
       <c r="T79" s="74"/>
       <c r="U79" s="83"/>
     </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A80" s="35" t="s">
         <v>52</v>
       </c>
@@ -6428,7 +6433,7 @@
       <c r="T80" s="74"/>
       <c r="U80" s="83"/>
     </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A81" s="58"/>
       <c r="B81" s="14" t="s">
         <v>55</v>
@@ -6479,7 +6484,7 @@
       <c r="T81" s="74"/>
       <c r="U81" s="83"/>
     </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A82" s="59"/>
       <c r="B82" s="60"/>
       <c r="C82" s="21"/>
@@ -6488,7 +6493,7 @@
       <c r="F82" s="24"/>
       <c r="G82" s="21"/>
     </row>
-    <row r="83" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A83" s="59"/>
       <c r="B83" s="13"/>
       <c r="C83" s="22"/>
@@ -6497,7 +6502,7 @@
       <c r="F83" s="24"/>
       <c r="G83" s="21"/>
     </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A84" s="59"/>
       <c r="B84" s="60"/>
       <c r="C84" s="21"/>
@@ -6506,7 +6511,7 @@
       <c r="F84" s="24"/>
       <c r="G84" s="21"/>
     </row>
-    <row r="85" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A85" s="59"/>
       <c r="B85" s="60"/>
       <c r="C85" s="21"/>
@@ -6526,7 +6531,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A86" s="59"/>
       <c r="B86" s="13"/>
       <c r="C86" s="22" t="s">
@@ -6553,7 +6558,7 @@
         <v>1.13625</v>
       </c>
     </row>
-    <row r="87" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B87" s="60"/>
       <c r="C87" s="21"/>
       <c r="D87" s="23"/>
@@ -6561,7 +6566,7 @@
       <c r="F87" s="24"/>
       <c r="G87" s="21"/>
     </row>
-    <row r="88" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B88" s="60"/>
       <c r="C88" s="26"/>
       <c r="D88" s="23"/>
@@ -6572,19 +6577,19 @@
         <v>22725</v>
       </c>
     </row>
-    <row r="89" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B89" s="27"/>
     </row>
-    <row r="90" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:21" x14ac:dyDescent="0.3">
       <c r="D90" s="7" t="s">
         <v>148</v>
       </c>
       <c r="E90" s="28">
         <f ca="1">G86/(DATEDIF("2020-01-06",TODAY(),"d")/7)</f>
-        <v>20.525806451612905</v>
-      </c>
-    </row>
-    <row r="93" spans="1:21" x14ac:dyDescent="0.25">
+        <v>20.39423076923077</v>
+      </c>
+    </row>
+    <row r="93" spans="1:21" x14ac:dyDescent="0.3">
       <c r="D93" s="76" t="s">
         <v>234</v>
       </c>
@@ -6592,7 +6597,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="94" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B94" s="7" t="s">
         <v>149</v>
       </c>
@@ -6606,7 +6611,7 @@
         <v>44008</v>
       </c>
     </row>
-    <row r="95" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B95" s="7" t="s">
         <v>23</v>
       </c>
@@ -6621,7 +6626,7 @@
         <v>44014</v>
       </c>
     </row>
-    <row r="96" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B96" s="7" t="s">
         <v>54</v>
       </c>
@@ -6630,7 +6635,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B97" s="7" t="s">
         <v>68</v>
       </c>
@@ -6639,7 +6644,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B98" s="7" t="s">
         <v>78</v>
       </c>
@@ -6648,7 +6653,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="99" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B99" s="7" t="s">
         <v>83</v>
       </c>
@@ -6657,7 +6662,7 @@
         <v>22.5</v>
       </c>
     </row>
-    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B100" s="7" t="s">
         <v>92</v>
       </c>
@@ -6666,7 +6671,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B101" s="7" t="s">
         <v>97</v>
       </c>
@@ -6675,7 +6680,7 @@
         <v>20.5</v>
       </c>
     </row>
-    <row r="102" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B102" s="7" t="s">
         <v>110</v>
       </c>
@@ -6684,7 +6689,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B103" s="7" t="s">
         <v>118</v>
       </c>
@@ -6693,7 +6698,7 @@
         <v>24.5</v>
       </c>
     </row>
-    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B104" s="7" t="s">
         <v>133</v>
       </c>
@@ -6702,7 +6707,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B105" s="7" t="s">
         <v>27</v>
       </c>
@@ -6711,7 +6716,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="106" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B106" s="7" t="s">
         <v>56</v>
       </c>
@@ -6720,7 +6725,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="107" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B107" s="7" t="s">
         <v>69</v>
       </c>
@@ -6729,7 +6734,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="108" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B108" s="7" t="s">
         <v>150</v>
       </c>
@@ -6738,7 +6743,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="109" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B109" s="7" t="s">
         <v>151</v>
       </c>
@@ -6750,7 +6755,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="110" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B110" s="7" t="s">
         <v>152</v>
       </c>
@@ -6759,7 +6764,7 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="111" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B111" s="7" t="s">
         <v>153</v>
       </c>
@@ -6768,7 +6773,7 @@
         <v>24.5</v>
       </c>
     </row>
-    <row r="112" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B112" s="7" t="s">
         <v>154</v>
       </c>
@@ -6777,7 +6782,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B113" s="7" t="s">
         <v>155</v>
       </c>
@@ -6786,7 +6791,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B114" s="7" t="s">
         <v>156</v>
       </c>
@@ -6795,7 +6800,7 @@
         <v>27.5</v>
       </c>
     </row>
-    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B115" s="7" t="s">
         <v>157</v>
       </c>
@@ -6804,7 +6809,7 @@
         <v>29.5</v>
       </c>
     </row>
-    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B116" s="5" t="s">
         <v>213</v>
       </c>
@@ -6813,16 +6818,16 @@
         <v>31.5</v>
       </c>
     </row>
-    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B117" s="5" t="s">
         <v>214</v>
       </c>
       <c r="C117" s="7">
         <f>U25</f>
-        <v>10.5</v>
-      </c>
-    </row>
-    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="118" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B118" s="5" t="s">
         <v>215</v>
       </c>
@@ -6831,7 +6836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B119" s="5" t="s">
         <v>216</v>
       </c>
@@ -6840,13 +6845,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B120" s="5" t="s">
         <v>158</v>
       </c>
       <c r="C120" s="29">
         <f ca="1">E90</f>
-        <v>20.525806451612905</v>
+        <v>20.39423076923077</v>
       </c>
     </row>
   </sheetData>
@@ -6877,9 +6882,9 @@
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1025" width="11.5703125" style="8"/>
+    <col min="1" max="1025" width="11.5546875" style="8"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>